<commit_message>
Beginning to add endothermic plotting in Excel
</commit_message>
<xml_diff>
--- a/sources_list_.xlsx
+++ b/sources_list_.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/peterbaz_stanford_edu/Documents/DiazMarin2026/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/peterbaz_stanford_edu/Documents/DiazMarin2026/hygroscopic-salts-main/hygroscopic-salts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="579" documentId="8_{0B5C881D-AA95-4664-BDBF-B508CE6D9B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAEB4034-69BB-4DA5-A685-C9B98E10E52B}"/>
+  <xr:revisionPtr revIDLastSave="674" documentId="8_{0B5C881D-AA95-4664-BDBF-B508CE6D9B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33F31F6C-D5D7-4A43-BC6D-9CE0491DCC27}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="3" xr2:uid="{A5D934FD-846B-4DBC-ADED-26484461699C}"/>
+    <workbookView xWindow="13092" yWindow="210" windowWidth="9906" windowHeight="12558" activeTab="3" xr2:uid="{A5D934FD-846B-4DBC-ADED-26484461699C}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sources" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="163">
   <si>
     <t xml:space="preserve">Data Source </t>
   </si>
@@ -473,9 +473,6 @@
     <t>Makes a ML model and cites these as reference experiemntal values</t>
   </si>
   <si>
-    <t>Havent checked source</t>
-  </si>
-  <si>
     <t>MODELING CHEMICAL EQUILIBRIUM OF ELECTROLYTE SOLUTIONS</t>
   </si>
   <si>
@@ -495,6 +492,42 @@
   </si>
   <si>
     <t>10ish</t>
+  </si>
+  <si>
+    <t>The Vapor Pressures and Activity Coefficients of Aqueous Solutions of Ammonium Chloride at 25°1</t>
+  </si>
+  <si>
+    <t>NH4Cl, (NaCl, KCl)</t>
+  </si>
+  <si>
+    <t>List of endothermic salts, NaCl, KCl, NH4OH, NH4Cl, KBr</t>
+  </si>
+  <si>
+    <t>O-P</t>
+  </si>
+  <si>
+    <t>Havent checked source. Also seems to plot 10 experimetnal points when table showed 6</t>
+  </si>
+  <si>
+    <t>NaCl molality</t>
+  </si>
+  <si>
+    <t>NaCl γ</t>
+  </si>
+  <si>
+    <t>Paper 1 (NaCl)</t>
+  </si>
+  <si>
+    <t>25C</t>
+  </si>
+  <si>
+    <t>110C</t>
+  </si>
+  <si>
+    <t>NaCl mass fraction</t>
+  </si>
+  <si>
+    <t>Water mole fraction (for RH)</t>
   </si>
 </sst>
 </file>
@@ -526,12 +559,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -547,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -559,6 +598,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -583,16 +628,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>104228</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>529814</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>167981</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>468630</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>807720</xdr:rowOff>
+      <xdr:colOff>179630</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>532053</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -622,8 +667,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6926580" y="104228"/>
-          <a:ext cx="2907030" cy="1069252"/>
+          <a:off x="6865620" y="167981"/>
+          <a:ext cx="2684033" cy="987121"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -645,15 +690,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>895350</xdr:rowOff>
+      <xdr:colOff>48810</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>895606</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:colOff>248835</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>215073</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -683,8 +728,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6903720" y="1261110"/>
-          <a:ext cx="1440180" cy="838200"/>
+          <a:off x="6927266" y="1256789"/>
+          <a:ext cx="1440193" cy="836474"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -706,15 +751,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>229364</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>179967</xdr:rowOff>
+      <xdr:colOff>27659</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>145385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>432464</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>92476</xdr:rowOff>
+      <xdr:colOff>173243</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57963</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -737,8 +782,96 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7109558" y="2192239"/>
-          <a:ext cx="1445974" cy="1192373"/>
+          <a:off x="6907430" y="2156521"/>
+          <a:ext cx="1390366" cy="1148617"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>97816</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>37190</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>17417</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>591348</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABDF06B9-BD6F-53D1-4772-D15539F53582}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6977587" y="3327397"/>
+          <a:ext cx="1156763" cy="1178454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>240972</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>52750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>161109</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>513346</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F52A7BD7-547B-F647-EF3F-094161B7C7BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8361715" y="3342957"/>
+          <a:ext cx="1161108" cy="1077272"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1073,7 +1206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D422A4-CFD7-4638-AF22-DADFBBEF90F0}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="78" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -1752,7 +1885,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="94" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.62890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1819,111 +1952,238 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADEB32D0-53C4-465C-8106-B93762800774}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="215" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.578125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="20.578125" defaultRowHeight="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="20.578125" style="2"/>
     <col min="2" max="3" width="7.578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.578125" style="2" customWidth="1"/>
     <col min="5" max="6" width="20.578125" style="2"/>
     <col min="7" max="7" width="7.578125" style="2" customWidth="1"/>
-    <col min="8" max="35" width="8.578125" style="2" customWidth="1"/>
+    <col min="8" max="13" width="8.578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.578125" style="6" customWidth="1"/>
+    <col min="15" max="35" width="8.578125" style="2" customWidth="1"/>
     <col min="36" max="16384" width="20.578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N1" s="5"/>
+    </row>
+    <row r="2" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2024</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I2"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="O2" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C3" s="2">
+        <v>2024</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="R3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="2">
         <v>2007</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G4"/>
+      <c r="O4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="O5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.82850000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G3"/>
-    </row>
-    <row r="5" spans="1:11" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="4" t="s">
+      <c r="C6" s="2">
+        <v>2002</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2002</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0.65810000000000002</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.71199999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>150</v>
+      <c r="B7" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1937</v>
+      </c>
+      <c r="O7" s="2">
+        <v>2</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0.66839999999999999</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.72199999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="O8" s="2">
+        <v>3</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0.7147</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.75900000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="O9" s="2">
+        <v>4</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0.78320000000000001</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="O10" s="2">
+        <v>5</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0.87470000000000003</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="O11" s="2">
+        <v>6</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0.98529999999999995</v>
+      </c>
+      <c r="S11" s="2">
+        <v>1.04</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{9D68AF26-BC88-48F3-AD15-D7063E47E647}"/>
-    <hyperlink ref="A3" r:id="rId2" location="abstract" xr:uid="{8642617F-EDF7-4B17-AEF5-18DF92DCFE33}"/>
-    <hyperlink ref="A5" r:id="rId3" xr:uid="{67E4DD68-33A8-493F-B9CE-7F0B03DD45AB}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{9D68AF26-BC88-48F3-AD15-D7063E47E647}"/>
+    <hyperlink ref="A4" r:id="rId2" location="abstract" xr:uid="{8642617F-EDF7-4B17-AEF5-18DF92DCFE33}"/>
+    <hyperlink ref="A6" r:id="rId3" xr:uid="{67E4DD68-33A8-493F-B9CE-7F0B03DD45AB}"/>
+    <hyperlink ref="A7" r:id="rId4" xr:uid="{B172C2B9-22E2-400D-9AE6-B101DAE0D864}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added several endothermic datapoints to list
</commit_message>
<xml_diff>
--- a/sources_list_.xlsx
+++ b/sources_list_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/peterbaz_stanford_edu/Documents/DiazMarin2026/hygroscopic-salts-main/hygroscopic-salts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="674" documentId="8_{0B5C881D-AA95-4664-BDBF-B508CE6D9B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33F31F6C-D5D7-4A43-BC6D-9CE0491DCC27}"/>
+  <xr:revisionPtr revIDLastSave="1035" documentId="8_{0B5C881D-AA95-4664-BDBF-B508CE6D9B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AC49C39-A121-4ED9-A25F-66E13D083BF3}"/>
   <bookViews>
-    <workbookView xWindow="13092" yWindow="210" windowWidth="9906" windowHeight="12558" activeTab="3" xr2:uid="{A5D934FD-846B-4DBC-ADED-26484461699C}"/>
+    <workbookView xWindow="11565" yWindow="0" windowWidth="19530" windowHeight="20850" activeTab="3" xr2:uid="{A5D934FD-846B-4DBC-ADED-26484461699C}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sources" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="264">
   <si>
     <t xml:space="preserve">Data Source </t>
   </si>
@@ -500,15 +500,6 @@
     <t>NH4Cl, (NaCl, KCl)</t>
   </si>
   <si>
-    <t>List of endothermic salts, NaCl, KCl, NH4OH, NH4Cl, KBr</t>
-  </si>
-  <si>
-    <t>O-P</t>
-  </si>
-  <si>
-    <t>Havent checked source. Also seems to plot 10 experimetnal points when table showed 6</t>
-  </si>
-  <si>
     <t>NaCl molality</t>
   </si>
   <si>
@@ -528,13 +519,325 @@
   </si>
   <si>
     <t>Water mole fraction (for RH)</t>
+  </si>
+  <si>
+    <t>NaCl mole fraction</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Molar Masses (g, kg)</t>
+  </si>
+  <si>
+    <t>KCl</t>
+  </si>
+  <si>
+    <t>NH4Cl</t>
+  </si>
+  <si>
+    <t>Annoying cuz only has salt activity coeffiicents. Havent checked source. Also seems to plot 10 experimetnal points when table showed 6</t>
+  </si>
+  <si>
+    <t>Water activities, osmotic and activity coefficients in aqueous chloride solutions atT =  298.15 K by the hygrometric method</t>
+  </si>
+  <si>
+    <t>NaCl, many more</t>
+  </si>
+  <si>
+    <t>10ish each</t>
+  </si>
+  <si>
+    <t>Seems experimentally regisered</t>
+  </si>
+  <si>
+    <t>Paper 3 (NaCl)</t>
+  </si>
+  <si>
+    <t>a_w</t>
+  </si>
+  <si>
+    <t>Column O</t>
+  </si>
+  <si>
+    <t>Col V</t>
+  </si>
+  <si>
+    <t>CsCl</t>
+  </si>
+  <si>
+    <t>Paper 3 (CsCl)</t>
+  </si>
+  <si>
+    <t>CsCl molality</t>
+  </si>
+  <si>
+    <t>CsCl mole fraction</t>
+  </si>
+  <si>
+    <t>CsCl mass fraction</t>
+  </si>
+  <si>
+    <t>Paper 3 (NH4Cl)</t>
+  </si>
+  <si>
+    <t>NH4Cl molality</t>
+  </si>
+  <si>
+    <t>NH4Cl mole fraction</t>
+  </si>
+  <si>
+    <t>NH4Cl mass fraction</t>
+  </si>
+  <si>
+    <t>Paper 3 (KCl)</t>
+  </si>
+  <si>
+    <t>KCl molality</t>
+  </si>
+  <si>
+    <t>KCl mole fraction</t>
+  </si>
+  <si>
+    <t>KCl mass fraction</t>
+  </si>
+  <si>
+    <t>LiCl</t>
+  </si>
+  <si>
+    <t>Paper 3 (Others, pasted in a row)</t>
+  </si>
+  <si>
+    <t>MgCl2</t>
+  </si>
+  <si>
+    <t>0.9906</t>
+  </si>
+  <si>
+    <t>0.9856</t>
+  </si>
+  <si>
+    <t>0.9750</t>
+  </si>
+  <si>
+    <t>0.942</t>
+  </si>
+  <si>
+    <t>0.902</t>
+  </si>
+  <si>
+    <t>0.849</t>
+  </si>
+  <si>
+    <t>0.789</t>
+  </si>
+  <si>
+    <t>0.723</t>
+  </si>
+  <si>
+    <t>0.653</t>
+  </si>
+  <si>
+    <t>0.582</t>
+  </si>
+  <si>
+    <t>0.512</t>
+  </si>
+  <si>
+    <t>0.443</t>
+  </si>
+  <si>
+    <t>0.9907</t>
+  </si>
+  <si>
+    <t>0.9860</t>
+  </si>
+  <si>
+    <t>0.9756</t>
+  </si>
+  <si>
+    <t>0.945</t>
+  </si>
+  <si>
+    <t>0.908</t>
+  </si>
+  <si>
+    <t>0.862</t>
+  </si>
+  <si>
+    <t>0.810</t>
+  </si>
+  <si>
+    <t>0.750</t>
+  </si>
+  <si>
+    <t>0.688</t>
+  </si>
+  <si>
+    <t>0.625</t>
+  </si>
+  <si>
+    <t>0.561</t>
+  </si>
+  <si>
+    <t>0.500</t>
+  </si>
+  <si>
+    <t>0.444</t>
+  </si>
+  <si>
+    <t>0.394</t>
+  </si>
+  <si>
+    <t>CaCl2</t>
+  </si>
+  <si>
+    <t>THE ACTIVITY COEFFICIENTS OF AMMONIUM PERCHLORATE IN WATER AT 25°</t>
+  </si>
+  <si>
+    <t>NH4ClO3</t>
+  </si>
+  <si>
+    <t>Only mean activtiy coefficient</t>
+  </si>
+  <si>
+    <t>Note about 0.98 relative humidty but most data seem not to use that so should be ok…</t>
+  </si>
+  <si>
+    <t>CHEMEO</t>
+  </si>
+  <si>
+    <t>KCl (+other but eh)</t>
+  </si>
+  <si>
+    <t>Solid sagreement with KCl from 3</t>
+  </si>
+  <si>
+    <t>Database of properties published.</t>
+  </si>
+  <si>
+    <t>The Solubility, Activity Coefficients and Solubility Product of Manganese(II) Iodatela</t>
+  </si>
+  <si>
+    <t>Activity Coefficients, Phase Diagrams of the NaNO3-Pb(NO3)2-H2O System at 298.2 K, and Its Applications</t>
+  </si>
+  <si>
+    <t>List of endothermic salts, NaCl, KCl, NH4OH, NH4Cl, KBr, NH4ClO3, KNO3, NaNO3</t>
+  </si>
+  <si>
+    <t>NaNO3</t>
+  </si>
+  <si>
+    <t>10ish (for no Pb)</t>
+  </si>
+  <si>
+    <t>–0.0036</t>
+  </si>
+  <si>
+    <t>–0.0368</t>
+  </si>
+  <si>
+    <t>–0.0989</t>
+  </si>
+  <si>
+    <t>–0.2604</t>
+  </si>
+  <si>
+    <t>–0.4556</t>
+  </si>
+  <si>
+    <t>–0.6770</t>
+  </si>
+  <si>
+    <t>–0.9175</t>
+  </si>
+  <si>
+    <t>–1.1742</t>
+  </si>
+  <si>
+    <t>–1.4471</t>
+  </si>
+  <si>
+    <t>–1.7324</t>
+  </si>
+  <si>
+    <t>–2.0293</t>
+  </si>
+  <si>
+    <t>–2.3433</t>
+  </si>
+  <si>
+    <t>I (molality?)</t>
+  </si>
+  <si>
+    <t>Mean γ</t>
+  </si>
+  <si>
+    <t>G_xs</t>
+  </si>
+  <si>
+    <t>φ</t>
+  </si>
+  <si>
+    <t>25.05C</t>
+  </si>
+  <si>
+    <t>Osmotic and activity coefficient investigation on the CsNO3 + methanol + water and CsNO3 + ethanol + water ternary systems at 298.15 K</t>
+  </si>
+  <si>
+    <t>CsNO3</t>
+  </si>
+  <si>
+    <t>Mean Activity Coefficients of NaNO3 and the Mixing Ion-Interaction Parameters in the Ternary System (NaNO3 + CsNO3 + H2O) at 298.15 K by EMF Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (and CsNO3 mix)</t>
+  </si>
+  <si>
+    <t>Solid agreement with the paper two above</t>
+  </si>
+  <si>
+    <t>Thermodynamic description of aqueous solutions of silver nitrate: Experimental and modeling</t>
+  </si>
+  <si>
+    <t>AgNO3</t>
+  </si>
+  <si>
+    <t>Paper 12 (AgNO3)</t>
+  </si>
+  <si>
+    <t>Paper 9 (NaNO3)</t>
+  </si>
+  <si>
+    <t>40.05C</t>
+  </si>
+  <si>
+    <t>ϕ</t>
+  </si>
+  <si>
+    <t>m / mol.kg-1</t>
+  </si>
+  <si>
+    <t>aw</t>
+  </si>
+  <si>
+    <t>NaNO3 mole fraction</t>
+  </si>
+  <si>
+    <t>NaNO3 mass fraction</t>
+  </si>
+  <si>
+    <t>AgNO3 mole fraction</t>
+  </si>
+  <si>
+    <t>AgNO3 mass fraction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,6 +860,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE6E8F0"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -586,7 +895,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -604,6 +913,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -635,7 +948,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>179630</xdr:colOff>
+      <xdr:colOff>181535</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>532053</xdr:rowOff>
     </xdr:to>
@@ -698,7 +1011,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>248835</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>215073</xdr:rowOff>
+      <xdr:rowOff>211263</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -752,14 +1065,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>27659</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>145385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>173243</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>57963</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57962</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -796,13 +1109,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>97816</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>37190</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>17417</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>591348</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -840,13 +1153,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>240972</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>52750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>161109</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:colOff>163014</xdr:colOff>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>513346</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -872,6 +1185,94 @@
         <a:xfrm>
           <a:off x="8361715" y="3342957"/>
           <a:ext cx="1161108" cy="1077272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>265705</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>273021</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>103200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76535</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4174E5A-EAA8-F403-20B7-D416806ABC44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6611326" y="2769228"/>
+          <a:ext cx="1639296" cy="1047807"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>56084</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>486382</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>188584</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>374921</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B512555-5DBB-6398-2749-69893EE0A832}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5882547" y="9758058"/>
+          <a:ext cx="1774042" cy="1124762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1206,18 +1607,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D422A4-CFD7-4638-AF22-DADFBBEF90F0}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="78" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.5234375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="25.5234375" style="2"/>
-    <col min="5" max="8" width="13.1015625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="25.5234375" style="2"/>
+    <col min="1" max="4" width="25.5703125" style="2"/>
+    <col min="5" max="8" width="13.140625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="25.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1249,7 +1650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1281,7 +1682,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1310,7 +1711,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
@@ -1330,7 +1731,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
@@ -1353,7 +1754,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>37</v>
       </c>
@@ -1367,7 +1768,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
@@ -1378,7 +1779,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>44</v>
       </c>
@@ -1395,7 +1796,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>99</v>
       </c>
@@ -1421,7 +1822,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>48</v>
       </c>
@@ -1450,7 +1851,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>50</v>
       </c>
@@ -1473,10 +1874,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -1490,7 +1891,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1511,7 +1912,7 @@
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1520,7 +1921,7 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1528,12 +1929,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>5</v>
       </c>
@@ -1556,7 +1957,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>119</v>
       </c>
@@ -1585,10 +1986,10 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
     </row>
@@ -1622,17 +2023,17 @@
       <selection activeCell="D16" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.62890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="25.62890625" style="2"/>
-    <col min="4" max="4" width="10.62890625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.62890625" style="2"/>
-    <col min="6" max="6" width="10.62890625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="13.15625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="25.62890625" style="2"/>
+    <col min="1" max="3" width="25.5703125" style="2"/>
+    <col min="4" max="4" width="10.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="2"/>
+    <col min="6" max="6" width="10.5703125" style="2" customWidth="1"/>
+    <col min="7" max="9" width="13.140625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="25.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -1655,7 +2056,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>56</v>
       </c>
@@ -1672,7 +2073,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>58</v>
       </c>
@@ -1689,7 +2090,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>65</v>
       </c>
@@ -1709,7 +2110,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>66</v>
       </c>
@@ -1726,7 +2127,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" ht="360" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>83</v>
       </c>
@@ -1746,7 +2147,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>88</v>
       </c>
@@ -1763,10 +2164,10 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>73</v>
       </c>
@@ -1783,7 +2184,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>133</v>
       </c>
@@ -1806,7 +2207,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>61</v>
       </c>
@@ -1835,7 +2236,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>128</v>
       </c>
@@ -1888,15 +2289,15 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.62890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.62890625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.62890625" style="2"/>
-    <col min="3" max="3" width="13.15625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="25.62890625" style="2"/>
+    <col min="1" max="1" width="25.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="2"/>
+    <col min="3" max="3" width="13.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="25.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -1907,7 +2308,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
@@ -1918,7 +2319,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>79</v>
       </c>
@@ -1929,7 +2330,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>81</v>
       </c>
@@ -1952,32 +2353,58 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADEB32D0-53C4-465C-8106-B93762800774}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:BN32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="BQ10" sqref="BQ10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.578125" defaultRowHeight="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.578125" style="2"/>
-    <col min="2" max="3" width="7.578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.578125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="20.578125" style="2"/>
-    <col min="7" max="7" width="7.578125" style="2" customWidth="1"/>
-    <col min="8" max="13" width="8.578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.578125" style="6" customWidth="1"/>
-    <col min="15" max="35" width="8.578125" style="2" customWidth="1"/>
-    <col min="36" max="16384" width="20.578125" style="2"/>
+    <col min="1" max="1" width="20.5703125" style="2"/>
+    <col min="2" max="3" width="7.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="20.5703125" style="2"/>
+    <col min="7" max="7" width="7.5703125" style="2" customWidth="1"/>
+    <col min="8" max="13" width="8.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="6" customWidth="1"/>
+    <col min="15" max="77" width="8.5703125" style="2" customWidth="1"/>
+    <col min="78" max="16384" width="20.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:66" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>227</v>
       </c>
       <c r="N1" s="5"/>
-    </row>
-    <row r="2" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="O1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+    </row>
+    <row r="2" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -2005,11 +2432,29 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="O2" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="P2" s="2">
+        <v>18.015000000000001</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>58.442999999999998</v>
+      </c>
+      <c r="R2" s="2">
+        <v>74.551000000000002</v>
+      </c>
+      <c r="S2" s="2">
+        <v>53.491</v>
+      </c>
+      <c r="T2" s="2">
+        <v>168.363</v>
+      </c>
+      <c r="U2" s="2">
+        <v>84.994</v>
+      </c>
+      <c r="V2" s="2">
+        <v>169.87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>139</v>
       </c>
@@ -2026,22 +2471,44 @@
         <v>143</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="I3"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="R3" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="P3" s="2">
+        <f>P2/1000</f>
+        <v>1.8015E-2</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>Q2/1000</f>
+        <v>5.8442999999999995E-2</v>
+      </c>
+      <c r="R3" s="2">
+        <f>R2/1000</f>
+        <v>7.4551000000000006E-2</v>
+      </c>
+      <c r="S3" s="2">
+        <f>S2/1000</f>
+        <v>5.3490999999999997E-2</v>
+      </c>
+      <c r="T3" s="2">
+        <f>T2/1000</f>
+        <v>0.16836300000000001</v>
+      </c>
+      <c r="U3" s="2">
+        <f>U2/1000</f>
+        <v>8.4994E-2</v>
+      </c>
+      <c r="V3" s="2">
+        <f>V2/1000</f>
+        <v>0.16986999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>144</v>
       </c>
@@ -2057,133 +2524,2548 @@
       <c r="F4" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G4"/>
-      <c r="O4" s="2" t="s">
+      <c r="G4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="V4" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AX4" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="BD4"/>
+      <c r="BE4" s="7"/>
+      <c r="BF4" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S5" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="R4" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="S4" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="O5" s="2">
+      <c r="Z5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AR5" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2001</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AN6" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="AO6" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="AP6" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="AQ6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AR6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AT6" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="AU6" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AV6" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="BC6" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="BG6" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="BJ6" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="BK6" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="BL6" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="BM6" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="BN6" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="2">
         <v>0.1</v>
       </c>
-      <c r="R5" s="2">
+      <c r="P7" s="2">
+        <f>$P$3*O7/(1+$P$3*O7)</f>
+        <v>1.7982604338284581E-3</v>
+      </c>
+      <c r="Q7" s="2">
+        <f>P7*$Q$3/(P7*$Q$3+(1-P7)*$P$3)</f>
+        <v>5.810342614657159E-3</v>
+      </c>
+      <c r="R7" s="2">
+        <f>1-P7</f>
+        <v>0.99820173956617153</v>
+      </c>
+      <c r="S7" s="2">
         <v>0.77749999999999997</v>
       </c>
-      <c r="S5" s="2">
+      <c r="T7" s="2">
         <v>0.82850000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="4" t="s">
+      <c r="V7" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="W7" s="2">
+        <f>$P$3*V7/(1+$P$3*V7)</f>
+        <v>3.5900649958200605E-3</v>
+      </c>
+      <c r="X7" s="2">
+        <f>W7*$Q$3/(W7*$Q$3+(1-W7)*$P$3)</f>
+        <v>1.1553555115674923E-2</v>
+      </c>
+      <c r="Y7" s="2">
+        <f>1-W7</f>
+        <v>0.99640993500417996</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>0.99339999999999995</v>
+      </c>
+      <c r="AA7"/>
+      <c r="AB7" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AC7" s="2">
+        <f>$T$3*AB7/(1+$T$3*AB7)</f>
+        <v>3.2575691761588726E-2</v>
+      </c>
+      <c r="AD7" s="2">
+        <f>AC7*$T$3/(AC7*$T$3+(1-AC7)*$P$3)</f>
+        <v>0.23936696943613739</v>
+      </c>
+      <c r="AE7" s="2">
+        <f>1-AC7</f>
+        <v>0.9674243082384113</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AI7" s="2">
+        <f>$S$3*AH7/(1+$S$3*AH7)</f>
+        <v>1.0584959981129877E-2</v>
+      </c>
+      <c r="AJ7" s="2">
+        <f>AI7*$S$3/(AI7*$S$3+(1-AI7)*$P$3)</f>
+        <v>3.0787619893897878E-2</v>
+      </c>
+      <c r="AK7" s="2">
+        <f>1-AI7</f>
+        <v>0.98941504001887015</v>
+      </c>
+      <c r="AL7" s="2">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="AN7" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AO7" s="2">
+        <f>$R$3*AN7/(1+$R$3*AN7)</f>
+        <v>1.4691151985663363E-2</v>
+      </c>
+      <c r="AP7" s="2">
+        <f>AO7*$R$3/(AO7*$R$3+(1-AO7)*$P$3)</f>
+        <v>5.8116552083885414E-2</v>
+      </c>
+      <c r="AQ7" s="2">
+        <f>1-AO7</f>
+        <v>0.9853088480143366</v>
+      </c>
+      <c r="AR7" s="2">
+        <v>0.99350000000000005</v>
+      </c>
+      <c r="AT7" s="8">
+        <v>0.99329999999999996</v>
+      </c>
+      <c r="AU7" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AV7" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AX7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="AY7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="AZ7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BA7" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="BB7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="BC7" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BD7" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="BG7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="BH7" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="BI7" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="BJ7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="BK7" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="BL7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="BM7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="BN7" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C8" s="2">
         <v>2002</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O8" s="2">
         <v>1</v>
       </c>
-      <c r="R6" s="2">
+      <c r="P8" s="2">
+        <f t="shared" ref="P8:P13" si="0">$P$3*O8/(1+$P$3*O8)</f>
+        <v>1.7696202904672331E-2</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" ref="Q8:Q13" si="1">P8*$Q$3/(P8*$Q$3+(1-P8)*$P$3)</f>
+        <v>5.5216010687396497E-2</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" ref="R8:R13" si="2">1-P8</f>
+        <v>0.98230379709532767</v>
+      </c>
+      <c r="S8" s="2">
         <v>0.65810000000000002</v>
       </c>
-      <c r="S6" s="2">
+      <c r="T8" s="2">
         <v>0.71199999999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="4" t="s">
+      <c r="V8" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="W8" s="2">
+        <f t="shared" ref="W8:W20" si="3">$P$3*V8/(1+$P$3*V8)</f>
+        <v>5.3754483891806726E-3</v>
+      </c>
+      <c r="X8" s="2">
+        <f t="shared" ref="X8:X20" si="4">W8*$Q$3/(W8*$Q$3+(1-W8)*$P$3)</f>
+        <v>1.7230794208226582E-2</v>
+      </c>
+      <c r="Y8" s="2">
+        <f t="shared" ref="Y8:Y20" si="5">1-W8</f>
+        <v>0.99462455161081931</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="AC8" s="2">
+        <f t="shared" ref="AC8:AC20" si="6">$T$3*AB8/(1+$T$3*AB8)</f>
+        <v>4.8080411313031236E-2</v>
+      </c>
+      <c r="AD8" s="2">
+        <f t="shared" ref="AD8:AD20" si="7">AC8*$T$3/(AC8*$T$3+(1-AC8)*$P$3)</f>
+        <v>0.32067138531083489</v>
+      </c>
+      <c r="AE8" s="2">
+        <f t="shared" ref="AE8:AE20" si="8">1-AC8</f>
+        <v>0.9519195886869688</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="AH8" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="AI8" s="2">
+        <f t="shared" ref="AI8:AI20" si="9">$S$3*AH8/(1+$S$3*AH8)</f>
+        <v>1.5793851329559162E-2</v>
+      </c>
+      <c r="AJ8" s="2">
+        <f t="shared" ref="AJ8:AJ20" si="10">AI8*$S$3/(AI8*$S$3+(1-AI8)*$P$3)</f>
+        <v>4.5481299362322918E-2</v>
+      </c>
+      <c r="AK8" s="2">
+        <f t="shared" ref="AK8:AK20" si="11">1-AI8</f>
+        <v>0.98420614867044087</v>
+      </c>
+      <c r="AL8" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="AN8" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="AO8" s="2">
+        <f t="shared" ref="AO8:AO17" si="12">$R$3*AN8/(1+$R$3*AN8)</f>
+        <v>2.1876035894410738E-2</v>
+      </c>
+      <c r="AP8" s="2">
+        <f t="shared" ref="AP8:AP17" si="13">AO8*$R$3/(AO8*$R$3+(1-AO8)*$P$3)</f>
+        <v>8.4713208333669743E-2</v>
+      </c>
+      <c r="AQ8" s="2">
+        <f t="shared" ref="AQ8:AQ20" si="14">1-AO8</f>
+        <v>0.97812396410558922</v>
+      </c>
+      <c r="AR8" s="2">
+        <v>0.99029999999999996</v>
+      </c>
+      <c r="AT8" s="8">
+        <v>0.98980000000000001</v>
+      </c>
+      <c r="AU8" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="AV8" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AX8" s="2">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="AY8" s="2">
+        <f>$U$3*AX8/(1+$U$3*AX8)</f>
+        <v>8.6618786812902974E-4</v>
+      </c>
+      <c r="AZ8" s="2">
+        <f>AY8*$U$3/(AY8*$U$3+(1-AY8)*$P$3)</f>
+        <v>4.0735187777003025E-3</v>
+      </c>
+      <c r="BA8" s="2">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="BB8" s="2">
+        <v>0.96589999999999998</v>
+      </c>
+      <c r="BC8" s="2">
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="BD8" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="BG8" s="2">
+        <v>0.499</v>
+      </c>
+      <c r="BH8" s="2">
+        <f>$V$3*BG8/(1+$V$3*BG8)</f>
+        <v>7.8141459064046417E-2</v>
+      </c>
+      <c r="BI8" s="2">
+        <f>BH8*$V$3/(BH8*$V$3+(1-BH8)*$P$3)</f>
+        <v>0.44422253508640985</v>
+      </c>
+      <c r="BJ8" s="2">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="BK8" s="2">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="BL8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="BM8" s="2">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="BN8" s="2">
+        <v>0.95099999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C9" s="2">
         <v>1937</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O9" s="2">
         <v>2</v>
       </c>
-      <c r="R7" s="2">
+      <c r="P9" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4776985222435643E-2</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.10465347403405539</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.96522301477756434</v>
+      </c>
+      <c r="S9" s="2">
         <v>0.66839999999999999</v>
       </c>
-      <c r="S7" s="2">
+      <c r="T9" s="2">
         <v>0.72199999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="O8" s="2">
+      <c r="V9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="W9" s="2">
+        <f t="shared" si="3"/>
+        <v>8.9270892436379302E-3</v>
+      </c>
+      <c r="X9" s="2">
+        <f t="shared" si="4"/>
+        <v>2.839184762463667E-2</v>
+      </c>
+      <c r="Y9" s="2">
+        <f t="shared" si="5"/>
+        <v>0.99107291075636206</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>0.98350000000000004</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AC9" s="2">
+        <f t="shared" si="6"/>
+        <v>7.7645209773455834E-2</v>
+      </c>
+      <c r="AD9" s="2">
+        <f t="shared" si="7"/>
+        <v>0.44032024106328244</v>
+      </c>
+      <c r="AE9" s="2">
+        <f t="shared" si="8"/>
+        <v>0.92235479022654421</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="AH9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AI9" s="2">
+        <f t="shared" si="9"/>
+        <v>2.6048811511713465E-2</v>
+      </c>
+      <c r="AJ9" s="2">
+        <f t="shared" si="10"/>
+        <v>7.3571416524238833E-2</v>
+      </c>
+      <c r="AK9" s="2">
+        <f t="shared" si="11"/>
+        <v>0.97395118848828655</v>
+      </c>
+      <c r="AL9" s="2">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="AN9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AO9" s="2">
+        <f t="shared" si="12"/>
+        <v>3.5935968795175438E-2</v>
+      </c>
+      <c r="AP9" s="2">
+        <f t="shared" si="13"/>
+        <v>0.13364122903781739</v>
+      </c>
+      <c r="AQ9" s="2">
+        <f t="shared" si="14"/>
+        <v>0.96406403120482453</v>
+      </c>
+      <c r="AR9" s="2">
+        <v>0.9839</v>
+      </c>
+      <c r="AT9" s="8">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="AU9" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="AV9" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AX9" s="2">
+        <v>5.0099999999999999E-2</v>
+      </c>
+      <c r="AY9" s="2">
+        <f t="shared" ref="AY9:AY19" si="15">$U$3*AX9/(1+$U$3*AX9)</f>
+        <v>4.2401440212727036E-3</v>
+      </c>
+      <c r="AZ9" s="2">
+        <f t="shared" ref="AZ9:AZ19" si="16">AY9*$U$3/(AY9*$U$3+(1-AY9)*$P$3)</f>
+        <v>1.9694343352171489E-2</v>
+      </c>
+      <c r="BA9" s="2">
+        <v>0.62919999999999998</v>
+      </c>
+      <c r="BB9" s="2">
+        <v>0.9355</v>
+      </c>
+      <c r="BC9" s="2">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="BD9" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="BG9" s="2">
+        <v>0.999</v>
+      </c>
+      <c r="BH9" s="2">
+        <f t="shared" ref="BH9:BH32" si="17">$V$3*BG9/(1+$V$3*BG9)</f>
+        <v>0.14508003004154577</v>
+      </c>
+      <c r="BI9" s="2">
+        <f t="shared" ref="BI9:BI32" si="18">BH9*$V$3/(BH9*$V$3+(1-BH9)*$P$3)</f>
+        <v>0.61540892858775742</v>
+      </c>
+      <c r="BJ9" s="2">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="BK9" s="2">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="BL9" s="2">
+        <v>0.998</v>
+      </c>
+      <c r="BM9" s="2">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="BN9" s="2">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O10" s="2">
         <v>3</v>
       </c>
-      <c r="R8" s="2">
+      <c r="P10" s="2">
+        <f t="shared" si="0"/>
+        <v>5.1273901968132293E-2</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14917440138037943</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" si="2"/>
+        <v>0.94872609803186769</v>
+      </c>
+      <c r="S10" s="2">
         <v>0.7147</v>
       </c>
-      <c r="S8" s="2">
+      <c r="T10" s="2">
         <v>0.75900000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="O9" s="2">
+      <c r="V10" s="2">
+        <v>1</v>
+      </c>
+      <c r="W10" s="2">
+        <f t="shared" si="3"/>
+        <v>1.7696202904672331E-2</v>
+      </c>
+      <c r="X10" s="2">
+        <f t="shared" si="4"/>
+        <v>5.5216010687396497E-2</v>
+      </c>
+      <c r="Y10" s="2">
+        <f t="shared" si="5"/>
+        <v>0.98230379709532767</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="2">
+        <f t="shared" si="6"/>
+        <v>0.14410161910296715</v>
+      </c>
+      <c r="AD10" s="2">
+        <f t="shared" si="7"/>
+        <v>0.61141991691823538</v>
+      </c>
+      <c r="AE10" s="2">
+        <f t="shared" si="8"/>
+        <v>0.85589838089703285</v>
+      </c>
+      <c r="AF10" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="AH10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="2">
+        <f t="shared" si="9"/>
+        <v>5.0774994755531842E-2</v>
+      </c>
+      <c r="AJ10" s="2">
+        <f t="shared" si="10"/>
+        <v>0.13705919399834871</v>
+      </c>
+      <c r="AK10" s="2">
+        <f t="shared" si="11"/>
+        <v>0.94922500524446818</v>
+      </c>
+      <c r="AL10" s="2">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="AN10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="2">
+        <f t="shared" si="12"/>
+        <v>6.9378745168912417E-2</v>
+      </c>
+      <c r="AP10" s="2">
+        <f t="shared" si="13"/>
+        <v>0.23577340981369546</v>
+      </c>
+      <c r="AQ10" s="2">
+        <f t="shared" si="14"/>
+        <v>0.9306212548310876</v>
+      </c>
+      <c r="AR10" s="2">
+        <v>0.96819999999999995</v>
+      </c>
+      <c r="AT10" s="8">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="AU10" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AV10" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AX10" s="2">
+        <v>0.1003</v>
+      </c>
+      <c r="AY10" s="2">
+        <f t="shared" si="15"/>
+        <v>8.4528386113373218E-3</v>
+      </c>
+      <c r="AZ10" s="2">
+        <f t="shared" si="16"/>
+        <v>3.8664995157047646E-2</v>
+      </c>
+      <c r="BA10" s="2">
+        <v>0.53680000000000005</v>
+      </c>
+      <c r="BB10" s="2">
+        <v>0.91769999999999996</v>
+      </c>
+      <c r="BC10" s="2">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="BD10" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="BG10" s="2">
+        <v>1.4990000000000001</v>
+      </c>
+      <c r="BH10" s="2">
+        <f t="shared" si="17"/>
+        <v>0.20295552381033677</v>
+      </c>
+      <c r="BI10" s="2">
+        <f t="shared" si="18"/>
+        <v>0.70597293355965607</v>
+      </c>
+      <c r="BJ10" s="2">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="BK10" s="2">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="BL10" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="BM10" s="2">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="BN10" s="2">
+        <v>0.71599999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1962</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="O11" s="2">
         <v>4</v>
       </c>
-      <c r="R9" s="2">
+      <c r="P11" s="2">
+        <f t="shared" si="0"/>
+        <v>6.7216387142510672E-2</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.1894774723368661</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.93278361285748934</v>
+      </c>
+      <c r="S11" s="2">
         <v>0.78320000000000001</v>
       </c>
-      <c r="S9" s="2">
+      <c r="T11" s="2">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="O10" s="2">
+      <c r="V11" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="W11" s="2">
+        <f t="shared" si="3"/>
+        <v>2.6311497557258968E-2</v>
+      </c>
+      <c r="X11" s="2">
+        <f t="shared" si="4"/>
+        <v>8.0598842749763352E-2</v>
+      </c>
+      <c r="Y11" s="2">
+        <f t="shared" si="5"/>
+        <v>0.97368850244274108</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="AC11" s="2">
+        <f t="shared" si="6"/>
+        <v>0.20162517180028336</v>
+      </c>
+      <c r="AD11" s="2">
+        <f t="shared" si="7"/>
+        <v>0.70239938773207178</v>
+      </c>
+      <c r="AE11" s="2">
+        <f t="shared" si="8"/>
+        <v>0.79837482819971661</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="AH11" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="AI11" s="2">
+        <f t="shared" si="9"/>
+        <v>7.4276790313972899E-2</v>
+      </c>
+      <c r="AJ11" s="2">
+        <f t="shared" si="10"/>
+        <v>0.19240345945951545</v>
+      </c>
+      <c r="AK11" s="2">
+        <f t="shared" si="11"/>
+        <v>0.92572320968602706</v>
+      </c>
+      <c r="AL11" s="2">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="AN11" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="AO11" s="2">
+        <f t="shared" si="12"/>
+        <v>0.10057909215151825</v>
+      </c>
+      <c r="AP11" s="2">
+        <f t="shared" si="13"/>
+        <v>0.31636489920507044</v>
+      </c>
+      <c r="AQ11" s="2">
+        <f t="shared" si="14"/>
+        <v>0.89942090784848172</v>
+      </c>
+      <c r="AR11" s="2">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="AT11" s="8">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="AU11" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AV11" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AX11" s="2">
+        <v>0.2001</v>
+      </c>
+      <c r="AY11" s="2">
+        <f t="shared" si="15"/>
+        <v>1.6722888232988821E-2</v>
+      </c>
+      <c r="AZ11" s="2">
+        <f t="shared" si="16"/>
+        <v>7.4279542564348072E-2</v>
+      </c>
+      <c r="BA11" s="2">
+        <v>0.43940000000000001</v>
+      </c>
+      <c r="BB11" s="2">
+        <v>0.89759999999999995</v>
+      </c>
+      <c r="BC11" s="2">
+        <v>0.99350000000000005</v>
+      </c>
+      <c r="BD11" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="BG11" s="2">
+        <v>1.9970000000000001</v>
+      </c>
+      <c r="BH11" s="2">
+        <f t="shared" si="17"/>
+        <v>0.25330248815515605</v>
+      </c>
+      <c r="BI11" s="2">
+        <f t="shared" si="18"/>
+        <v>0.76183257274249183</v>
+      </c>
+      <c r="BJ11" s="2">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="BK11" s="2">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="BL11" s="2">
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="BM11" s="2">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="BN11" s="2">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="O12" s="2">
         <v>5</v>
       </c>
-      <c r="R10" s="2">
+      <c r="P12" s="2">
+        <f t="shared" si="0"/>
+        <v>8.2631928995711312E-2</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.22613496979991718</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" si="2"/>
+        <v>0.91736807100428863</v>
+      </c>
+      <c r="S12" s="2">
         <v>0.87470000000000003</v>
       </c>
-      <c r="S10" s="2">
+      <c r="T12" s="2">
         <v>0.93799999999999994</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="O11" s="2">
+      <c r="V12" s="2">
+        <v>2</v>
+      </c>
+      <c r="W12" s="2">
+        <f t="shared" si="3"/>
+        <v>3.4776985222435643E-2</v>
+      </c>
+      <c r="X12" s="2">
+        <f t="shared" si="4"/>
+        <v>0.10465347403405539</v>
+      </c>
+      <c r="Y12" s="2">
+        <f t="shared" si="5"/>
+        <v>0.96522301477756434</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC12" s="2">
+        <f t="shared" si="6"/>
+        <v>0.25190353146418937</v>
+      </c>
+      <c r="AD12" s="2">
+        <f t="shared" si="7"/>
+        <v>0.75885858242033788</v>
+      </c>
+      <c r="AE12" s="2">
+        <f t="shared" si="8"/>
+        <v>0.74809646853581069</v>
+      </c>
+      <c r="AF12" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="AH12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI12" s="2">
+        <f t="shared" si="9"/>
+        <v>9.6642944510389517E-2</v>
+      </c>
+      <c r="AJ12" s="2">
+        <f t="shared" si="10"/>
+        <v>0.24107662067511987</v>
+      </c>
+      <c r="AK12" s="2">
+        <f t="shared" si="11"/>
+        <v>0.90335705548961043</v>
+      </c>
+      <c r="AL12" s="2">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="AN12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AO12" s="2">
+        <f t="shared" si="12"/>
+        <v>0.12975523495738411</v>
+      </c>
+      <c r="AP12" s="2">
+        <f t="shared" si="13"/>
+        <v>0.38158032523007684</v>
+      </c>
+      <c r="AQ12" s="2">
+        <f t="shared" si="14"/>
+        <v>0.87024476504261594</v>
+      </c>
+      <c r="AR12" s="2">
+        <v>0.93630000000000002</v>
+      </c>
+      <c r="AT12" s="8">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="AU12" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AV12" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX12" s="2">
+        <v>0.29980000000000001</v>
+      </c>
+      <c r="AY12" s="2">
+        <f t="shared" si="15"/>
+        <v>2.4848043211501438E-2</v>
+      </c>
+      <c r="AZ12" s="2">
+        <f t="shared" si="16"/>
+        <v>0.10731758230290443</v>
+      </c>
+      <c r="BA12" s="2">
+        <v>0.38250000000000001</v>
+      </c>
+      <c r="BB12" s="2">
+        <v>0.88480000000000003</v>
+      </c>
+      <c r="BC12" s="2">
+        <v>0.99050000000000005</v>
+      </c>
+      <c r="BD12" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="BG12" s="2">
+        <v>2</v>
+      </c>
+      <c r="BH12" s="2">
+        <f t="shared" si="17"/>
+        <v>0.25358651678683924</v>
+      </c>
+      <c r="BI12" s="2">
+        <f t="shared" si="18"/>
+        <v>0.76210483556447217</v>
+      </c>
+      <c r="BJ12" s="2">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="BK12" s="2">
+        <v>0.624</v>
+      </c>
+      <c r="BL12" s="2">
+        <v>2.4980000000000002</v>
+      </c>
+      <c r="BM12" s="2">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="BN12" s="2">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1951</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="O13" s="2">
         <v>6</v>
       </c>
-      <c r="R11" s="2">
+      <c r="P13" s="2">
+        <f t="shared" si="0"/>
+        <v>9.7546228194460724E-2</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25962012589419375</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.90245377180553932</v>
+      </c>
+      <c r="S13" s="2">
         <v>0.98529999999999995</v>
       </c>
-      <c r="S11" s="2">
+      <c r="T13" s="2">
         <v>1.04</v>
+      </c>
+      <c r="V13" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="W13" s="2">
+        <f t="shared" si="3"/>
+        <v>4.3096539597861319E-2</v>
+      </c>
+      <c r="X13" s="2">
+        <f t="shared" si="4"/>
+        <v>0.12748149715449902</v>
+      </c>
+      <c r="Y13" s="2">
+        <f t="shared" si="5"/>
+        <v>0.95690346040213869</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="AC13" s="2">
+        <f t="shared" si="6"/>
+        <v>0.29622441995696414</v>
+      </c>
+      <c r="AD13" s="2">
+        <f t="shared" si="7"/>
+        <v>0.79731154989941444</v>
+      </c>
+      <c r="AE13" s="2">
+        <f t="shared" si="8"/>
+        <v>0.70377558004303586</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="AH13" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="AI13" s="2">
+        <f t="shared" si="9"/>
+        <v>0.11795382929319435</v>
+      </c>
+      <c r="AJ13" s="2">
+        <f t="shared" si="10"/>
+        <v>0.28421629958284483</v>
+      </c>
+      <c r="AK13" s="2">
+        <f t="shared" si="11"/>
+        <v>0.88204617070680569</v>
+      </c>
+      <c r="AL13" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="AN13" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="AO13" s="2">
+        <f t="shared" si="12"/>
+        <v>0.15709797260989863</v>
+      </c>
+      <c r="AP13" s="2">
+        <f t="shared" si="13"/>
+        <v>0.43543687083956412</v>
+      </c>
+      <c r="AQ13" s="2">
+        <f t="shared" si="14"/>
+        <v>0.84290202739010134</v>
+      </c>
+      <c r="AR13" s="2">
+        <v>0.92010000000000003</v>
+      </c>
+      <c r="AT13" s="8">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="AU13" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AV13" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="AX13" s="2">
+        <v>0.4002</v>
+      </c>
+      <c r="AY13" s="2">
+        <f t="shared" si="15"/>
+        <v>3.2895665921423928E-2</v>
+      </c>
+      <c r="AZ13" s="2">
+        <f t="shared" si="16"/>
+        <v>0.13828717688701364</v>
+      </c>
+      <c r="BA13" s="2">
+        <v>0.34320000000000001</v>
+      </c>
+      <c r="BB13" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="BC13" s="2">
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="BD13" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="BG13" s="2">
+        <v>2.4969999999999999</v>
+      </c>
+      <c r="BH13" s="2">
+        <f t="shared" si="17"/>
+        <v>0.29783436178013001</v>
+      </c>
+      <c r="BI13" s="2">
+        <f t="shared" si="18"/>
+        <v>0.79998440022501749</v>
+      </c>
+      <c r="BJ13" s="2">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="BK13" s="2">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="BL13" s="2">
+        <v>2.9980000000000002</v>
+      </c>
+      <c r="BM13" s="2">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="BN13" s="2">
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2024</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="V14" s="2">
+        <v>3</v>
+      </c>
+      <c r="W14" s="2">
+        <f t="shared" si="3"/>
+        <v>5.1273901968132293E-2</v>
+      </c>
+      <c r="X14" s="2">
+        <f t="shared" si="4"/>
+        <v>0.14917440138037943</v>
+      </c>
+      <c r="Y14" s="2">
+        <f t="shared" si="5"/>
+        <v>0.94872609803186769</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AC14" s="2">
+        <f t="shared" si="6"/>
+        <v>0.33558746359849817</v>
+      </c>
+      <c r="AD14" s="2">
+        <f t="shared" si="7"/>
+        <v>0.82518754740367339</v>
+      </c>
+      <c r="AE14" s="2">
+        <f t="shared" si="8"/>
+        <v>0.66441253640150189</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="AH14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI14" s="2">
+        <f t="shared" si="9"/>
+        <v>0.13828240725979835</v>
+      </c>
+      <c r="AJ14" s="2">
+        <f t="shared" si="10"/>
+        <v>0.3227153660669968</v>
+      </c>
+      <c r="AK14" s="2">
+        <f t="shared" si="11"/>
+        <v>0.86171759274020165</v>
+      </c>
+      <c r="AL14" s="2">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="AN14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AO14" s="2">
+        <f t="shared" si="12"/>
+        <v>0.18277485528985751</v>
+      </c>
+      <c r="AP14" s="2">
+        <f t="shared" si="13"/>
+        <v>0.480664440986109</v>
+      </c>
+      <c r="AQ14" s="2">
+        <f t="shared" si="14"/>
+        <v>0.81722514471014251</v>
+      </c>
+      <c r="AR14" s="2">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="AT14" s="8">
+        <v>0.871</v>
+      </c>
+      <c r="AU14" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AV14" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="AX14" s="2">
+        <v>0.50019999999999998</v>
+      </c>
+      <c r="AY14" s="2">
+        <f t="shared" si="15"/>
+        <v>4.0780266594919894E-2</v>
+      </c>
+      <c r="AZ14" s="2">
+        <f t="shared" si="16"/>
+        <v>0.16706871510031945</v>
+      </c>
+      <c r="BA14" s="2">
+        <v>0.31409999999999999</v>
+      </c>
+      <c r="BB14" s="2">
+        <v>0.86719999999999997</v>
+      </c>
+      <c r="BC14" s="2">
+        <v>0.98450000000000004</v>
+      </c>
+      <c r="BD14" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="BG14" s="2">
+        <v>2.5009999999999999</v>
+      </c>
+      <c r="BH14" s="2">
+        <f t="shared" si="17"/>
+        <v>0.29816921051903705</v>
+      </c>
+      <c r="BI14" s="2">
+        <f t="shared" si="18"/>
+        <v>0.8002403947272414</v>
+      </c>
+      <c r="BJ14" s="2">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="BK14" s="2">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="BL14" s="2">
+        <v>3</v>
+      </c>
+      <c r="BM14" s="2">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="BN14" s="2">
+        <v>0.60099999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2014</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="V15" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="W15" s="2">
+        <f t="shared" si="3"/>
+        <v>5.9312686814621103E-2</v>
+      </c>
+      <c r="X15" s="2">
+        <f t="shared" si="4"/>
+        <v>0.16981479813424177</v>
+      </c>
+      <c r="Y15" s="2">
+        <f t="shared" si="5"/>
+        <v>0.9406873131853789</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>0.872</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="AC15" s="2">
+        <f>$T$3*AB15/(1+$T$3*AB15)</f>
+        <v>0.37078049331438545</v>
+      </c>
+      <c r="AD15" s="2">
+        <f t="shared" si="7"/>
+        <v>0.84632294595670765</v>
+      </c>
+      <c r="AE15" s="2">
+        <f t="shared" si="8"/>
+        <v>0.62921950668561455</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="AH15" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="AI15" s="2">
+        <f t="shared" si="9"/>
+        <v>0.15769506624096574</v>
+      </c>
+      <c r="AJ15" s="2">
+        <f t="shared" si="10"/>
+        <v>0.3572843994516518</v>
+      </c>
+      <c r="AK15" s="2">
+        <f t="shared" si="11"/>
+        <v>0.84230493375903426</v>
+      </c>
+      <c r="AL15" s="2">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="AN15" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="AO15" s="2">
+        <f t="shared" si="12"/>
+        <v>0.20693362074058921</v>
+      </c>
+      <c r="AP15" s="2">
+        <f t="shared" si="13"/>
+        <v>0.51918304327307407</v>
+      </c>
+      <c r="AQ15" s="2">
+        <f t="shared" si="14"/>
+        <v>0.79306637925941081</v>
+      </c>
+      <c r="AR15" s="2">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="AT15" s="8">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="AU15" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AV15" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="AX15" s="2">
+        <v>0.59989999999999999</v>
+      </c>
+      <c r="AY15" s="2">
+        <f t="shared" si="15"/>
+        <v>4.8514260317260971E-2</v>
+      </c>
+      <c r="AZ15" s="2">
+        <f t="shared" si="16"/>
+        <v>0.19391160513049979</v>
+      </c>
+      <c r="BA15" s="2">
+        <v>0.29160000000000003</v>
+      </c>
+      <c r="BB15" s="2">
+        <v>0.86050000000000004</v>
+      </c>
+      <c r="BC15" s="2">
+        <v>0.98160000000000003</v>
+      </c>
+      <c r="BD15" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="BG15" s="2">
+        <v>2.9940000000000002</v>
+      </c>
+      <c r="BH15" s="2">
+        <f t="shared" si="17"/>
+        <v>0.33712971519022544</v>
+      </c>
+      <c r="BI15" s="2">
+        <f t="shared" si="18"/>
+        <v>0.827457924973381</v>
+      </c>
+      <c r="BJ15" s="2">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="BK15" s="2">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="BL15" s="2">
+        <v>3.4990000000000001</v>
+      </c>
+      <c r="BM15" s="2">
+        <v>0.93</v>
+      </c>
+      <c r="BN15" s="2">
+        <v>0.57499999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="V16" s="2">
+        <v>4</v>
+      </c>
+      <c r="W16" s="2">
+        <f t="shared" si="3"/>
+        <v>6.7216387142510672E-2</v>
+      </c>
+      <c r="X16" s="2">
+        <f t="shared" si="4"/>
+        <v>0.1894774723368661</v>
+      </c>
+      <c r="Y16" s="2">
+        <f t="shared" si="5"/>
+        <v>0.93278361285748934</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>4</v>
+      </c>
+      <c r="AC16" s="2">
+        <f t="shared" si="6"/>
+        <v>0.40243281552144905</v>
+      </c>
+      <c r="AD16" s="2">
+        <f t="shared" si="7"/>
+        <v>0.86289891638256044</v>
+      </c>
+      <c r="AE16" s="2">
+        <f t="shared" si="8"/>
+        <v>0.59756718447855095</v>
+      </c>
+      <c r="AF16" s="2">
+        <v>0.879</v>
+      </c>
+      <c r="AH16" s="2">
+        <v>4</v>
+      </c>
+      <c r="AI16" s="2">
+        <f t="shared" si="9"/>
+        <v>0.17625234356208255</v>
+      </c>
+      <c r="AJ16" s="2">
+        <f t="shared" si="10"/>
+        <v>0.38849595046594171</v>
+      </c>
+      <c r="AK16" s="2">
+        <f t="shared" si="11"/>
+        <v>0.82374765643791747</v>
+      </c>
+      <c r="AL16" s="2">
+        <v>0.873</v>
+      </c>
+      <c r="AN16" s="2">
+        <v>4</v>
+      </c>
+      <c r="AO16" s="2">
+        <f t="shared" si="12"/>
+        <v>0.22970503865340117</v>
+      </c>
+      <c r="AP16" s="2">
+        <f t="shared" si="13"/>
+        <v>0.55238239610358042</v>
+      </c>
+      <c r="AQ16" s="2">
+        <f t="shared" si="14"/>
+        <v>0.77029496134659881</v>
+      </c>
+      <c r="AR16" s="2">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="AT16" s="8">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="AU16" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AV16" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="AX16" s="2">
+        <v>0.70020000000000004</v>
+      </c>
+      <c r="AY16" s="2">
+        <f t="shared" si="15"/>
+        <v>5.6169966863452679E-2</v>
+      </c>
+      <c r="AZ16" s="2">
+        <f t="shared" si="16"/>
+        <v>0.21922507777099209</v>
+      </c>
+      <c r="BA16" s="2">
+        <v>0.27350000000000002</v>
+      </c>
+      <c r="BB16" s="2">
+        <v>0.85470000000000002</v>
+      </c>
+      <c r="BC16" s="2">
+        <v>0.97870000000000001</v>
+      </c>
+      <c r="BD16" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="BG16" s="2">
+        <v>2.9990000000000001</v>
+      </c>
+      <c r="BH16" s="2">
+        <f t="shared" si="17"/>
+        <v>0.33750270704675117</v>
+      </c>
+      <c r="BI16" s="2">
+        <f t="shared" si="18"/>
+        <v>0.82769602498945793</v>
+      </c>
+      <c r="BJ16" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="BK16" s="2">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="BL16" s="2">
+        <v>4.0060000000000002</v>
+      </c>
+      <c r="BM16" s="2">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="BN16" s="2">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2025</v>
+      </c>
+      <c r="V17" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="W17" s="2">
+        <f t="shared" si="3"/>
+        <v>7.4988379541517991E-2</v>
+      </c>
+      <c r="X17" s="2">
+        <f t="shared" si="4"/>
+        <v>0.20823028780433153</v>
+      </c>
+      <c r="Y17" s="2">
+        <f t="shared" si="5"/>
+        <v>0.92501162045848195</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="AC17" s="2">
+        <f t="shared" si="6"/>
+        <v>0.43105317462371995</v>
+      </c>
+      <c r="AD17" s="2">
+        <f t="shared" si="7"/>
+        <v>0.87624718737205387</v>
+      </c>
+      <c r="AE17" s="2">
+        <f t="shared" si="8"/>
+        <v>0.56894682537628005</v>
+      </c>
+      <c r="AF17" s="2">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="AH17" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="AI17" s="2">
+        <f t="shared" si="9"/>
+        <v>0.19400955662868707</v>
+      </c>
+      <c r="AJ17" s="2">
+        <f t="shared" si="10"/>
+        <v>0.41681650379759239</v>
+      </c>
+      <c r="AK17" s="2">
+        <f t="shared" si="11"/>
+        <v>0.80599044337131298</v>
+      </c>
+      <c r="AL17" s="2">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="AN17" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="AO17" s="2">
+        <f t="shared" si="12"/>
+        <v>0.25120527870326731</v>
+      </c>
+      <c r="AP17" s="2">
+        <f t="shared" si="13"/>
+        <v>0.58129318062265156</v>
+      </c>
+      <c r="AQ17" s="2">
+        <f t="shared" si="14"/>
+        <v>0.74879472129673275</v>
+      </c>
+      <c r="AR17" s="2">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="AT17" s="8">
+        <v>0.78</v>
+      </c>
+      <c r="AU17" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AV17" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="AX17" s="2">
+        <v>0.80020000000000002</v>
+      </c>
+      <c r="AY17" s="2">
+        <f t="shared" si="15"/>
+        <v>6.3681106710595001E-2</v>
+      </c>
+      <c r="AZ17" s="2">
+        <f t="shared" si="16"/>
+        <v>0.2429281809430828</v>
+      </c>
+      <c r="BA17" s="2">
+        <v>0.25890000000000002</v>
+      </c>
+      <c r="BB17" s="2">
+        <v>0.84950000000000003</v>
+      </c>
+      <c r="BC17" s="2">
+        <v>0.9758</v>
+      </c>
+      <c r="BD17" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="BG17" s="2">
+        <v>3.496</v>
+      </c>
+      <c r="BH17" s="2">
+        <f t="shared" si="17"/>
+        <v>0.3725944959271093</v>
+      </c>
+      <c r="BI17" s="2">
+        <f t="shared" si="18"/>
+        <v>0.84847966932907226</v>
+      </c>
+      <c r="BJ17" s="2">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="BK17" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="BL17" s="2">
+        <v>4.492</v>
+      </c>
+      <c r="BM17" s="2">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="BN17" s="2">
+        <v>0.53500000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V18" s="2">
+        <v>5</v>
+      </c>
+      <c r="W18" s="2">
+        <f t="shared" si="3"/>
+        <v>8.2631928995711312E-2</v>
+      </c>
+      <c r="X18" s="2">
+        <f t="shared" si="4"/>
+        <v>0.22613496979991718</v>
+      </c>
+      <c r="Y18" s="2">
+        <f t="shared" si="5"/>
+        <v>0.91736807100428863</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>5</v>
+      </c>
+      <c r="AC18" s="2">
+        <f t="shared" si="6"/>
+        <v>0.45705730488675578</v>
+      </c>
+      <c r="AD18" s="2">
+        <f t="shared" si="7"/>
+        <v>0.88722686942509832</v>
+      </c>
+      <c r="AE18" s="2">
+        <f t="shared" si="8"/>
+        <v>0.54294269511324422</v>
+      </c>
+      <c r="AF18" s="2">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="AH18" s="2">
+        <v>5</v>
+      </c>
+      <c r="AI18" s="2">
+        <f t="shared" si="9"/>
+        <v>0.21101735367330596</v>
+      </c>
+      <c r="AJ18" s="2">
+        <f t="shared" si="10"/>
+        <v>0.44262995209633699</v>
+      </c>
+      <c r="AK18" s="2">
+        <f t="shared" si="11"/>
+        <v>0.78898264632669401</v>
+      </c>
+      <c r="AL18" s="2">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="AT18" s="8">
+        <v>0.748</v>
+      </c>
+      <c r="AU18" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AV18" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="AX18" s="2">
+        <v>0.90010000000000001</v>
+      </c>
+      <c r="AY18" s="2">
+        <f t="shared" si="15"/>
+        <v>7.1066306676348431E-2</v>
+      </c>
+      <c r="AZ18" s="2">
+        <f t="shared" si="16"/>
+        <v>0.26521286011932754</v>
+      </c>
+      <c r="BA18" s="2">
+        <v>0.24679999999999999</v>
+      </c>
+      <c r="BB18" s="2">
+        <v>0.8448</v>
+      </c>
+      <c r="BC18" s="2">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="BD18" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="BG18" s="2">
+        <v>3.9950000000000001</v>
+      </c>
+      <c r="BH18" s="2">
+        <f t="shared" si="17"/>
+        <v>0.40427633678677316</v>
+      </c>
+      <c r="BI18" s="2">
+        <f t="shared" si="18"/>
+        <v>0.86484761840624835</v>
+      </c>
+      <c r="BJ18" s="2">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="BK18" s="2">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="BL18" s="2">
+        <v>5</v>
+      </c>
+      <c r="BM18" s="2">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="BN18" s="2">
+        <v>0.51100000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V19" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="W19" s="2">
+        <f t="shared" si="3"/>
+        <v>9.0150193456815117E-2</v>
+      </c>
+      <c r="X19" s="2">
+        <f t="shared" si="4"/>
+        <v>0.24324778375654069</v>
+      </c>
+      <c r="Y19" s="2">
+        <f t="shared" si="5"/>
+        <v>0.90984980654318492</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="AC19" s="2">
+        <f t="shared" si="6"/>
+        <v>0.48078825688416366</v>
+      </c>
+      <c r="AD19" s="2">
+        <f t="shared" si="7"/>
+        <v>0.8964170289391088</v>
+      </c>
+      <c r="AE19" s="2">
+        <f t="shared" si="8"/>
+        <v>0.51921174311583629</v>
+      </c>
+      <c r="AF19" s="2">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="AH19" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="AI19" s="2">
+        <f t="shared" si="9"/>
+        <v>0.22732219621302879</v>
+      </c>
+      <c r="AJ19" s="2">
+        <f t="shared" si="10"/>
+        <v>0.46625510004616011</v>
+      </c>
+      <c r="AK19" s="2">
+        <f t="shared" si="11"/>
+        <v>0.77267780378697126</v>
+      </c>
+      <c r="AL19" s="2">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="AT19" s="8">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="AV19" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AX19" s="2">
+        <v>1.002</v>
+      </c>
+      <c r="AY19" s="2">
+        <f t="shared" si="15"/>
+        <v>7.8480293247622956E-2</v>
+      </c>
+      <c r="AZ19" s="2">
+        <f t="shared" si="16"/>
+        <v>0.28663150195679926</v>
+      </c>
+      <c r="BA19" s="2">
+        <v>0.2366</v>
+      </c>
+      <c r="BB19" s="2">
+        <v>0.84040000000000004</v>
+      </c>
+      <c r="BC19" s="2">
+        <v>0.97009999999999996</v>
+      </c>
+      <c r="BD19" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="BG19" s="2">
+        <v>4.4969999999999999</v>
+      </c>
+      <c r="BH19" s="2">
+        <f t="shared" si="17"/>
+        <v>0.43307616969184493</v>
+      </c>
+      <c r="BI19" s="2">
+        <f t="shared" si="18"/>
+        <v>0.87809549523948771</v>
+      </c>
+      <c r="BJ19" s="2">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="BK19" s="2">
+        <v>0.501</v>
+      </c>
+      <c r="BL19" s="2">
+        <v>5.4989999999999997</v>
+      </c>
+      <c r="BM19" s="2">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="BN19" s="2">
+        <v>0.49199999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V20" s="2">
+        <v>6</v>
+      </c>
+      <c r="W20" s="2">
+        <f t="shared" si="3"/>
+        <v>9.7546228194460724E-2</v>
+      </c>
+      <c r="X20" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25962012589419375</v>
+      </c>
+      <c r="Y20" s="2">
+        <f t="shared" si="5"/>
+        <v>0.90245377180553932</v>
+      </c>
+      <c r="Z20" s="2">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>6</v>
+      </c>
+      <c r="AC20" s="2">
+        <f t="shared" si="6"/>
+        <v>0.50253161660310686</v>
+      </c>
+      <c r="AD20" s="2">
+        <f t="shared" si="7"/>
+        <v>0.90422219741472754</v>
+      </c>
+      <c r="AE20" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49746838339689314</v>
+      </c>
+      <c r="AF20" s="2">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="AH20" s="2">
+        <v>6</v>
+      </c>
+      <c r="AI20" s="2">
+        <f>$S$3*AH20/(1+$S$3*AH20)</f>
+        <v>0.24296678289649989</v>
+      </c>
+      <c r="AJ20" s="2">
+        <f>AI20*$S$3/(AI20*$S$3+(1-AI20)*$P$3)</f>
+        <v>0.48795889780364277</v>
+      </c>
+      <c r="AK20" s="2">
+        <f>1-AI20</f>
+        <v>0.75703321710350013</v>
+      </c>
+      <c r="AL20" s="2">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="AT20" s="8">
+        <v>0.68</v>
+      </c>
+      <c r="AV20" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="BG20" s="2">
+        <v>4.9859999999999998</v>
+      </c>
+      <c r="BH20" s="2">
+        <f t="shared" si="17"/>
+        <v>0.45857322284429874</v>
+      </c>
+      <c r="BI20" s="2">
+        <f t="shared" si="18"/>
+        <v>0.88872080714566659</v>
+      </c>
+      <c r="BJ20" s="2">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="BK20" s="2">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="BL20" s="2">
+        <v>6</v>
+      </c>
+      <c r="BM20" s="2">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="BN20" s="2">
+        <v>0.48199999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG21" s="2">
+        <v>4.9909999999999997</v>
+      </c>
+      <c r="BH21" s="2">
+        <f t="shared" si="17"/>
+        <v>0.45882208936917845</v>
+      </c>
+      <c r="BI21" s="2">
+        <f t="shared" si="18"/>
+        <v>0.88881989265984018</v>
+      </c>
+      <c r="BJ21" s="2">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="BK21" s="2">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="BL21" s="2">
+        <v>6.4950000000000001</v>
+      </c>
+      <c r="BM21" s="2">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="BN21" s="2">
+        <v>0.46899999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG22" s="2">
+        <v>5.4969999999999999</v>
+      </c>
+      <c r="BH22" s="2">
+        <f t="shared" si="17"/>
+        <v>0.48287686089541143</v>
+      </c>
+      <c r="BI22" s="2">
+        <f t="shared" si="18"/>
+        <v>0.89801026634902636</v>
+      </c>
+      <c r="BJ22" s="2">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="BK22" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="BL22" s="2">
+        <v>7</v>
+      </c>
+      <c r="BM22" s="2">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="BN22" s="2">
+        <v>0.45700000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG23" s="2">
+        <v>6.0090000000000003</v>
+      </c>
+      <c r="BH23" s="2">
+        <f t="shared" si="17"/>
+        <v>0.50513394581552229</v>
+      </c>
+      <c r="BI23" s="2">
+        <f t="shared" si="18"/>
+        <v>0.90588246542043027</v>
+      </c>
+      <c r="BJ23" s="2">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="BK23" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="BL23" s="2">
+        <v>7.4980000000000002</v>
+      </c>
+      <c r="BM23" s="2">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="BN23" s="2">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG24" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="BH24" s="2">
+        <f t="shared" si="17"/>
+        <v>0.52474984019713378</v>
+      </c>
+      <c r="BI24" s="2">
+        <f t="shared" si="18"/>
+        <v>0.91236894675964941</v>
+      </c>
+      <c r="BJ24" s="2">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="BK24" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="BL24" s="2">
+        <v>8.1010000000000009</v>
+      </c>
+      <c r="BM24" s="2">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="BN24" s="2">
+        <v>0.434</v>
+      </c>
+    </row>
+    <row r="25" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG25" s="2">
+        <v>6.9850000000000003</v>
+      </c>
+      <c r="BH25" s="2">
+        <f t="shared" si="17"/>
+        <v>0.54265684223437838</v>
+      </c>
+      <c r="BI25" s="2">
+        <f t="shared" si="18"/>
+        <v>0.91795434885155569</v>
+      </c>
+      <c r="BJ25" s="2">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="BK25" s="2">
+        <v>0.436</v>
+      </c>
+      <c r="BL25" s="2">
+        <v>9.016</v>
+      </c>
+      <c r="BM25" s="2">
+        <v>0.872</v>
+      </c>
+      <c r="BN25" s="2">
+        <v>0.42099999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG26" s="2">
+        <v>7.4950000000000001</v>
+      </c>
+      <c r="BH26" s="2">
+        <f t="shared" si="17"/>
+        <v>0.56008678871780104</v>
+      </c>
+      <c r="BI26" s="2">
+        <f t="shared" si="18"/>
+        <v>0.92310789978501107</v>
+      </c>
+      <c r="BJ26" s="2">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="BK26" s="2">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="BL26" s="2">
+        <v>9.9990000000000006</v>
+      </c>
+      <c r="BM26" s="2">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="BN26" s="2">
+        <v>0.41199999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG27" s="2">
+        <v>7.9480000000000004</v>
+      </c>
+      <c r="BH27" s="2">
+        <f t="shared" si="17"/>
+        <v>0.57449103724090178</v>
+      </c>
+      <c r="BI27" s="2">
+        <f t="shared" si="18"/>
+        <v>0.9271712290257752</v>
+      </c>
+      <c r="BJ27" s="2">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="BK27" s="2">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="BL27" s="2">
+        <v>11.02</v>
+      </c>
+      <c r="BM27" s="2">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="BN27" s="2">
+        <v>0.39700000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG28" s="2">
+        <v>7.9969999999999999</v>
+      </c>
+      <c r="BH28" s="2">
+        <f t="shared" si="17"/>
+        <v>0.57599277718960207</v>
+      </c>
+      <c r="BI28" s="2">
+        <f t="shared" si="18"/>
+        <v>0.92758515793215013</v>
+      </c>
+      <c r="BJ28" s="2">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="BK28" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="BL28" s="2">
+        <v>11.992000000000001</v>
+      </c>
+      <c r="BM28" s="2">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="BN28" s="2">
+        <v>0.38900000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG29" s="2">
+        <v>8.9870000000000001</v>
+      </c>
+      <c r="BH29" s="2">
+        <f t="shared" si="17"/>
+        <v>0.604214590590331</v>
+      </c>
+      <c r="BI29" s="2">
+        <f t="shared" si="18"/>
+        <v>0.93504415022326359</v>
+      </c>
+      <c r="BJ29" s="2">
+        <v>0.879</v>
+      </c>
+      <c r="BK29" s="2">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="BL29" s="2">
+        <v>12.997999999999999</v>
+      </c>
+      <c r="BM29" s="2">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="BN29" s="2">
+        <v>0.379</v>
+      </c>
+    </row>
+    <row r="30" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG30" s="2">
+        <v>9.9670000000000005</v>
+      </c>
+      <c r="BH30" s="2">
+        <f t="shared" si="17"/>
+        <v>0.62867991525094347</v>
+      </c>
+      <c r="BI30" s="2">
+        <f t="shared" si="18"/>
+        <v>0.94105442917687832</v>
+      </c>
+      <c r="BJ30" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="BK30" s="2">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="BL30" s="2">
+        <v>13.972</v>
+      </c>
+      <c r="BM30" s="2">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="BN30" s="2">
+        <v>0.377</v>
+      </c>
+    </row>
+    <row r="31" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG31" s="2">
+        <v>11.013</v>
+      </c>
+      <c r="BH31" s="2">
+        <f t="shared" si="17"/>
+        <v>0.65166240927882724</v>
+      </c>
+      <c r="BI31" s="2">
+        <f t="shared" si="18"/>
+        <v>0.94635265209091057</v>
+      </c>
+      <c r="BJ31" s="2">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="BK31" s="2">
+        <v>0.374</v>
+      </c>
+      <c r="BL31" s="2">
+        <v>15.007999999999999</v>
+      </c>
+      <c r="BM31" s="2">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="BN31" s="2">
+        <v>0.373</v>
+      </c>
+    </row>
+    <row r="32" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG32" s="2">
+        <v>11.999000000000001</v>
+      </c>
+      <c r="BH32" s="2">
+        <f t="shared" si="17"/>
+        <v>0.67086534204909554</v>
+      </c>
+      <c r="BI32" s="2">
+        <f t="shared" si="18"/>
+        <v>0.95054301748754755</v>
+      </c>
+      <c r="BJ32" s="2">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="BK32" s="2">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="BL32" s="2">
+        <v>15.779</v>
+      </c>
+      <c r="BM32" s="2">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="BN32" s="2">
+        <v>0.36799999999999999</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{9D68AF26-BC88-48F3-AD15-D7063E47E647}"/>
     <hyperlink ref="A4" r:id="rId2" location="abstract" xr:uid="{8642617F-EDF7-4B17-AEF5-18DF92DCFE33}"/>
-    <hyperlink ref="A6" r:id="rId3" xr:uid="{67E4DD68-33A8-493F-B9CE-7F0B03DD45AB}"/>
-    <hyperlink ref="A7" r:id="rId4" xr:uid="{B172C2B9-22E2-400D-9AE6-B101DAE0D864}"/>
+    <hyperlink ref="A8" r:id="rId3" xr:uid="{67E4DD68-33A8-493F-B9CE-7F0B03DD45AB}"/>
+    <hyperlink ref="A9" r:id="rId4" xr:uid="{B172C2B9-22E2-400D-9AE6-B101DAE0D864}"/>
+    <hyperlink ref="A11" r:id="rId5" xr:uid="{276B5A75-A52A-4EEB-BACC-259839441474}"/>
+    <hyperlink ref="A12" r:id="rId6" location="ref-doi_10.1016_j.jct.2016.12.003" xr:uid="{88A570D8-A2F5-43BF-B85C-874CAD57A655}"/>
+    <hyperlink ref="A13" r:id="rId7" xr:uid="{5D323EA8-16CA-417C-A5AC-E33822B23DBC}"/>
+    <hyperlink ref="A14" r:id="rId8" xr:uid="{D36FC1AF-9F08-446F-B52C-4002C8B7962B}"/>
+    <hyperlink ref="A15" r:id="rId9" xr:uid="{5BC2FFA3-BDD4-4796-90FC-33F2E8AC5983}"/>
+    <hyperlink ref="A16" r:id="rId10" xr:uid="{BD0A540B-8EC4-4001-BE15-3CBF3CEF38EB}"/>
+    <hyperlink ref="A17" r:id="rId11" location="fig0003" xr:uid="{A08C39A0-20C1-4E98-A85A-A81E8F1031B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
+  <drawing r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding polynomial fit script (naive) and updated endothermic data
</commit_message>
<xml_diff>
--- a/sources_list_.xlsx
+++ b/sources_list_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/peterbaz_stanford_edu/Documents/DiazMarin2026/hygroscopic-salts-main/hygroscopic-salts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1035" documentId="8_{0B5C881D-AA95-4664-BDBF-B508CE6D9B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AC49C39-A121-4ED9-A25F-66E13D083BF3}"/>
+  <xr:revisionPtr revIDLastSave="1098" documentId="8_{0B5C881D-AA95-4664-BDBF-B508CE6D9B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{900B135F-17BD-4147-8587-45637E796329}"/>
   <bookViews>
-    <workbookView xWindow="11565" yWindow="0" windowWidth="19530" windowHeight="20850" activeTab="3" xr2:uid="{A5D934FD-846B-4DBC-ADED-26484461699C}"/>
+    <workbookView xWindow="165" yWindow="360" windowWidth="19530" windowHeight="20850" activeTab="3" xr2:uid="{A5D934FD-846B-4DBC-ADED-26484461699C}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sources" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="305">
   <si>
     <t xml:space="preserve">Data Source </t>
   </si>
@@ -831,6 +831,129 @@
   </si>
   <si>
     <t>AgNO3 mass fraction</t>
+  </si>
+  <si>
+    <t>KI</t>
+  </si>
+  <si>
+    <t>Measurements and Calculations mean activity coefficients of KI in the KI–KCl–H2O ternary system at 298.15 K</t>
+  </si>
+  <si>
+    <t>Cites some other past paperbut not checking it out</t>
+  </si>
+  <si>
+    <t>KI–H2O binary system at 298.15 K and 95.5 kPa</t>
+  </si>
+  <si>
+    <t>Paper 13 (KI)</t>
+  </si>
+  <si>
+    <t>−0.0001</t>
+  </si>
+  <si>
+    <t>−0.0004</t>
+  </si>
+  <si>
+    <t>−0.0003</t>
+  </si>
+  <si>
+    <t>−0.0010</t>
+  </si>
+  <si>
+    <t>−0.0009</t>
+  </si>
+  <si>
+    <t>−0.0035</t>
+  </si>
+  <si>
+    <t>−0.0033</t>
+  </si>
+  <si>
+    <t>−0.0092</t>
+  </si>
+  <si>
+    <t>−0.0085</t>
+  </si>
+  <si>
+    <t>−0.0233</t>
+  </si>
+  <si>
+    <t>−0.0214</t>
+  </si>
+  <si>
+    <t>−0.0399</t>
+  </si>
+  <si>
+    <t>−0.0364</t>
+  </si>
+  <si>
+    <t>−0.0579</t>
+  </si>
+  <si>
+    <t>−0.0531</t>
+  </si>
+  <si>
+    <t>−0.0767</t>
+  </si>
+  <si>
+    <t>−0.0712</t>
+  </si>
+  <si>
+    <t>−0.0968</t>
+  </si>
+  <si>
+    <t>−0.0906</t>
+  </si>
+  <si>
+    <t>−0.1173</t>
+  </si>
+  <si>
+    <t>−0.1111</t>
+  </si>
+  <si>
+    <t>−0.1379</t>
+  </si>
+  <si>
+    <t>−0.1328</t>
+  </si>
+  <si>
+    <t>−0.1587</t>
+  </si>
+  <si>
+    <t>−0.1555</t>
+  </si>
+  <si>
+    <t>−0.1809</t>
+  </si>
+  <si>
+    <t>−0.1792</t>
+  </si>
+  <si>
+    <t>m0a/mol·kg−1</t>
+  </si>
+  <si>
+    <t>Φ</t>
+  </si>
+  <si>
+    <t>GE (kJ/mol)b</t>
+  </si>
+  <si>
+    <t>aw calc</t>
+  </si>
+  <si>
+    <t>Φ calc</t>
+  </si>
+  <si>
+    <t>GE (kJ/mol) calc</t>
+  </si>
+  <si>
+    <t>KI mole fraction</t>
+  </si>
+  <si>
+    <t>KI mass fraction</t>
+  </si>
+  <si>
+    <t>For this and next, my data has a before φ but φ was before a (def for model that was order done)</t>
   </si>
 </sst>
 </file>
@@ -895,7 +1018,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -916,9 +1039,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1240,15 +1360,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>56084</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>486382</xdr:rowOff>
+      <xdr:colOff>198104</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>188584</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>475480</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>374921</xdr:rowOff>
+      <xdr:rowOff>237210</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1271,8 +1391,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5882547" y="9758058"/>
-          <a:ext cx="1774042" cy="1124762"/>
+          <a:off x="6039339" y="9915181"/>
+          <a:ext cx="1356111" cy="856909"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>195090</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>511409</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>103282</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>106595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{461EEC33-00A4-18CA-52BD-43FE6DEC05F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6036325" y="11046289"/>
+          <a:ext cx="986927" cy="834583"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2353,10 +2517,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADEB32D0-53C4-465C-8106-B93762800774}">
-  <dimension ref="A1:BN32"/>
+  <dimension ref="A1:BT32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="BQ10" sqref="BQ10"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="AC7" sqref="AC7:AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2368,11 +2532,11 @@
     <col min="7" max="7" width="7.5703125" style="2" customWidth="1"/>
     <col min="8" max="13" width="8.5703125" style="2" customWidth="1"/>
     <col min="14" max="14" width="8.5703125" style="6" customWidth="1"/>
-    <col min="15" max="77" width="8.5703125" style="2" customWidth="1"/>
-    <col min="78" max="16384" width="20.5703125" style="2"/>
+    <col min="15" max="73" width="8.5703125" style="2" customWidth="1"/>
+    <col min="74" max="16384" width="20.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:72" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>227</v>
       </c>
@@ -2401,10 +2565,12 @@
       <c r="V1" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="W1" s="2"/>
+      <c r="W1" s="2" t="s">
+        <v>264</v>
+      </c>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -2453,8 +2619,11 @@
       <c r="V2" s="2">
         <v>169.87</v>
       </c>
-    </row>
-    <row r="3" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W2" s="2">
+        <v>165.99799999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>139</v>
       </c>
@@ -2480,35 +2649,39 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="P3" s="2">
-        <f>P2/1000</f>
+        <f t="shared" ref="P3:V3" si="0">P2/1000</f>
         <v>1.8015E-2</v>
       </c>
       <c r="Q3" s="2">
-        <f>Q2/1000</f>
+        <f t="shared" si="0"/>
         <v>5.8442999999999995E-2</v>
       </c>
       <c r="R3" s="2">
-        <f>R2/1000</f>
+        <f t="shared" si="0"/>
         <v>7.4551000000000006E-2</v>
       </c>
       <c r="S3" s="2">
-        <f>S2/1000</f>
+        <f t="shared" si="0"/>
         <v>5.3490999999999997E-2</v>
       </c>
       <c r="T3" s="2">
-        <f>T2/1000</f>
+        <f t="shared" si="0"/>
         <v>0.16836300000000001</v>
       </c>
       <c r="U3" s="2">
-        <f>U2/1000</f>
+        <f t="shared" si="0"/>
         <v>8.4994E-2</v>
       </c>
       <c r="V3" s="2">
-        <f>V2/1000</f>
+        <f t="shared" si="0"/>
         <v>0.16986999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W3" s="2">
+        <f>W2/1000</f>
+        <v>0.16599799999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>144</v>
       </c>
@@ -2534,48 +2707,51 @@
       <c r="V4" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="AN4" s="1" t="s">
+      <c r="AK4" s="1" t="s">
         <v>183</v>
       </c>
+      <c r="AP4" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="AT4" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AX4" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="BD4"/>
-      <c r="BE4" s="7"/>
-      <c r="BF4" s="1" t="s">
+      <c r="AZ4"/>
+      <c r="BA4" s="7"/>
+      <c r="BB4" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="5" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BL4" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S5" s="2" t="s">
         <v>156</v>
       </c>
       <c r="T5" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="Y5" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="AF5" s="2" t="s">
+      <c r="AD5" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="AL5" s="2" t="s">
+      <c r="AI5" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="AR5" s="2" t="s">
+      <c r="AN5" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>166</v>
       </c>
@@ -2622,88 +2798,79 @@
         <v>158</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="Z6" s="2" t="s">
         <v>171</v>
       </c>
+      <c r="AA6" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="AB6" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="AE6" s="2" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="AF6" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI6" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AH6" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="AI6" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AJ6" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="AK6" s="2" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="AL6" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="AM6" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="AN6" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AN6" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="AO6" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="AP6" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AQ6" s="2" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="AR6" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="AT6" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="AU6" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="AV6" s="2" t="s">
         <v>216</v>
+      </c>
+      <c r="AW6" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="BC6" s="2" t="s">
         <v>246</v>
       </c>
+      <c r="BF6" s="2" t="s">
+        <v>246</v>
+      </c>
       <c r="BG6" s="2" t="s">
         <v>246</v>
       </c>
+      <c r="BH6" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="BI6" s="2" t="s">
+        <v>256</v>
+      </c>
       <c r="BJ6" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="BK6" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="BL6" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="BM6" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="BN6" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="7" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BO6" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O7" s="2">
         <v>0.1</v>
       </c>
@@ -2737,123 +2904,134 @@
         <v>1.1553555115674923E-2</v>
       </c>
       <c r="Y7" s="2">
-        <f>1-W7</f>
-        <v>0.99640993500417996</v>
-      </c>
-      <c r="Z7" s="2">
         <v>0.99339999999999995</v>
       </c>
-      <c r="AA7"/>
+      <c r="Z7"/>
+      <c r="AA7" s="2">
+        <v>0.2</v>
+      </c>
       <c r="AB7" s="2">
+        <f>$T$3*AA7/(1+$T$3*AA7)</f>
+        <v>3.2575691761588726E-2</v>
+      </c>
+      <c r="AC7" s="2">
+        <f>AB7*$T$3/(AB7*$T$3+(1-AB7)*$P$3)</f>
+        <v>0.23936696943613739</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="AF7" s="2">
         <v>0.2</v>
       </c>
-      <c r="AC7" s="2">
-        <f>$T$3*AB7/(1+$T$3*AB7)</f>
-        <v>3.2575691761588726E-2</v>
-      </c>
-      <c r="AD7" s="2">
-        <f>AC7*$T$3/(AC7*$T$3+(1-AC7)*$P$3)</f>
-        <v>0.23936696943613739</v>
-      </c>
-      <c r="AE7" s="2">
-        <f>1-AC7</f>
-        <v>0.9674243082384113</v>
-      </c>
-      <c r="AF7" s="2">
+      <c r="AG7" s="2">
+        <f>$S$3*AF7/(1+$S$3*AF7)</f>
+        <v>1.0584959981129877E-2</v>
+      </c>
+      <c r="AH7" s="2">
+        <f>AG7*$S$3/(AG7*$S$3+(1-AG7)*$P$3)</f>
+        <v>3.0787619893897878E-2</v>
+      </c>
+      <c r="AI7" s="2">
         <v>0.99299999999999999</v>
       </c>
-      <c r="AH7" s="2">
+      <c r="AK7" s="2">
         <v>0.2</v>
       </c>
-      <c r="AI7" s="2">
-        <f>$S$3*AH7/(1+$S$3*AH7)</f>
-        <v>1.0584959981129877E-2</v>
-      </c>
-      <c r="AJ7" s="2">
-        <f>AI7*$S$3/(AI7*$S$3+(1-AI7)*$P$3)</f>
-        <v>3.0787619893897878E-2</v>
-      </c>
-      <c r="AK7" s="2">
-        <f>1-AI7</f>
-        <v>0.98941504001887015</v>
-      </c>
       <c r="AL7" s="2">
-        <v>0.99299999999999999</v>
+        <f>$R$3*AK7/(1+$R$3*AK7)</f>
+        <v>1.4691151985663363E-2</v>
+      </c>
+      <c r="AM7" s="2">
+        <f>AL7*$R$3/(AL7*$R$3+(1-AL7)*$P$3)</f>
+        <v>5.8116552083885414E-2</v>
       </c>
       <c r="AN7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="AO7" s="2">
-        <f>$R$3*AN7/(1+$R$3*AN7)</f>
-        <v>1.4691151985663363E-2</v>
+        <v>0.99350000000000005</v>
       </c>
       <c r="AP7" s="2">
-        <f>AO7*$R$3/(AO7*$R$3+(1-AO7)*$P$3)</f>
-        <v>5.8116552083885414E-2</v>
-      </c>
-      <c r="AQ7" s="2">
-        <f>1-AO7</f>
-        <v>0.9853088480143366</v>
-      </c>
-      <c r="AR7" s="2">
-        <v>0.99350000000000005</v>
-      </c>
-      <c r="AT7" s="8">
         <v>0.99329999999999996</v>
       </c>
+      <c r="AQ7" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AR7" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AT7" s="2" t="s">
+        <v>242</v>
+      </c>
       <c r="AU7" s="2" t="s">
-        <v>190</v>
+        <v>260</v>
       </c>
       <c r="AV7" s="2" t="s">
-        <v>202</v>
+        <v>261</v>
+      </c>
+      <c r="AW7" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="AX7" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AY7" s="2" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="AZ7" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="BA7" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="BB7" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="BC7" s="2" t="s">
-        <v>171</v>
+        <v>258</v>
       </c>
       <c r="BD7" s="2" t="s">
-        <v>244</v>
+        <v>262</v>
+      </c>
+      <c r="BE7" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="BF7" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="BG7" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="BH7" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="BH7" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="BI7" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BJ7" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="BL7" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="BM7" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="BN7" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="BO7" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="BK7" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="BL7" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="BM7" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="BN7" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="8" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BP7" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="BQ7" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="BR7" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="BS7" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="BT7" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>148</v>
       </c>
@@ -2873,15 +3051,15 @@
         <v>1</v>
       </c>
       <c r="P8" s="2">
-        <f t="shared" ref="P8:P13" si="0">$P$3*O8/(1+$P$3*O8)</f>
+        <f t="shared" ref="P8:P13" si="1">$P$3*O8/(1+$P$3*O8)</f>
         <v>1.7696202904672331E-2</v>
       </c>
       <c r="Q8" s="2">
-        <f t="shared" ref="Q8:Q13" si="1">P8*$Q$3/(P8*$Q$3+(1-P8)*$P$3)</f>
+        <f t="shared" ref="Q8:Q13" si="2">P8*$Q$3/(P8*$Q$3+(1-P8)*$P$3)</f>
         <v>5.5216010687396497E-2</v>
       </c>
       <c r="R8" s="2">
-        <f t="shared" ref="R8:R13" si="2">1-P8</f>
+        <f t="shared" ref="R8:R13" si="3">1-P8</f>
         <v>0.98230379709532767</v>
       </c>
       <c r="S8" s="2">
@@ -2894,134 +3072,147 @@
         <v>0.3</v>
       </c>
       <c r="W8" s="2">
-        <f t="shared" ref="W8:W20" si="3">$P$3*V8/(1+$P$3*V8)</f>
+        <f t="shared" ref="W8:W20" si="4">$P$3*V8/(1+$P$3*V8)</f>
         <v>5.3754483891806726E-3</v>
       </c>
       <c r="X8" s="2">
-        <f t="shared" ref="X8:X20" si="4">W8*$Q$3/(W8*$Q$3+(1-W8)*$P$3)</f>
+        <f t="shared" ref="X8:X20" si="5">W8*$Q$3/(W8*$Q$3+(1-W8)*$P$3)</f>
         <v>1.7230794208226582E-2</v>
       </c>
       <c r="Y8" s="2">
-        <f t="shared" ref="Y8:Y20" si="5">1-W8</f>
-        <v>0.99462455161081931</v>
-      </c>
-      <c r="Z8" s="2">
         <v>0.99</v>
       </c>
+      <c r="AA8" s="2">
+        <v>0.3</v>
+      </c>
       <c r="AB8" s="2">
+        <f t="shared" ref="AB8:AB20" si="6">$T$3*AA8/(1+$T$3*AA8)</f>
+        <v>4.8080411313031236E-2</v>
+      </c>
+      <c r="AC8" s="2">
+        <f t="shared" ref="AC8:AC20" si="7">AB8*$T$3/(AB8*$T$3+(1-AB8)*$P$3)</f>
+        <v>0.32067138531083489</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="AF8" s="2">
         <v>0.3</v>
       </c>
-      <c r="AC8" s="2">
-        <f t="shared" ref="AC8:AC20" si="6">$T$3*AB8/(1+$T$3*AB8)</f>
-        <v>4.8080411313031236E-2</v>
-      </c>
-      <c r="AD8" s="2">
-        <f t="shared" ref="AD8:AD20" si="7">AC8*$T$3/(AC8*$T$3+(1-AC8)*$P$3)</f>
-        <v>0.32067138531083489</v>
-      </c>
-      <c r="AE8" s="2">
-        <f t="shared" ref="AE8:AE20" si="8">1-AC8</f>
-        <v>0.9519195886869688</v>
-      </c>
-      <c r="AF8" s="2">
+      <c r="AG8" s="2">
+        <f t="shared" ref="AG8:AG19" si="8">$S$3*AF8/(1+$S$3*AF8)</f>
+        <v>1.5793851329559162E-2</v>
+      </c>
+      <c r="AH8" s="2">
+        <f t="shared" ref="AH8:AH19" si="9">AG8*$S$3/(AG8*$S$3+(1-AG8)*$P$3)</f>
+        <v>4.5481299362322918E-2</v>
+      </c>
+      <c r="AI8" s="2">
         <v>0.99</v>
       </c>
-      <c r="AH8" s="2">
+      <c r="AK8" s="2">
         <v>0.3</v>
       </c>
-      <c r="AI8" s="2">
-        <f t="shared" ref="AI8:AI20" si="9">$S$3*AH8/(1+$S$3*AH8)</f>
-        <v>1.5793851329559162E-2</v>
-      </c>
-      <c r="AJ8" s="2">
-        <f t="shared" ref="AJ8:AJ20" si="10">AI8*$S$3/(AI8*$S$3+(1-AI8)*$P$3)</f>
-        <v>4.5481299362322918E-2</v>
-      </c>
-      <c r="AK8" s="2">
-        <f t="shared" ref="AK8:AK20" si="11">1-AI8</f>
-        <v>0.98420614867044087</v>
-      </c>
       <c r="AL8" s="2">
-        <v>0.99</v>
+        <f t="shared" ref="AL8:AL17" si="10">$R$3*AK8/(1+$R$3*AK8)</f>
+        <v>2.1876035894410738E-2</v>
+      </c>
+      <c r="AM8" s="2">
+        <f t="shared" ref="AM8:AM17" si="11">AL8*$R$3/(AL8*$R$3+(1-AL8)*$P$3)</f>
+        <v>8.4713208333669743E-2</v>
       </c>
       <c r="AN8" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="AO8" s="2">
-        <f t="shared" ref="AO8:AO17" si="12">$R$3*AN8/(1+$R$3*AN8)</f>
-        <v>2.1876035894410738E-2</v>
+        <v>0.99029999999999996</v>
       </c>
       <c r="AP8" s="2">
-        <f t="shared" ref="AP8:AP17" si="13">AO8*$R$3/(AO8*$R$3+(1-AO8)*$P$3)</f>
-        <v>8.4713208333669743E-2</v>
-      </c>
-      <c r="AQ8" s="2">
-        <f t="shared" ref="AQ8:AQ20" si="14">1-AO8</f>
-        <v>0.97812396410558922</v>
-      </c>
-      <c r="AR8" s="2">
-        <v>0.99029999999999996</v>
-      </c>
-      <c r="AT8" s="8">
         <v>0.98980000000000001</v>
       </c>
-      <c r="AU8" s="2" t="s">
+      <c r="AQ8" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="AV8" s="2" t="s">
+      <c r="AR8" s="2" t="s">
         <v>203</v>
       </c>
+      <c r="AT8" s="2">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="AU8" s="2">
+        <f>$U$3*AT8/(1+$U$3*AT8)</f>
+        <v>8.6618786812902974E-4</v>
+      </c>
+      <c r="AV8" s="2">
+        <f>AU8*$U$3/(AU8*$U$3+(1-AU8)*$P$3)</f>
+        <v>4.0735187777003025E-3</v>
+      </c>
+      <c r="AW8" s="2">
+        <v>0.99960000000000004</v>
+      </c>
       <c r="AX8" s="2">
-        <v>1.0200000000000001E-2</v>
+        <v>0.79800000000000004</v>
       </c>
       <c r="AY8" s="2">
-        <f>$U$3*AX8/(1+$U$3*AX8)</f>
-        <v>8.6618786812902974E-4</v>
-      </c>
-      <c r="AZ8" s="2">
-        <f>AY8*$U$3/(AY8*$U$3+(1-AY8)*$P$3)</f>
-        <v>4.0735187777003025E-3</v>
-      </c>
-      <c r="BA8" s="2">
-        <v>0.79800000000000004</v>
-      </c>
-      <c r="BB8" s="2">
         <v>0.96589999999999998</v>
       </c>
+      <c r="AZ8" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="BC8" s="2">
-        <v>0.99960000000000004</v>
-      </c>
-      <c r="BD8" s="2" t="s">
-        <v>230</v>
+        <v>0.499</v>
+      </c>
+      <c r="BD8" s="2">
+        <f>$V$3*BC8/(1+$V$3*BC8)</f>
+        <v>7.8141459064046417E-2</v>
+      </c>
+      <c r="BE8" s="2">
+        <f>BD8*$V$3/(BD8*$V$3+(1-BD8)*$P$3)</f>
+        <v>0.44422253508640985</v>
+      </c>
+      <c r="BF8" s="2">
+        <v>0.98599999999999999</v>
       </c>
       <c r="BG8" s="2">
-        <v>0.499</v>
+        <v>0.78200000000000003</v>
       </c>
       <c r="BH8" s="2">
-        <f>$V$3*BG8/(1+$V$3*BG8)</f>
-        <v>7.8141459064046417E-2</v>
+        <v>0.5</v>
       </c>
       <c r="BI8" s="2">
-        <f>BH8*$V$3/(BH8*$V$3+(1-BH8)*$P$3)</f>
-        <v>0.44422253508640985</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="BJ8" s="2">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="BK8" s="2">
-        <v>0.78200000000000003</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="BL8" s="2">
-        <v>0.5</v>
+        <v>1E-3</v>
       </c>
       <c r="BM8" s="2">
-        <v>0.98299999999999998</v>
+        <f>$W$3*BL8/(1+$W$3*BL8)</f>
+        <v>1.6597044923736751E-4</v>
       </c>
       <c r="BN8" s="2">
-        <v>0.95099999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <f>BM8*$W$3/(BM8*$W$3+(1-BM8)*$P$3)</f>
+        <v>1.5272413186957615E-3</v>
+      </c>
+      <c r="BO8" s="2">
+        <v>1</v>
+      </c>
+      <c r="BP8" s="2">
+        <v>1</v>
+      </c>
+      <c r="BQ8" s="2">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="BR8" s="2">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="BS8" s="2">
+        <v>0</v>
+      </c>
+      <c r="BT8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>151</v>
       </c>
@@ -3035,15 +3226,15 @@
         <v>2</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.4776985222435643E-2</v>
       </c>
       <c r="Q9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.10465347403405539</v>
       </c>
       <c r="R9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.96522301477756434</v>
       </c>
       <c r="S9" s="2">
@@ -3056,147 +3247,160 @@
         <v>0.5</v>
       </c>
       <c r="W9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.9270892436379302E-3</v>
       </c>
       <c r="X9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.839184762463667E-2</v>
       </c>
       <c r="Y9" s="2">
-        <f t="shared" si="5"/>
-        <v>0.99107291075636206</v>
-      </c>
-      <c r="Z9" s="2">
         <v>0.98350000000000004</v>
       </c>
+      <c r="AA9" s="2">
+        <v>0.5</v>
+      </c>
       <c r="AB9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="AC9" s="2">
         <f t="shared" si="6"/>
         <v>7.7645209773455834E-2</v>
       </c>
-      <c r="AD9" s="2">
+      <c r="AC9" s="2">
         <f t="shared" si="7"/>
         <v>0.44032024106328244</v>
       </c>
-      <c r="AE9" s="2">
+      <c r="AD9" s="2">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AG9" s="2">
         <f t="shared" si="8"/>
-        <v>0.92235479022654421</v>
-      </c>
-      <c r="AF9" s="2">
+        <v>2.6048811511713465E-2</v>
+      </c>
+      <c r="AH9" s="2">
+        <f t="shared" si="9"/>
+        <v>7.3571416524238833E-2</v>
+      </c>
+      <c r="AI9" s="2">
         <v>0.98399999999999999</v>
       </c>
-      <c r="AH9" s="2">
+      <c r="AK9" s="2">
         <v>0.5</v>
       </c>
-      <c r="AI9" s="2">
-        <f t="shared" si="9"/>
-        <v>2.6048811511713465E-2</v>
-      </c>
-      <c r="AJ9" s="2">
+      <c r="AL9" s="2">
         <f t="shared" si="10"/>
-        <v>7.3571416524238833E-2</v>
-      </c>
-      <c r="AK9" s="2">
+        <v>3.5935968795175438E-2</v>
+      </c>
+      <c r="AM9" s="2">
         <f t="shared" si="11"/>
-        <v>0.97395118848828655</v>
-      </c>
-      <c r="AL9" s="2">
+        <v>0.13364122903781739</v>
+      </c>
+      <c r="AN9" s="2">
+        <v>0.9839</v>
+      </c>
+      <c r="AP9" s="2">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="AQ9" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="AR9" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AT9" s="2">
+        <v>5.0099999999999999E-2</v>
+      </c>
+      <c r="AU9" s="2">
+        <f t="shared" ref="AU9:AU19" si="12">$U$3*AT9/(1+$U$3*AT9)</f>
+        <v>4.2401440212727036E-3</v>
+      </c>
+      <c r="AV9" s="2">
+        <f t="shared" ref="AV9:AV19" si="13">AU9*$U$3/(AU9*$U$3+(1-AU9)*$P$3)</f>
+        <v>1.9694343352171489E-2</v>
+      </c>
+      <c r="AW9" s="2">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="AX9" s="2">
+        <v>0.62919999999999998</v>
+      </c>
+      <c r="AY9" s="2">
+        <v>0.9355</v>
+      </c>
+      <c r="AZ9" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="BC9" s="2">
+        <v>0.999</v>
+      </c>
+      <c r="BD9" s="2">
+        <f t="shared" ref="BD9:BD32" si="14">$V$3*BC9/(1+$V$3*BC9)</f>
+        <v>0.14508003004154577</v>
+      </c>
+      <c r="BE9" s="2">
+        <f t="shared" ref="BE9:BE32" si="15">BD9*$V$3/(BD9*$V$3+(1-BD9)*$P$3)</f>
+        <v>0.61540892858775742</v>
+      </c>
+      <c r="BF9" s="2">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="BG9" s="2">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="BH9" s="2">
+        <v>0.998</v>
+      </c>
+      <c r="BI9" s="2">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="BJ9" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="BL9" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="BM9" s="2">
+        <f t="shared" ref="BM9:BM23" si="16">$W$3*BL9/(1+$W$3*BL9)</f>
+        <v>3.3188581523688464E-4</v>
+      </c>
+      <c r="BN9" s="2">
+        <f t="shared" ref="BN9:BN23" si="17">BM9*$W$3/(BM9*$W$3+(1-BM9)*$P$3)</f>
+        <v>3.0498248189132953E-3</v>
+      </c>
+      <c r="BO9" s="2">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="BP9" s="2">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="BQ9" s="2">
         <v>0.98399999999999999</v>
       </c>
-      <c r="AN9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="AO9" s="2">
-        <f t="shared" si="12"/>
-        <v>3.5935968795175438E-2</v>
-      </c>
-      <c r="AP9" s="2">
-        <f t="shared" si="13"/>
-        <v>0.13364122903781739</v>
-      </c>
-      <c r="AQ9" s="2">
-        <f t="shared" si="14"/>
-        <v>0.96406403120482453</v>
-      </c>
-      <c r="AR9" s="2">
-        <v>0.9839</v>
-      </c>
-      <c r="AT9" s="8">
-        <v>0.98270000000000002</v>
-      </c>
-      <c r="AU9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="AV9" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="AX9" s="2">
-        <v>5.0099999999999999E-2</v>
-      </c>
-      <c r="AY9" s="2">
-        <f t="shared" ref="AY9:AY19" si="15">$U$3*AX9/(1+$U$3*AX9)</f>
-        <v>4.2401440212727036E-3</v>
-      </c>
-      <c r="AZ9" s="2">
-        <f t="shared" ref="AZ9:AZ19" si="16">AY9*$U$3/(AY9*$U$3+(1-AY9)*$P$3)</f>
-        <v>1.9694343352171489E-2</v>
-      </c>
-      <c r="BA9" s="2">
-        <v>0.62919999999999998</v>
-      </c>
-      <c r="BB9" s="2">
-        <v>0.9355</v>
-      </c>
-      <c r="BC9" s="2">
-        <v>0.99829999999999997</v>
-      </c>
-      <c r="BD9" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="BG9" s="2">
-        <v>0.999</v>
-      </c>
-      <c r="BH9" s="2">
-        <f t="shared" ref="BH9:BH32" si="17">$V$3*BG9/(1+$V$3*BG9)</f>
-        <v>0.14508003004154577</v>
-      </c>
-      <c r="BI9" s="2">
-        <f t="shared" ref="BI9:BI32" si="18">BH9*$V$3/(BH9*$V$3+(1-BH9)*$P$3)</f>
-        <v>0.61540892858775742</v>
-      </c>
-      <c r="BJ9" s="2">
-        <v>0.97399999999999998</v>
-      </c>
-      <c r="BK9" s="2">
-        <v>0.73099999999999998</v>
-      </c>
-      <c r="BL9" s="2">
-        <v>0.998</v>
-      </c>
-      <c r="BM9" s="2">
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="BN9" s="2">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BR9" s="2">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="BS9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BT9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O10" s="2">
         <v>3</v>
       </c>
       <c r="P10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.1273901968132293E-2</v>
       </c>
       <c r="Q10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.14917440138037943</v>
       </c>
       <c r="R10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.94872609803186769</v>
       </c>
       <c r="S10" s="2">
@@ -3209,134 +3413,147 @@
         <v>1</v>
       </c>
       <c r="W10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.7696202904672331E-2</v>
       </c>
       <c r="X10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.5216010687396497E-2</v>
       </c>
       <c r="Y10" s="2">
-        <f t="shared" si="5"/>
-        <v>0.98230379709532767</v>
-      </c>
-      <c r="Z10" s="2">
         <v>0.96699999999999997</v>
       </c>
+      <c r="AA10" s="2">
+        <v>1</v>
+      </c>
       <c r="AB10" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="2">
         <f t="shared" si="6"/>
         <v>0.14410161910296715</v>
       </c>
-      <c r="AD10" s="2">
+      <c r="AC10" s="2">
         <f t="shared" si="7"/>
         <v>0.61141991691823538</v>
       </c>
-      <c r="AE10" s="2">
+      <c r="AD10" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="AF10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="2">
         <f t="shared" si="8"/>
-        <v>0.85589838089703285</v>
-      </c>
-      <c r="AF10" s="2">
-        <v>0.97</v>
+        <v>5.0774994755531842E-2</v>
       </c>
       <c r="AH10" s="2">
+        <f t="shared" si="9"/>
+        <v>0.13705919399834871</v>
+      </c>
+      <c r="AI10" s="2">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="AK10" s="2">
         <v>1</v>
       </c>
-      <c r="AI10" s="2">
-        <f t="shared" si="9"/>
-        <v>5.0774994755531842E-2</v>
-      </c>
-      <c r="AJ10" s="2">
+      <c r="AL10" s="2">
         <f t="shared" si="10"/>
-        <v>0.13705919399834871</v>
-      </c>
-      <c r="AK10" s="2">
+        <v>6.9378745168912417E-2</v>
+      </c>
+      <c r="AM10" s="2">
         <f t="shared" si="11"/>
-        <v>0.94922500524446818</v>
-      </c>
-      <c r="AL10" s="2">
-        <v>0.96799999999999997</v>
+        <v>0.23577340981369546</v>
       </c>
       <c r="AN10" s="2">
-        <v>1</v>
-      </c>
-      <c r="AO10" s="2">
+        <v>0.96819999999999995</v>
+      </c>
+      <c r="AP10" s="2">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="AQ10" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AR10" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT10" s="2">
+        <v>0.1003</v>
+      </c>
+      <c r="AU10" s="2">
         <f t="shared" si="12"/>
-        <v>6.9378745168912417E-2</v>
-      </c>
-      <c r="AP10" s="2">
+        <v>8.4528386113373218E-3</v>
+      </c>
+      <c r="AV10" s="2">
         <f t="shared" si="13"/>
-        <v>0.23577340981369546</v>
-      </c>
-      <c r="AQ10" s="2">
+        <v>3.8664995157047646E-2</v>
+      </c>
+      <c r="AW10" s="2">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="AX10" s="2">
+        <v>0.53680000000000005</v>
+      </c>
+      <c r="AY10" s="2">
+        <v>0.91769999999999996</v>
+      </c>
+      <c r="AZ10" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="BC10" s="2">
+        <v>1.4990000000000001</v>
+      </c>
+      <c r="BD10" s="2">
         <f t="shared" si="14"/>
-        <v>0.9306212548310876</v>
-      </c>
-      <c r="AR10" s="2">
-        <v>0.96819999999999995</v>
-      </c>
-      <c r="AT10" s="8">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="AU10" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="AV10" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="AX10" s="2">
-        <v>0.1003</v>
-      </c>
-      <c r="AY10" s="2">
+        <v>0.20295552381033677</v>
+      </c>
+      <c r="BE10" s="2">
         <f t="shared" si="15"/>
-        <v>8.4528386113373218E-3</v>
-      </c>
-      <c r="AZ10" s="2">
+        <v>0.70597293355965607</v>
+      </c>
+      <c r="BF10" s="2">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="BG10" s="2">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="BH10" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="BI10" s="2">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="BJ10" s="2">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="BL10" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="BM10" s="2">
         <f t="shared" si="16"/>
-        <v>3.8664995157047646E-2</v>
-      </c>
-      <c r="BA10" s="2">
-        <v>0.53680000000000005</v>
-      </c>
-      <c r="BB10" s="2">
-        <v>0.91769999999999996</v>
-      </c>
-      <c r="BC10" s="2">
-        <v>0.99670000000000003</v>
-      </c>
-      <c r="BD10" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="BG10" s="2">
-        <v>1.4990000000000001</v>
-      </c>
-      <c r="BH10" s="2">
+        <v>8.293016878920665E-4</v>
+      </c>
+      <c r="BN10" s="2">
         <f t="shared" si="17"/>
-        <v>0.20295552381033677</v>
-      </c>
-      <c r="BI10" s="2">
-        <f t="shared" si="18"/>
-        <v>0.70597293355965607</v>
-      </c>
-      <c r="BJ10" s="2">
-        <v>0.96499999999999997</v>
-      </c>
-      <c r="BK10" s="2">
-        <v>0.65900000000000003</v>
-      </c>
-      <c r="BL10" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="BM10" s="2">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="BN10" s="2">
-        <v>0.71599999999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7.5898405212930873E-3</v>
+      </c>
+      <c r="BO10" s="2">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="BP10" s="2">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="BQ10" s="2">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="BR10" s="2">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="BS10" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="BT10" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>217</v>
       </c>
@@ -3353,15 +3570,15 @@
         <v>4</v>
       </c>
       <c r="P11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.7216387142510672E-2</v>
       </c>
       <c r="Q11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1894774723368661</v>
       </c>
       <c r="R11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.93278361285748934</v>
       </c>
       <c r="S11" s="2">
@@ -3374,134 +3591,147 @@
         <v>1.5</v>
       </c>
       <c r="W11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.6311497557258968E-2</v>
       </c>
       <c r="X11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.0598842749763352E-2</v>
       </c>
       <c r="Y11" s="2">
-        <f t="shared" si="5"/>
-        <v>0.97368850244274108</v>
-      </c>
-      <c r="Z11" s="2">
         <v>0.95</v>
       </c>
+      <c r="AA11" s="2">
+        <v>1.5</v>
+      </c>
       <c r="AB11" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="AC11" s="2">
         <f t="shared" si="6"/>
         <v>0.20162517180028336</v>
       </c>
-      <c r="AD11" s="2">
+      <c r="AC11" s="2">
         <f t="shared" si="7"/>
         <v>0.70239938773207178</v>
       </c>
-      <c r="AE11" s="2">
+      <c r="AD11" s="2">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="AG11" s="2">
         <f t="shared" si="8"/>
-        <v>0.79837482819971661</v>
-      </c>
-      <c r="AF11" s="2">
+        <v>7.4276790313972899E-2</v>
+      </c>
+      <c r="AH11" s="2">
+        <f t="shared" si="9"/>
+        <v>0.19240345945951545</v>
+      </c>
+      <c r="AI11" s="2">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="AK11" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="AL11" s="2">
+        <f t="shared" si="10"/>
+        <v>0.10057909215151825</v>
+      </c>
+      <c r="AM11" s="2">
+        <f t="shared" si="11"/>
+        <v>0.31636489920507044</v>
+      </c>
+      <c r="AN11" s="2">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="AP11" s="2">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="AQ11" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AR11" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AT11" s="2">
+        <v>0.2001</v>
+      </c>
+      <c r="AU11" s="2">
+        <f t="shared" si="12"/>
+        <v>1.6722888232988821E-2</v>
+      </c>
+      <c r="AV11" s="2">
+        <f t="shared" si="13"/>
+        <v>7.4279542564348072E-2</v>
+      </c>
+      <c r="AW11" s="2">
+        <v>0.99350000000000005</v>
+      </c>
+      <c r="AX11" s="2">
+        <v>0.43940000000000001</v>
+      </c>
+      <c r="AY11" s="2">
+        <v>0.89759999999999995</v>
+      </c>
+      <c r="AZ11" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="BC11" s="2">
+        <v>1.9970000000000001</v>
+      </c>
+      <c r="BD11" s="2">
+        <f t="shared" si="14"/>
+        <v>0.25330248815515605</v>
+      </c>
+      <c r="BE11" s="2">
+        <f t="shared" si="15"/>
+        <v>0.76183257274249183</v>
+      </c>
+      <c r="BF11" s="2">
         <v>0.95499999999999996</v>
       </c>
-      <c r="AH11" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="AI11" s="2">
-        <f t="shared" si="9"/>
-        <v>7.4276790313972899E-2</v>
-      </c>
-      <c r="AJ11" s="2">
-        <f t="shared" si="10"/>
-        <v>0.19240345945951545</v>
-      </c>
-      <c r="AK11" s="2">
-        <f t="shared" si="11"/>
-        <v>0.92572320968602706</v>
-      </c>
-      <c r="AL11" s="2">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="AN11" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="AO11" s="2">
-        <f t="shared" si="12"/>
-        <v>0.10057909215151825</v>
-      </c>
-      <c r="AP11" s="2">
-        <f t="shared" si="13"/>
-        <v>0.31636489920507044</v>
-      </c>
-      <c r="AQ11" s="2">
-        <f t="shared" si="14"/>
-        <v>0.89942090784848172</v>
-      </c>
-      <c r="AR11" s="2">
-        <v>0.95250000000000001</v>
-      </c>
-      <c r="AT11" s="8">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="AU11" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="AV11" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="AX11" s="2">
-        <v>0.2001</v>
-      </c>
-      <c r="AY11" s="2">
-        <f t="shared" si="15"/>
-        <v>1.6722888232988821E-2</v>
-      </c>
-      <c r="AZ11" s="2">
+      <c r="BG11" s="2">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="BH11" s="2">
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="BI11" s="2">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="BJ11" s="2">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="BL11" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="BM11" s="2">
         <f t="shared" si="16"/>
-        <v>7.4279542564348072E-2</v>
-      </c>
-      <c r="BA11" s="2">
-        <v>0.43940000000000001</v>
-      </c>
-      <c r="BB11" s="2">
-        <v>0.89759999999999995</v>
-      </c>
-      <c r="BC11" s="2">
-        <v>0.99350000000000005</v>
-      </c>
-      <c r="BD11" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="BG11" s="2">
-        <v>1.9970000000000001</v>
-      </c>
-      <c r="BH11" s="2">
+        <v>1.657229032949884E-3</v>
+      </c>
+      <c r="BN11" s="2">
         <f t="shared" si="17"/>
-        <v>0.25330248815515605</v>
-      </c>
-      <c r="BI11" s="2">
-        <f t="shared" si="18"/>
-        <v>0.76183257274249183</v>
-      </c>
-      <c r="BJ11" s="2">
-        <v>0.95499999999999996</v>
-      </c>
-      <c r="BK11" s="2">
-        <v>0.63900000000000001</v>
-      </c>
-      <c r="BL11" s="2">
-        <v>2.0009999999999999</v>
-      </c>
-      <c r="BM11" s="2">
-        <v>0.95299999999999996</v>
-      </c>
-      <c r="BN11" s="2">
-        <v>0.66700000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.5065337533308909E-2</v>
+      </c>
+      <c r="BO11" s="2">
+        <v>0.99970000000000003</v>
+      </c>
+      <c r="BP11" s="2">
+        <v>0.99970000000000003</v>
+      </c>
+      <c r="BQ11" s="2">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="BR11" s="2">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="BS11" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="BT11" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>221</v>
       </c>
@@ -3518,15 +3748,15 @@
         <v>5</v>
       </c>
       <c r="P12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.2631928995711312E-2</v>
       </c>
       <c r="Q12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.22613496979991718</v>
       </c>
       <c r="R12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.91736807100428863</v>
       </c>
       <c r="S12" s="2">
@@ -3539,134 +3769,145 @@
         <v>2</v>
       </c>
       <c r="W12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4776985222435643E-2</v>
       </c>
       <c r="X12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.10465347403405539</v>
       </c>
       <c r="Y12" s="2">
-        <f t="shared" si="5"/>
-        <v>0.96522301477756434</v>
-      </c>
-      <c r="Z12" s="2">
         <v>0.93200000000000005</v>
       </c>
+      <c r="AA12" s="2">
+        <v>2</v>
+      </c>
       <c r="AB12" s="2">
-        <v>2</v>
-      </c>
-      <c r="AC12" s="2">
         <f t="shared" si="6"/>
         <v>0.25190353146418937</v>
       </c>
-      <c r="AD12" s="2">
+      <c r="AC12" s="2">
         <f t="shared" si="7"/>
         <v>0.75885858242033788</v>
       </c>
-      <c r="AE12" s="2">
+      <c r="AD12" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="AF12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG12" s="2">
         <f t="shared" si="8"/>
-        <v>0.74809646853581069</v>
-      </c>
-      <c r="AF12" s="2">
-        <v>0.94</v>
+        <v>9.6642944510389517E-2</v>
       </c>
       <c r="AH12" s="2">
+        <f t="shared" si="9"/>
+        <v>0.24107662067511987</v>
+      </c>
+      <c r="AI12" s="2">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="AK12" s="2">
         <v>2</v>
       </c>
-      <c r="AI12" s="2">
-        <f t="shared" si="9"/>
-        <v>9.6642944510389517E-2</v>
-      </c>
-      <c r="AJ12" s="2">
+      <c r="AL12" s="2">
         <f t="shared" si="10"/>
-        <v>0.24107662067511987</v>
-      </c>
-      <c r="AK12" s="2">
+        <v>0.12975523495738411</v>
+      </c>
+      <c r="AM12" s="2">
         <f t="shared" si="11"/>
-        <v>0.90335705548961043</v>
-      </c>
-      <c r="AL12" s="2">
-        <v>0.93700000000000006</v>
+        <v>0.38158032523007684</v>
       </c>
       <c r="AN12" s="2">
+        <v>0.93630000000000002</v>
+      </c>
+      <c r="AP12" s="2">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="AQ12" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AR12" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AT12" s="2">
+        <v>0.29980000000000001</v>
+      </c>
+      <c r="AU12" s="2">
+        <f t="shared" si="12"/>
+        <v>2.4848043211501438E-2</v>
+      </c>
+      <c r="AV12" s="2">
+        <f t="shared" si="13"/>
+        <v>0.10731758230290443</v>
+      </c>
+      <c r="AW12" s="2">
+        <v>0.99050000000000005</v>
+      </c>
+      <c r="AX12" s="2">
+        <v>0.38250000000000001</v>
+      </c>
+      <c r="AY12" s="2">
+        <v>0.88480000000000003</v>
+      </c>
+      <c r="AZ12" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="BC12" s="2">
         <v>2</v>
       </c>
-      <c r="AO12" s="2">
-        <f t="shared" si="12"/>
-        <v>0.12975523495738411</v>
-      </c>
-      <c r="AP12" s="2">
-        <f t="shared" si="13"/>
-        <v>0.38158032523007684</v>
-      </c>
-      <c r="AQ12" s="2">
+      <c r="BD12" s="2">
         <f t="shared" si="14"/>
-        <v>0.87024476504261594</v>
-      </c>
-      <c r="AR12" s="2">
-        <v>0.93630000000000002</v>
-      </c>
-      <c r="AT12" s="8">
-        <v>0.92100000000000004</v>
-      </c>
-      <c r="AU12" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="AV12" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="AX12" s="2">
-        <v>0.29980000000000001</v>
-      </c>
-      <c r="AY12" s="2">
+        <v>0.25358651678683924</v>
+      </c>
+      <c r="BE12" s="2">
         <f t="shared" si="15"/>
-        <v>2.4848043211501438E-2</v>
-      </c>
-      <c r="AZ12" s="2">
+        <v>0.76210483556447217</v>
+      </c>
+      <c r="BF12" s="2">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="BG12" s="2">
+        <v>0.624</v>
+      </c>
+      <c r="BH12"/>
+      <c r="BI12" s="2">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="BJ12" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="BL12" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="BM12" s="2">
         <f t="shared" si="16"/>
-        <v>0.10731758230290443</v>
-      </c>
-      <c r="BA12" s="2">
-        <v>0.38250000000000001</v>
-      </c>
-      <c r="BB12" s="2">
-        <v>0.88480000000000003</v>
-      </c>
-      <c r="BC12" s="2">
-        <v>0.99050000000000005</v>
-      </c>
-      <c r="BD12" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="BG12" s="2">
-        <v>2</v>
-      </c>
-      <c r="BH12" s="2">
+        <v>3.3089743375582796E-3</v>
+      </c>
+      <c r="BN12" s="2">
         <f t="shared" si="17"/>
-        <v>0.25358651678683924</v>
-      </c>
-      <c r="BI12" s="2">
-        <f t="shared" si="18"/>
-        <v>0.76210483556447217</v>
-      </c>
-      <c r="BJ12" s="2">
-        <v>0.95599999999999996</v>
-      </c>
-      <c r="BK12" s="2">
-        <v>0.624</v>
-      </c>
-      <c r="BL12" s="2">
-        <v>2.4980000000000002</v>
-      </c>
-      <c r="BM12" s="2">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="BN12" s="2">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2.9683483370477211E-2</v>
+      </c>
+      <c r="BO12" s="2">
+        <v>0.99929999999999997</v>
+      </c>
+      <c r="BP12" s="2">
+        <v>0.99929999999999997</v>
+      </c>
+      <c r="BQ12" s="2">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="BR12" s="2">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="BS12" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="BT12" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>225</v>
       </c>
@@ -3680,15 +3921,15 @@
         <v>6</v>
       </c>
       <c r="P13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.7546228194460724E-2</v>
       </c>
       <c r="Q13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25962012589419375</v>
       </c>
       <c r="R13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.90245377180553932</v>
       </c>
       <c r="S13" s="2">
@@ -3701,134 +3942,147 @@
         <v>2.5</v>
       </c>
       <c r="W13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.3096539597861319E-2</v>
       </c>
       <c r="X13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.12748149715449902</v>
       </c>
       <c r="Y13" s="2">
-        <f t="shared" si="5"/>
-        <v>0.95690346040213869</v>
-      </c>
-      <c r="Z13" s="2">
         <v>0.91300000000000003</v>
       </c>
+      <c r="AA13" s="2">
+        <v>2.5</v>
+      </c>
       <c r="AB13" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="AC13" s="2">
         <f t="shared" si="6"/>
         <v>0.29622441995696414</v>
       </c>
-      <c r="AD13" s="2">
+      <c r="AC13" s="2">
         <f t="shared" si="7"/>
         <v>0.79731154989941444</v>
       </c>
-      <c r="AE13" s="2">
+      <c r="AD13" s="2">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="AG13" s="2">
         <f t="shared" si="8"/>
-        <v>0.70377558004303586</v>
-      </c>
-      <c r="AF13" s="2">
-        <v>0.92400000000000004</v>
+        <v>0.11795382929319435</v>
       </c>
       <c r="AH13" s="2">
+        <f t="shared" si="9"/>
+        <v>0.28421629958284483</v>
+      </c>
+      <c r="AI13" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="AK13" s="2">
         <v>2.5</v>
       </c>
-      <c r="AI13" s="2">
-        <f t="shared" si="9"/>
-        <v>0.11795382929319435</v>
-      </c>
-      <c r="AJ13" s="2">
+      <c r="AL13" s="2">
         <f t="shared" si="10"/>
-        <v>0.28421629958284483</v>
-      </c>
-      <c r="AK13" s="2">
+        <v>0.15709797260989863</v>
+      </c>
+      <c r="AM13" s="2">
         <f t="shared" si="11"/>
-        <v>0.88204617070680569</v>
-      </c>
-      <c r="AL13" s="2">
-        <v>0.92</v>
+        <v>0.43543687083956412</v>
       </c>
       <c r="AN13" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="AO13" s="2">
+        <v>0.92010000000000003</v>
+      </c>
+      <c r="AP13" s="2">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="AQ13" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AR13" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="AT13" s="2">
+        <v>0.4002</v>
+      </c>
+      <c r="AU13" s="2">
         <f t="shared" si="12"/>
-        <v>0.15709797260989863</v>
-      </c>
-      <c r="AP13" s="2">
+        <v>3.2895665921423928E-2</v>
+      </c>
+      <c r="AV13" s="2">
         <f t="shared" si="13"/>
-        <v>0.43543687083956412</v>
-      </c>
-      <c r="AQ13" s="2">
+        <v>0.13828717688701364</v>
+      </c>
+      <c r="AW13" s="2">
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="AX13" s="2">
+        <v>0.34320000000000001</v>
+      </c>
+      <c r="AY13" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="AZ13" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="BC13" s="2">
+        <v>2.4969999999999999</v>
+      </c>
+      <c r="BD13" s="2">
         <f t="shared" si="14"/>
-        <v>0.84290202739010134</v>
-      </c>
-      <c r="AR13" s="2">
-        <v>0.92010000000000003</v>
-      </c>
-      <c r="AT13" s="8">
-        <v>0.89700000000000002</v>
-      </c>
-      <c r="AU13" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="AV13" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="AX13" s="2">
-        <v>0.4002</v>
-      </c>
-      <c r="AY13" s="2">
+        <v>0.29783436178013001</v>
+      </c>
+      <c r="BE13" s="2">
         <f t="shared" si="15"/>
-        <v>3.2895665921423928E-2</v>
-      </c>
-      <c r="AZ13" s="2">
+        <v>0.79998440022501749</v>
+      </c>
+      <c r="BF13" s="2">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="BG13" s="2">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="BH13" s="2">
+        <v>2.9980000000000002</v>
+      </c>
+      <c r="BI13" s="2">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="BJ13" s="2">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="BL13" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="BM13" s="2">
         <f t="shared" si="16"/>
-        <v>0.13828717688701364</v>
-      </c>
-      <c r="BA13" s="2">
-        <v>0.34320000000000001</v>
-      </c>
-      <c r="BB13" s="2">
-        <v>0.875</v>
-      </c>
-      <c r="BC13" s="2">
-        <v>0.98750000000000004</v>
-      </c>
-      <c r="BD13" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="BG13" s="2">
-        <v>2.4969999999999999</v>
-      </c>
-      <c r="BH13" s="2">
+        <v>8.2315787197836665E-3</v>
+      </c>
+      <c r="BN13" s="2">
         <f t="shared" si="17"/>
-        <v>0.29783436178013001</v>
-      </c>
-      <c r="BI13" s="2">
-        <f t="shared" si="18"/>
-        <v>0.79998440022501749</v>
-      </c>
-      <c r="BJ13" s="2">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="BK13" s="2">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="BL13" s="2">
-        <v>2.9980000000000002</v>
-      </c>
-      <c r="BM13" s="2">
-        <v>0.93700000000000006</v>
-      </c>
-      <c r="BN13" s="2">
-        <v>0.60199999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7.1045396172442529E-2</v>
+      </c>
+      <c r="BO13" s="2">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="BP13" s="2">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="BQ13" s="2">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="BR13" s="2">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="BS13" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="BT13" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>226</v>
       </c>
@@ -3848,134 +4102,147 @@
         <v>3</v>
       </c>
       <c r="W14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.1273901968132293E-2</v>
       </c>
       <c r="X14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.14917440138037943</v>
       </c>
       <c r="Y14" s="2">
-        <f t="shared" si="5"/>
-        <v>0.94872609803186769</v>
-      </c>
-      <c r="Z14" s="2">
         <v>0.89400000000000002</v>
       </c>
+      <c r="AA14" s="2">
+        <v>3</v>
+      </c>
       <c r="AB14" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC14" s="2">
         <f t="shared" si="6"/>
         <v>0.33558746359849817</v>
       </c>
-      <c r="AD14" s="2">
+      <c r="AC14" s="2">
         <f t="shared" si="7"/>
         <v>0.82518754740367339</v>
       </c>
-      <c r="AE14" s="2">
+      <c r="AD14" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG14" s="2">
         <f t="shared" si="8"/>
-        <v>0.66441253640150189</v>
-      </c>
-      <c r="AF14" s="2">
-        <v>0.91</v>
+        <v>0.13828240725979835</v>
       </c>
       <c r="AH14" s="2">
+        <f t="shared" si="9"/>
+        <v>0.3227153660669968</v>
+      </c>
+      <c r="AI14" s="2">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="AK14" s="2">
         <v>3</v>
       </c>
-      <c r="AI14" s="2">
-        <f t="shared" si="9"/>
-        <v>0.13828240725979835</v>
-      </c>
-      <c r="AJ14" s="2">
+      <c r="AL14" s="2">
         <f t="shared" si="10"/>
-        <v>0.3227153660669968</v>
-      </c>
-      <c r="AK14" s="2">
+        <v>0.18277485528985751</v>
+      </c>
+      <c r="AM14" s="2">
         <f t="shared" si="11"/>
-        <v>0.86171759274020165</v>
-      </c>
-      <c r="AL14" s="2">
-        <v>0.90500000000000003</v>
+        <v>0.480664440986109</v>
       </c>
       <c r="AN14" s="2">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="AP14" s="2">
+        <v>0.871</v>
+      </c>
+      <c r="AQ14" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AR14" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="AT14" s="2">
+        <v>0.50019999999999998</v>
+      </c>
+      <c r="AU14" s="2">
+        <f t="shared" si="12"/>
+        <v>4.0780266594919894E-2</v>
+      </c>
+      <c r="AV14" s="2">
+        <f t="shared" si="13"/>
+        <v>0.16706871510031945</v>
+      </c>
+      <c r="AW14" s="2">
+        <v>0.98450000000000004</v>
+      </c>
+      <c r="AX14" s="2">
+        <v>0.31409999999999999</v>
+      </c>
+      <c r="AY14" s="2">
+        <v>0.86719999999999997</v>
+      </c>
+      <c r="AZ14" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="BC14" s="2">
+        <v>2.5009999999999999</v>
+      </c>
+      <c r="BD14" s="2">
+        <f t="shared" si="14"/>
+        <v>0.29816921051903705</v>
+      </c>
+      <c r="BE14" s="2">
+        <f t="shared" si="15"/>
+        <v>0.8002403947272414</v>
+      </c>
+      <c r="BF14" s="2">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="BG14" s="2">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="BH14" s="2">
         <v>3</v>
       </c>
-      <c r="AO14" s="2">
-        <f t="shared" si="12"/>
-        <v>0.18277485528985751</v>
-      </c>
-      <c r="AP14" s="2">
-        <f t="shared" si="13"/>
-        <v>0.480664440986109</v>
-      </c>
-      <c r="AQ14" s="2">
-        <f t="shared" si="14"/>
-        <v>0.81722514471014251</v>
-      </c>
-      <c r="AR14" s="2">
-        <v>0.90400000000000003</v>
-      </c>
-      <c r="AT14" s="8">
-        <v>0.871</v>
-      </c>
-      <c r="AU14" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="AV14" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="AX14" s="2">
-        <v>0.50019999999999998</v>
-      </c>
-      <c r="AY14" s="2">
-        <f t="shared" si="15"/>
-        <v>4.0780266594919894E-2</v>
-      </c>
-      <c r="AZ14" s="2">
+      <c r="BI14" s="2">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="BJ14" s="2">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="BL14" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BM14" s="2">
         <f t="shared" si="16"/>
-        <v>0.16706871510031945</v>
-      </c>
-      <c r="BA14" s="2">
-        <v>0.31409999999999999</v>
-      </c>
-      <c r="BB14" s="2">
-        <v>0.86719999999999997</v>
-      </c>
-      <c r="BC14" s="2">
-        <v>0.98450000000000004</v>
-      </c>
-      <c r="BD14" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="BG14" s="2">
-        <v>2.5009999999999999</v>
-      </c>
-      <c r="BH14" s="2">
+        <v>1.6328746080807803E-2</v>
+      </c>
+      <c r="BN14" s="2">
         <f t="shared" si="17"/>
-        <v>0.29816921051903705</v>
-      </c>
-      <c r="BI14" s="2">
-        <f t="shared" si="18"/>
-        <v>0.8002403947272414</v>
-      </c>
-      <c r="BJ14" s="2">
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="BK14" s="2">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="BL14" s="2">
-        <v>3</v>
-      </c>
-      <c r="BM14" s="2">
-        <v>0.93700000000000006</v>
-      </c>
-      <c r="BN14" s="2">
-        <v>0.60099999999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.13266551805616264</v>
+      </c>
+      <c r="BO14" s="2">
+        <v>0.99660000000000004</v>
+      </c>
+      <c r="BP14" s="2">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="BQ14" s="2">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="BR14" s="2">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="BS14" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="BT14" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>247</v>
       </c>
@@ -3992,134 +4259,147 @@
         <v>3.5</v>
       </c>
       <c r="W15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.9312686814621103E-2</v>
       </c>
       <c r="X15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.16981479813424177</v>
       </c>
       <c r="Y15" s="2">
-        <f t="shared" si="5"/>
-        <v>0.9406873131853789</v>
-      </c>
-      <c r="Z15" s="2">
         <v>0.872</v>
       </c>
+      <c r="AA15" s="2">
+        <v>3.5</v>
+      </c>
       <c r="AB15" s="2">
-        <v>3.5</v>
+        <f>$T$3*AA15/(1+$T$3*AA15)</f>
+        <v>0.37078049331438545</v>
       </c>
       <c r="AC15" s="2">
-        <f>$T$3*AB15/(1+$T$3*AB15)</f>
-        <v>0.37078049331438545</v>
-      </c>
-      <c r="AD15" s="2">
         <f t="shared" si="7"/>
         <v>0.84632294595670765</v>
       </c>
-      <c r="AE15" s="2">
+      <c r="AD15" s="2">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="AG15" s="2">
         <f t="shared" si="8"/>
-        <v>0.62921950668561455</v>
-      </c>
-      <c r="AF15" s="2">
-        <v>0.89400000000000002</v>
+        <v>0.15769506624096574</v>
       </c>
       <c r="AH15" s="2">
+        <f t="shared" si="9"/>
+        <v>0.3572843994516518</v>
+      </c>
+      <c r="AI15" s="2">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="AK15" s="2">
         <v>3.5</v>
       </c>
-      <c r="AI15" s="2">
-        <f t="shared" si="9"/>
-        <v>0.15769506624096574</v>
-      </c>
-      <c r="AJ15" s="2">
+      <c r="AL15" s="2">
         <f t="shared" si="10"/>
-        <v>0.3572843994516518</v>
-      </c>
-      <c r="AK15" s="2">
+        <v>0.20693362074058921</v>
+      </c>
+      <c r="AM15" s="2">
         <f t="shared" si="11"/>
-        <v>0.84230493375903426</v>
-      </c>
-      <c r="AL15" s="2">
-        <v>0.88900000000000001</v>
+        <v>0.51918304327307407</v>
       </c>
       <c r="AN15" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="AO15" s="2">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="AP15" s="2">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="AQ15" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AR15" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="AT15" s="2">
+        <v>0.59989999999999999</v>
+      </c>
+      <c r="AU15" s="2">
         <f t="shared" si="12"/>
-        <v>0.20693362074058921</v>
-      </c>
-      <c r="AP15" s="2">
+        <v>4.8514260317260971E-2</v>
+      </c>
+      <c r="AV15" s="2">
         <f t="shared" si="13"/>
-        <v>0.51918304327307407</v>
-      </c>
-      <c r="AQ15" s="2">
+        <v>0.19391160513049979</v>
+      </c>
+      <c r="AW15" s="2">
+        <v>0.98160000000000003</v>
+      </c>
+      <c r="AX15" s="2">
+        <v>0.29160000000000003</v>
+      </c>
+      <c r="AY15" s="2">
+        <v>0.86050000000000004</v>
+      </c>
+      <c r="AZ15" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="BC15" s="2">
+        <v>2.9940000000000002</v>
+      </c>
+      <c r="BD15" s="2">
         <f t="shared" si="14"/>
-        <v>0.79306637925941081</v>
-      </c>
-      <c r="AR15" s="2">
-        <v>0.88700000000000001</v>
-      </c>
-      <c r="AT15" s="8">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="AU15" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="AV15" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="AX15" s="2">
-        <v>0.59989999999999999</v>
-      </c>
-      <c r="AY15" s="2">
+        <v>0.33712971519022544</v>
+      </c>
+      <c r="BE15" s="2">
         <f t="shared" si="15"/>
-        <v>4.8514260317260971E-2</v>
-      </c>
-      <c r="AZ15" s="2">
+        <v>0.827457924973381</v>
+      </c>
+      <c r="BF15" s="2">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="BG15" s="2">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="BH15" s="2">
+        <v>3.4990000000000001</v>
+      </c>
+      <c r="BI15" s="2">
+        <v>0.93</v>
+      </c>
+      <c r="BJ15" s="2">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="BL15" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="BM15" s="2">
         <f t="shared" si="16"/>
-        <v>0.19391160513049979</v>
-      </c>
-      <c r="BA15" s="2">
-        <v>0.29160000000000003</v>
-      </c>
-      <c r="BB15" s="2">
-        <v>0.86050000000000004</v>
-      </c>
-      <c r="BC15" s="2">
-        <v>0.98160000000000003</v>
-      </c>
-      <c r="BD15" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="BG15" s="2">
-        <v>2.9940000000000002</v>
-      </c>
-      <c r="BH15" s="2">
+        <v>3.2132803768023133E-2</v>
+      </c>
+      <c r="BN15" s="2">
         <f t="shared" si="17"/>
-        <v>0.33712971519022544</v>
-      </c>
-      <c r="BI15" s="2">
-        <f t="shared" si="18"/>
-        <v>0.827457924973381</v>
-      </c>
-      <c r="BJ15" s="2">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="BK15" s="2">
-        <v>0.56299999999999994</v>
-      </c>
-      <c r="BL15" s="2">
-        <v>3.4990000000000001</v>
-      </c>
-      <c r="BM15" s="2">
-        <v>0.93</v>
-      </c>
-      <c r="BN15" s="2">
-        <v>0.57499999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.23425365377739787</v>
+      </c>
+      <c r="BO15" s="2">
+        <v>0.99339999999999995</v>
+      </c>
+      <c r="BP15" s="2">
+        <v>0.99350000000000005</v>
+      </c>
+      <c r="BQ15" s="2">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="BR15" s="2">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="BS15" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="BT15" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>249</v>
       </c>
@@ -4133,134 +4413,147 @@
         <v>4</v>
       </c>
       <c r="W16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.7216387142510672E-2</v>
       </c>
       <c r="X16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.1894774723368661</v>
       </c>
       <c r="Y16" s="2">
-        <f t="shared" si="5"/>
-        <v>0.93278361285748934</v>
-      </c>
-      <c r="Z16" s="2">
         <v>0.85199999999999998</v>
       </c>
+      <c r="AA16" s="2">
+        <v>4</v>
+      </c>
       <c r="AB16" s="2">
-        <v>4</v>
-      </c>
-      <c r="AC16" s="2">
         <f t="shared" si="6"/>
         <v>0.40243281552144905</v>
       </c>
-      <c r="AD16" s="2">
+      <c r="AC16" s="2">
         <f t="shared" si="7"/>
         <v>0.86289891638256044</v>
       </c>
-      <c r="AE16" s="2">
+      <c r="AD16" s="2">
+        <v>0.879</v>
+      </c>
+      <c r="AF16" s="2">
+        <v>4</v>
+      </c>
+      <c r="AG16" s="2">
         <f t="shared" si="8"/>
-        <v>0.59756718447855095</v>
-      </c>
-      <c r="AF16" s="2">
-        <v>0.879</v>
+        <v>0.17625234356208255</v>
       </c>
       <c r="AH16" s="2">
+        <f t="shared" si="9"/>
+        <v>0.38849595046594171</v>
+      </c>
+      <c r="AI16" s="2">
+        <v>0.873</v>
+      </c>
+      <c r="AK16" s="2">
         <v>4</v>
       </c>
-      <c r="AI16" s="2">
-        <f t="shared" si="9"/>
-        <v>0.17625234356208255</v>
-      </c>
-      <c r="AJ16" s="2">
+      <c r="AL16" s="2">
         <f t="shared" si="10"/>
-        <v>0.38849595046594171</v>
-      </c>
-      <c r="AK16" s="2">
+        <v>0.22970503865340117</v>
+      </c>
+      <c r="AM16" s="2">
         <f t="shared" si="11"/>
-        <v>0.82374765643791747</v>
-      </c>
-      <c r="AL16" s="2">
-        <v>0.873</v>
+        <v>0.55238239610358042</v>
       </c>
       <c r="AN16" s="2">
-        <v>4</v>
-      </c>
-      <c r="AO16" s="2">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="AP16" s="2">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="AQ16" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR16" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="AT16" s="2">
+        <v>0.70020000000000004</v>
+      </c>
+      <c r="AU16" s="2">
         <f t="shared" si="12"/>
-        <v>0.22970503865340117</v>
-      </c>
-      <c r="AP16" s="2">
+        <v>5.6169966863452679E-2</v>
+      </c>
+      <c r="AV16" s="2">
         <f t="shared" si="13"/>
-        <v>0.55238239610358042</v>
-      </c>
-      <c r="AQ16" s="2">
+        <v>0.21922507777099209</v>
+      </c>
+      <c r="AW16" s="2">
+        <v>0.97870000000000001</v>
+      </c>
+      <c r="AX16" s="2">
+        <v>0.27350000000000002</v>
+      </c>
+      <c r="AY16" s="2">
+        <v>0.85470000000000002</v>
+      </c>
+      <c r="AZ16" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="BC16" s="2">
+        <v>2.9990000000000001</v>
+      </c>
+      <c r="BD16" s="2">
         <f t="shared" si="14"/>
-        <v>0.77029496134659881</v>
-      </c>
-      <c r="AR16" s="2">
-        <v>0.86899999999999999</v>
-      </c>
-      <c r="AT16" s="8">
-        <v>0.81100000000000005</v>
-      </c>
-      <c r="AU16" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AV16" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="AX16" s="2">
-        <v>0.70020000000000004</v>
-      </c>
-      <c r="AY16" s="2">
+        <v>0.33750270704675117</v>
+      </c>
+      <c r="BE16" s="2">
         <f t="shared" si="15"/>
-        <v>5.6169966863452679E-2</v>
-      </c>
-      <c r="AZ16" s="2">
+        <v>0.82769602498945793</v>
+      </c>
+      <c r="BF16" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="BG16" s="2">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="BH16" s="2">
+        <v>4.0060000000000002</v>
+      </c>
+      <c r="BI16" s="2">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="BJ16" s="2">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="BL16" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="BM16" s="2">
         <f t="shared" si="16"/>
-        <v>0.21922507777099209</v>
-      </c>
-      <c r="BA16" s="2">
-        <v>0.27350000000000002</v>
-      </c>
-      <c r="BB16" s="2">
-        <v>0.85470000000000002</v>
-      </c>
-      <c r="BC16" s="2">
-        <v>0.97870000000000001</v>
-      </c>
-      <c r="BD16" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="BG16" s="2">
-        <v>2.9990000000000001</v>
-      </c>
-      <c r="BH16" s="2">
+        <v>4.7437062737890681E-2</v>
+      </c>
+      <c r="BN16" s="2">
         <f t="shared" si="17"/>
-        <v>0.33750270704675117</v>
-      </c>
-      <c r="BI16" s="2">
-        <f t="shared" si="18"/>
-        <v>0.82769602498945793</v>
-      </c>
-      <c r="BJ16" s="2">
-        <v>0.94</v>
-      </c>
-      <c r="BK16" s="2">
-        <v>0.57199999999999995</v>
-      </c>
-      <c r="BL16" s="2">
-        <v>4.0060000000000002</v>
-      </c>
-      <c r="BM16" s="2">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="BN16" s="2">
-        <v>0.55500000000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.31453947054939485</v>
+      </c>
+      <c r="BO16" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="BP16" s="2">
+        <v>0.99029999999999996</v>
+      </c>
+      <c r="BQ16" s="2">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="BR16" s="2">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="BS16" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="BT16" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>252</v>
       </c>
@@ -4270,783 +4563,952 @@
       <c r="C17" s="2">
         <v>2025</v>
       </c>
+      <c r="E17" s="2" t="s">
+        <v>304</v>
+      </c>
       <c r="V17" s="2">
         <v>4.5</v>
       </c>
       <c r="W17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.4988379541517991E-2</v>
       </c>
       <c r="X17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.20823028780433153</v>
       </c>
       <c r="Y17" s="2">
-        <f t="shared" si="5"/>
-        <v>0.92501162045848195</v>
-      </c>
-      <c r="Z17" s="2">
         <v>0.83</v>
       </c>
+      <c r="AA17" s="2">
+        <v>4.5</v>
+      </c>
       <c r="AB17" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="AC17" s="2">
         <f t="shared" si="6"/>
         <v>0.43105317462371995</v>
       </c>
-      <c r="AD17" s="2">
+      <c r="AC17" s="2">
         <f t="shared" si="7"/>
         <v>0.87624718737205387</v>
       </c>
-      <c r="AE17" s="2">
+      <c r="AD17" s="2">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="AF17" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="AG17" s="2">
         <f t="shared" si="8"/>
-        <v>0.56894682537628005</v>
-      </c>
-      <c r="AF17" s="2">
-        <v>0.86299999999999999</v>
+        <v>0.19400955662868707</v>
       </c>
       <c r="AH17" s="2">
+        <f t="shared" si="9"/>
+        <v>0.41681650379759239</v>
+      </c>
+      <c r="AI17" s="2">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="AK17" s="2">
         <v>4.5</v>
       </c>
-      <c r="AI17" s="2">
-        <f t="shared" si="9"/>
-        <v>0.19400955662868707</v>
-      </c>
-      <c r="AJ17" s="2">
+      <c r="AL17" s="2">
         <f t="shared" si="10"/>
-        <v>0.41681650379759239</v>
-      </c>
-      <c r="AK17" s="2">
+        <v>0.25120527870326731</v>
+      </c>
+      <c r="AM17" s="2">
         <f t="shared" si="11"/>
-        <v>0.80599044337131298</v>
-      </c>
-      <c r="AL17" s="2">
-        <v>0.85499999999999998</v>
+        <v>0.58129318062265156</v>
       </c>
       <c r="AN17" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="AO17" s="2">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="AP17" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="AQ17" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AR17" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="AT17" s="2">
+        <v>0.80020000000000002</v>
+      </c>
+      <c r="AU17" s="2">
         <f t="shared" si="12"/>
-        <v>0.25120527870326731</v>
-      </c>
-      <c r="AP17" s="2">
+        <v>6.3681106710595001E-2</v>
+      </c>
+      <c r="AV17" s="2">
         <f t="shared" si="13"/>
-        <v>0.58129318062265156</v>
-      </c>
-      <c r="AQ17" s="2">
+        <v>0.2429281809430828</v>
+      </c>
+      <c r="AW17" s="2">
+        <v>0.9758</v>
+      </c>
+      <c r="AX17" s="2">
+        <v>0.25890000000000002</v>
+      </c>
+      <c r="AY17" s="2">
+        <v>0.84950000000000003</v>
+      </c>
+      <c r="AZ17" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="BC17" s="2">
+        <v>3.496</v>
+      </c>
+      <c r="BD17" s="2">
         <f t="shared" si="14"/>
-        <v>0.74879472129673275</v>
-      </c>
-      <c r="AR17" s="2">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="AT17" s="8">
-        <v>0.78</v>
-      </c>
-      <c r="AU17" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="AV17" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="AX17" s="2">
-        <v>0.80020000000000002</v>
-      </c>
-      <c r="AY17" s="2">
+        <v>0.3725944959271093</v>
+      </c>
+      <c r="BE17" s="2">
         <f t="shared" si="15"/>
-        <v>6.3681106710595001E-2</v>
-      </c>
-      <c r="AZ17" s="2">
+        <v>0.84847966932907226</v>
+      </c>
+      <c r="BF17" s="2">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="BG17" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="BH17" s="2">
+        <v>4.492</v>
+      </c>
+      <c r="BI17" s="2">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="BJ17" s="2">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="BL17" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="BM17" s="2">
         <f t="shared" si="16"/>
-        <v>0.2429281809430828</v>
-      </c>
-      <c r="BA17" s="2">
-        <v>0.25890000000000002</v>
-      </c>
-      <c r="BB17" s="2">
-        <v>0.84950000000000003</v>
-      </c>
-      <c r="BC17" s="2">
-        <v>0.9758</v>
-      </c>
-      <c r="BD17" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="BG17" s="2">
-        <v>3.496</v>
-      </c>
-      <c r="BH17" s="2">
+        <v>6.2264862914375774E-2</v>
+      </c>
+      <c r="BN17" s="2">
         <f t="shared" si="17"/>
-        <v>0.3725944959271093</v>
-      </c>
-      <c r="BI17" s="2">
-        <f t="shared" si="18"/>
-        <v>0.84847966932907226</v>
-      </c>
-      <c r="BJ17" s="2">
-        <v>0.93300000000000005</v>
-      </c>
-      <c r="BK17" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="BL17" s="2">
-        <v>4.492</v>
-      </c>
-      <c r="BM17" s="2">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="BN17" s="2">
-        <v>0.53500000000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.3795875394988239</v>
+      </c>
+      <c r="BO17" s="2">
+        <v>0.98680000000000001</v>
+      </c>
+      <c r="BP17" s="2">
+        <v>0.98709999999999998</v>
+      </c>
+      <c r="BQ17" s="2">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="BR17" s="2">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="BS17" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="BT17" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="V18" s="2">
         <v>5</v>
       </c>
       <c r="W18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.2631928995711312E-2</v>
       </c>
       <c r="X18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.22613496979991718</v>
       </c>
       <c r="Y18" s="2">
-        <f t="shared" si="5"/>
-        <v>0.91736807100428863</v>
-      </c>
-      <c r="Z18" s="2">
         <v>0.80800000000000005</v>
       </c>
+      <c r="AA18" s="2">
+        <v>5</v>
+      </c>
       <c r="AB18" s="2">
-        <v>5</v>
-      </c>
-      <c r="AC18" s="2">
         <f t="shared" si="6"/>
         <v>0.45705730488675578</v>
       </c>
-      <c r="AD18" s="2">
+      <c r="AC18" s="2">
         <f t="shared" si="7"/>
         <v>0.88722686942509832</v>
       </c>
-      <c r="AE18" s="2">
+      <c r="AD18" s="2">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="AF18" s="2">
+        <v>5</v>
+      </c>
+      <c r="AG18" s="2">
         <f t="shared" si="8"/>
-        <v>0.54294269511324422</v>
-      </c>
-      <c r="AF18" s="2">
-        <v>0.84699999999999998</v>
+        <v>0.21101735367330596</v>
       </c>
       <c r="AH18" s="2">
+        <f t="shared" si="9"/>
+        <v>0.44262995209633699</v>
+      </c>
+      <c r="AI18" s="2">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="AP18" s="2">
+        <v>0.748</v>
+      </c>
+      <c r="AQ18" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AR18" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="AT18" s="2">
+        <v>0.90010000000000001</v>
+      </c>
+      <c r="AU18" s="2">
+        <f t="shared" si="12"/>
+        <v>7.1066306676348431E-2</v>
+      </c>
+      <c r="AV18" s="2">
+        <f t="shared" si="13"/>
+        <v>0.26521286011932754</v>
+      </c>
+      <c r="AW18" s="2">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="AX18" s="2">
+        <v>0.24679999999999999</v>
+      </c>
+      <c r="AY18" s="2">
+        <v>0.8448</v>
+      </c>
+      <c r="AZ18" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="BC18" s="2">
+        <v>3.9950000000000001</v>
+      </c>
+      <c r="BD18" s="2">
+        <f t="shared" si="14"/>
+        <v>0.40427633678677316</v>
+      </c>
+      <c r="BE18" s="2">
+        <f t="shared" si="15"/>
+        <v>0.86484761840624835</v>
+      </c>
+      <c r="BF18" s="2">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="BG18" s="2">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="BH18" s="2">
         <v>5</v>
       </c>
-      <c r="AI18" s="2">
-        <f t="shared" si="9"/>
-        <v>0.21101735367330596</v>
-      </c>
-      <c r="AJ18" s="2">
-        <f t="shared" si="10"/>
-        <v>0.44262995209633699</v>
-      </c>
-      <c r="AK18" s="2">
-        <f t="shared" si="11"/>
-        <v>0.78898264632669401</v>
-      </c>
-      <c r="AL18" s="2">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="AT18" s="8">
-        <v>0.748</v>
-      </c>
-      <c r="AU18" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="AV18" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="AX18" s="2">
-        <v>0.90010000000000001</v>
-      </c>
-      <c r="AY18" s="2">
-        <f t="shared" si="15"/>
-        <v>7.1066306676348431E-2</v>
-      </c>
-      <c r="AZ18" s="2">
+      <c r="BI18" s="2">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="BJ18" s="2">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="BL18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="BM18" s="2">
         <f t="shared" si="16"/>
-        <v>0.26521286011932754</v>
-      </c>
-      <c r="BA18" s="2">
-        <v>0.24679999999999999</v>
-      </c>
-      <c r="BB18" s="2">
-        <v>0.8448</v>
-      </c>
-      <c r="BC18" s="2">
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="BD18" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="BG18" s="2">
-        <v>3.9950000000000001</v>
-      </c>
-      <c r="BH18" s="2">
+        <v>7.6638113239255054E-2</v>
+      </c>
+      <c r="BN18" s="2">
         <f t="shared" si="17"/>
-        <v>0.40427633678677316</v>
-      </c>
-      <c r="BI18" s="2">
-        <f t="shared" si="18"/>
-        <v>0.86484761840624835</v>
-      </c>
-      <c r="BJ18" s="2">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="BK18" s="2">
-        <v>0.51900000000000002</v>
-      </c>
-      <c r="BL18" s="2">
-        <v>5</v>
-      </c>
-      <c r="BM18" s="2">
-        <v>0.91200000000000003</v>
-      </c>
-      <c r="BN18" s="2">
-        <v>0.51100000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.43335991811487096</v>
+      </c>
+      <c r="BO18" s="2">
+        <v>0.98360000000000003</v>
+      </c>
+      <c r="BP18" s="2">
+        <v>0.9839</v>
+      </c>
+      <c r="BQ18" s="2">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="BR18" s="2">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="BS18" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT18" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2022</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>267</v>
+      </c>
       <c r="V19" s="2">
         <v>5.5</v>
       </c>
       <c r="W19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.0150193456815117E-2</v>
       </c>
       <c r="X19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.24324778375654069</v>
       </c>
       <c r="Y19" s="2">
-        <f t="shared" si="5"/>
-        <v>0.90984980654318492</v>
-      </c>
-      <c r="Z19" s="2">
         <v>0.78400000000000003</v>
       </c>
+      <c r="AA19" s="2">
+        <v>5.5</v>
+      </c>
       <c r="AB19" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="AC19" s="2">
         <f t="shared" si="6"/>
         <v>0.48078825688416366</v>
       </c>
-      <c r="AD19" s="2">
+      <c r="AC19" s="2">
         <f t="shared" si="7"/>
         <v>0.8964170289391088</v>
       </c>
-      <c r="AE19" s="2">
+      <c r="AD19" s="2">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="AF19" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="AG19" s="2">
         <f t="shared" si="8"/>
-        <v>0.51921174311583629</v>
-      </c>
-      <c r="AF19" s="2">
-        <v>0.83299999999999996</v>
+        <v>0.22732219621302879</v>
       </c>
       <c r="AH19" s="2">
-        <v>5.5</v>
+        <f t="shared" si="9"/>
+        <v>0.46625510004616011</v>
       </c>
       <c r="AI19" s="2">
-        <f t="shared" si="9"/>
-        <v>0.22732219621302879</v>
-      </c>
-      <c r="AJ19" s="2">
-        <f t="shared" si="10"/>
-        <v>0.46625510004616011</v>
-      </c>
-      <c r="AK19" s="2">
-        <f t="shared" si="11"/>
-        <v>0.77267780378697126</v>
-      </c>
-      <c r="AL19" s="2">
         <v>0.82399999999999995</v>
       </c>
-      <c r="AT19" s="8">
+      <c r="AP19" s="2">
         <v>0.71399999999999997</v>
       </c>
-      <c r="AV19" s="2" t="s">
+      <c r="AR19" s="2" t="s">
         <v>214</v>
       </c>
+      <c r="AT19" s="2">
+        <v>1.002</v>
+      </c>
+      <c r="AU19" s="2">
+        <f t="shared" si="12"/>
+        <v>7.8480293247622956E-2</v>
+      </c>
+      <c r="AV19" s="2">
+        <f t="shared" si="13"/>
+        <v>0.28663150195679926</v>
+      </c>
+      <c r="AW19" s="2">
+        <v>0.97009999999999996</v>
+      </c>
       <c r="AX19" s="2">
-        <v>1.002</v>
+        <v>0.2366</v>
       </c>
       <c r="AY19" s="2">
+        <v>0.84040000000000004</v>
+      </c>
+      <c r="AZ19" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="BC19" s="2">
+        <v>4.4969999999999999</v>
+      </c>
+      <c r="BD19" s="2">
+        <f t="shared" si="14"/>
+        <v>0.43307616969184493</v>
+      </c>
+      <c r="BE19" s="2">
         <f t="shared" si="15"/>
-        <v>7.8480293247622956E-2</v>
-      </c>
-      <c r="AZ19" s="2">
+        <v>0.87809549523948771</v>
+      </c>
+      <c r="BF19" s="2">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="BG19" s="2">
+        <v>0.501</v>
+      </c>
+      <c r="BH19" s="2">
+        <v>5.4989999999999997</v>
+      </c>
+      <c r="BI19" s="2">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="BJ19" s="2">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="BL19" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="BM19" s="2">
         <f t="shared" si="16"/>
-        <v>0.28663150195679926</v>
-      </c>
-      <c r="BA19" s="2">
-        <v>0.2366</v>
-      </c>
-      <c r="BB19" s="2">
-        <v>0.84040000000000004</v>
-      </c>
-      <c r="BC19" s="2">
-        <v>0.97009999999999996</v>
-      </c>
-      <c r="BD19" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="BG19" s="2">
-        <v>4.4969999999999999</v>
-      </c>
-      <c r="BH19" s="2">
+        <v>9.0577399684321228E-2</v>
+      </c>
+      <c r="BN19" s="2">
         <f t="shared" si="17"/>
-        <v>0.43307616969184493</v>
-      </c>
-      <c r="BI19" s="2">
-        <f t="shared" si="18"/>
-        <v>0.87809549523948771</v>
-      </c>
-      <c r="BJ19" s="2">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="BK19" s="2">
-        <v>0.501</v>
-      </c>
-      <c r="BL19" s="2">
-        <v>5.4989999999999997</v>
-      </c>
-      <c r="BM19" s="2">
-        <v>0.90700000000000003</v>
-      </c>
-      <c r="BN19" s="2">
-        <v>0.49199999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.47855462326732134</v>
+      </c>
+      <c r="BO19" s="2">
+        <v>0.98029999999999995</v>
+      </c>
+      <c r="BP19" s="2">
+        <v>0.98060000000000003</v>
+      </c>
+      <c r="BQ19" s="2">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="BR19" s="2">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="BS19" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="BT19" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="20" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="V20" s="2">
         <v>6</v>
       </c>
       <c r="W20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.7546228194460724E-2</v>
       </c>
       <c r="X20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.25962012589419375</v>
       </c>
       <c r="Y20" s="2">
-        <f t="shared" si="5"/>
-        <v>0.90245377180553932</v>
-      </c>
-      <c r="Z20" s="2">
         <v>0.76200000000000001</v>
       </c>
+      <c r="AA20" s="2">
+        <v>6</v>
+      </c>
       <c r="AB20" s="2">
-        <v>6</v>
-      </c>
-      <c r="AC20" s="2">
         <f t="shared" si="6"/>
         <v>0.50253161660310686</v>
       </c>
-      <c r="AD20" s="2">
+      <c r="AC20" s="2">
         <f t="shared" si="7"/>
         <v>0.90422219741472754</v>
       </c>
-      <c r="AE20" s="2">
-        <f t="shared" si="8"/>
-        <v>0.49746838339689314</v>
+      <c r="AD20" s="2">
+        <v>0.81699999999999995</v>
       </c>
       <c r="AF20" s="2">
+        <v>6</v>
+      </c>
+      <c r="AG20" s="2">
+        <f>$S$3*AF20/(1+$S$3*AF20)</f>
+        <v>0.24296678289649989</v>
+      </c>
+      <c r="AH20" s="2">
+        <f>AG20*$S$3/(AG20*$S$3+(1-AG20)*$P$3)</f>
+        <v>0.48795889780364277</v>
+      </c>
+      <c r="AI20" s="2">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="AP20" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="AR20" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="BC20" s="2">
+        <v>4.9859999999999998</v>
+      </c>
+      <c r="BD20" s="2">
+        <f t="shared" si="14"/>
+        <v>0.45857322284429874</v>
+      </c>
+      <c r="BE20" s="2">
+        <f t="shared" si="15"/>
+        <v>0.88872080714566659</v>
+      </c>
+      <c r="BF20" s="2">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="BG20" s="2">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="BH20" s="2">
+        <v>6</v>
+      </c>
+      <c r="BI20" s="2">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="BJ20" s="2">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="BL20" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="BM20" s="2">
+        <f t="shared" si="16"/>
+        <v>0.10410208362562001</v>
+      </c>
+      <c r="BN20" s="2">
+        <f t="shared" si="17"/>
+        <v>0.51707248879871404</v>
+      </c>
+      <c r="BO20" s="2">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="BP20" s="2">
+        <v>0.97729999999999995</v>
+      </c>
+      <c r="BQ20" s="2">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="BR20" s="2">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="BS20" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="BT20" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="21" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC21" s="2">
+        <v>4.9909999999999997</v>
+      </c>
+      <c r="BD21" s="2">
+        <f t="shared" si="14"/>
+        <v>0.45882208936917845</v>
+      </c>
+      <c r="BE21" s="2">
+        <f t="shared" si="15"/>
+        <v>0.88881989265984018</v>
+      </c>
+      <c r="BF21" s="2">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="BG21" s="2">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="BH21" s="2">
+        <v>6.4950000000000001</v>
+      </c>
+      <c r="BI21" s="2">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="BJ21" s="2">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="BL21" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="BM21" s="2">
+        <f t="shared" si="16"/>
+        <v>0.11723039156834966</v>
+      </c>
+      <c r="BN21" s="2">
+        <f t="shared" si="17"/>
+        <v>0.55029134234819244</v>
+      </c>
+      <c r="BO21" s="2">
+        <v>0.97370000000000001</v>
+      </c>
+      <c r="BP21" s="2">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="BQ21" s="2">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="BR21" s="2">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="BS21" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="BT21" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC22" s="2">
+        <v>5.4969999999999999</v>
+      </c>
+      <c r="BD22" s="2">
+        <f t="shared" si="14"/>
+        <v>0.48287686089541143</v>
+      </c>
+      <c r="BE22" s="2">
+        <f t="shared" si="15"/>
+        <v>0.89801026634902636</v>
+      </c>
+      <c r="BF22" s="2">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="BG22" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="BH22" s="2">
+        <v>7</v>
+      </c>
+      <c r="BI22" s="2">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="BJ22" s="2">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="BL22" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="BM22" s="2">
+        <f t="shared" si="16"/>
+        <v>0.12997949709682857</v>
+      </c>
+      <c r="BN22" s="2">
+        <f t="shared" si="17"/>
+        <v>0.57923430709363155</v>
+      </c>
+      <c r="BO22" s="2">
+        <v>0.97040000000000004</v>
+      </c>
+      <c r="BP22" s="2">
+        <v>0.97050000000000003</v>
+      </c>
+      <c r="BQ22" s="2">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="BR22" s="2">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="BS22" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="BT22" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="23" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC23" s="2">
+        <v>6.0090000000000003</v>
+      </c>
+      <c r="BD23" s="2">
+        <f t="shared" si="14"/>
+        <v>0.50513394581552229</v>
+      </c>
+      <c r="BE23" s="2">
+        <f t="shared" si="15"/>
+        <v>0.90588246542043027</v>
+      </c>
+      <c r="BF23" s="2">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="BG23" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="BH23" s="2">
+        <v>7.4980000000000002</v>
+      </c>
+      <c r="BI23" s="2">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="BJ23" s="2">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="BL23" s="2">
+        <v>1</v>
+      </c>
+      <c r="BM23" s="2">
+        <f t="shared" si="16"/>
+        <v>0.14236559582434957</v>
+      </c>
+      <c r="BN23" s="2">
+        <f t="shared" si="17"/>
+        <v>0.60467704257395172</v>
+      </c>
+      <c r="BO23" s="2">
+        <v>0.96709999999999996</v>
+      </c>
+      <c r="BP23" s="2">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="BQ23" s="2">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="BR23" s="2">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="BS23" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="BT23" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="24" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC24" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="BD24" s="2">
+        <f t="shared" si="14"/>
+        <v>0.52474984019713378</v>
+      </c>
+      <c r="BE24" s="2">
+        <f t="shared" si="15"/>
+        <v>0.91236894675964941</v>
+      </c>
+      <c r="BF24" s="2">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="BG24" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="BH24" s="2">
+        <v>8.1010000000000009</v>
+      </c>
+      <c r="BI24" s="2">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="BJ24" s="2">
+        <v>0.434</v>
+      </c>
+    </row>
+    <row r="25" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC25" s="2">
+        <v>6.9850000000000003</v>
+      </c>
+      <c r="BD25" s="2">
+        <f t="shared" si="14"/>
+        <v>0.54265684223437838</v>
+      </c>
+      <c r="BE25" s="2">
+        <f t="shared" si="15"/>
+        <v>0.91795434885155569</v>
+      </c>
+      <c r="BF25" s="2">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="BG25" s="2">
+        <v>0.436</v>
+      </c>
+      <c r="BH25" s="2">
+        <v>9.016</v>
+      </c>
+      <c r="BI25" s="2">
+        <v>0.872</v>
+      </c>
+      <c r="BJ25" s="2">
+        <v>0.42099999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC26" s="2">
+        <v>7.4950000000000001</v>
+      </c>
+      <c r="BD26" s="2">
+        <f t="shared" si="14"/>
+        <v>0.56008678871780104</v>
+      </c>
+      <c r="BE26" s="2">
+        <f t="shared" si="15"/>
+        <v>0.92310789978501107</v>
+      </c>
+      <c r="BF26" s="2">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="BG26" s="2">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="BH26" s="2">
+        <v>9.9990000000000006</v>
+      </c>
+      <c r="BI26" s="2">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="BJ26" s="2">
+        <v>0.41199999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC27" s="2">
+        <v>7.9480000000000004</v>
+      </c>
+      <c r="BD27" s="2">
+        <f t="shared" si="14"/>
+        <v>0.57449103724090178</v>
+      </c>
+      <c r="BE27" s="2">
+        <f t="shared" si="15"/>
+        <v>0.9271712290257752</v>
+      </c>
+      <c r="BF27" s="2">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="BG27" s="2">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="BH27" s="2">
+        <v>11.02</v>
+      </c>
+      <c r="BI27" s="2">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="BJ27" s="2">
+        <v>0.39700000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC28" s="2">
+        <v>7.9969999999999999</v>
+      </c>
+      <c r="BD28" s="2">
+        <f t="shared" si="14"/>
+        <v>0.57599277718960207</v>
+      </c>
+      <c r="BE28" s="2">
+        <f t="shared" si="15"/>
+        <v>0.92758515793215013</v>
+      </c>
+      <c r="BF28" s="2">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="BG28" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="BH28" s="2">
+        <v>11.992000000000001</v>
+      </c>
+      <c r="BI28" s="2">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="BJ28" s="2">
+        <v>0.38900000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC29" s="2">
+        <v>8.9870000000000001</v>
+      </c>
+      <c r="BD29" s="2">
+        <f t="shared" si="14"/>
+        <v>0.604214590590331</v>
+      </c>
+      <c r="BE29" s="2">
+        <f t="shared" si="15"/>
+        <v>0.93504415022326359</v>
+      </c>
+      <c r="BF29" s="2">
+        <v>0.879</v>
+      </c>
+      <c r="BG29" s="2">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="BH29" s="2">
+        <v>12.997999999999999</v>
+      </c>
+      <c r="BI29" s="2">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="BJ29" s="2">
+        <v>0.379</v>
+      </c>
+    </row>
+    <row r="30" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC30" s="2">
+        <v>9.9670000000000005</v>
+      </c>
+      <c r="BD30" s="2">
+        <f t="shared" si="14"/>
+        <v>0.62867991525094347</v>
+      </c>
+      <c r="BE30" s="2">
+        <f t="shared" si="15"/>
+        <v>0.94105442917687832</v>
+      </c>
+      <c r="BF30" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="BG30" s="2">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="BH30" s="2">
+        <v>13.972</v>
+      </c>
+      <c r="BI30" s="2">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="BJ30" s="2">
+        <v>0.377</v>
+      </c>
+    </row>
+    <row r="31" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC31" s="2">
+        <v>11.013</v>
+      </c>
+      <c r="BD31" s="2">
+        <f t="shared" si="14"/>
+        <v>0.65166240927882724</v>
+      </c>
+      <c r="BE31" s="2">
+        <f t="shared" si="15"/>
+        <v>0.94635265209091057</v>
+      </c>
+      <c r="BF31" s="2">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="BG31" s="2">
+        <v>0.374</v>
+      </c>
+      <c r="BH31" s="2">
+        <v>15.007999999999999</v>
+      </c>
+      <c r="BI31" s="2">
         <v>0.81699999999999995</v>
       </c>
-      <c r="AH20" s="2">
-        <v>6</v>
-      </c>
-      <c r="AI20" s="2">
-        <f>$S$3*AH20/(1+$S$3*AH20)</f>
-        <v>0.24296678289649989</v>
-      </c>
-      <c r="AJ20" s="2">
-        <f>AI20*$S$3/(AI20*$S$3+(1-AI20)*$P$3)</f>
-        <v>0.48795889780364277</v>
-      </c>
-      <c r="AK20" s="2">
-        <f>1-AI20</f>
-        <v>0.75703321710350013</v>
-      </c>
-      <c r="AL20" s="2">
-        <v>0.81200000000000006</v>
-      </c>
-      <c r="AT20" s="8">
-        <v>0.68</v>
-      </c>
-      <c r="AV20" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="BG20" s="2">
-        <v>4.9859999999999998</v>
-      </c>
-      <c r="BH20" s="2">
-        <f t="shared" si="17"/>
-        <v>0.45857322284429874</v>
-      </c>
-      <c r="BI20" s="2">
-        <f t="shared" si="18"/>
-        <v>0.88872080714566659</v>
-      </c>
-      <c r="BJ20" s="2">
-        <v>0.91600000000000004</v>
-      </c>
-      <c r="BK20" s="2">
-        <v>0.48799999999999999</v>
-      </c>
-      <c r="BL20" s="2">
-        <v>6</v>
-      </c>
-      <c r="BM20" s="2">
-        <v>0.90100000000000002</v>
-      </c>
-      <c r="BN20" s="2">
-        <v>0.48199999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BG21" s="2">
-        <v>4.9909999999999997</v>
-      </c>
-      <c r="BH21" s="2">
-        <f t="shared" si="17"/>
-        <v>0.45882208936917845</v>
-      </c>
-      <c r="BI21" s="2">
-        <f t="shared" si="18"/>
-        <v>0.88881989265984018</v>
-      </c>
-      <c r="BJ21" s="2">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="BK21" s="2">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="BL21" s="2">
-        <v>6.4950000000000001</v>
-      </c>
-      <c r="BM21" s="2">
-        <v>0.89600000000000002</v>
-      </c>
-      <c r="BN21" s="2">
-        <v>0.46899999999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BG22" s="2">
-        <v>5.4969999999999999</v>
-      </c>
-      <c r="BH22" s="2">
-        <f t="shared" si="17"/>
-        <v>0.48287686089541143</v>
-      </c>
-      <c r="BI22" s="2">
-        <f t="shared" si="18"/>
-        <v>0.89801026634902636</v>
-      </c>
-      <c r="BJ22" s="2">
-        <v>0.91100000000000003</v>
-      </c>
-      <c r="BK22" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="BL22" s="2">
-        <v>7</v>
-      </c>
-      <c r="BM22" s="2">
-        <v>0.89100000000000001</v>
-      </c>
-      <c r="BN22" s="2">
-        <v>0.45700000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BG23" s="2">
-        <v>6.0090000000000003</v>
-      </c>
-      <c r="BH23" s="2">
-        <f t="shared" si="17"/>
-        <v>0.50513394581552229</v>
-      </c>
-      <c r="BI23" s="2">
-        <f t="shared" si="18"/>
-        <v>0.90588246542043027</v>
-      </c>
-      <c r="BJ23" s="2">
-        <v>0.90700000000000003</v>
-      </c>
-      <c r="BK23" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="BL23" s="2">
-        <v>7.4980000000000002</v>
-      </c>
-      <c r="BM23" s="2">
-        <v>0.88600000000000001</v>
-      </c>
-      <c r="BN23" s="2">
-        <v>0.44800000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BG24" s="2">
-        <v>6.5</v>
-      </c>
-      <c r="BH24" s="2">
-        <f t="shared" si="17"/>
-        <v>0.52474984019713378</v>
-      </c>
-      <c r="BI24" s="2">
-        <f t="shared" si="18"/>
-        <v>0.91236894675964941</v>
-      </c>
-      <c r="BJ24" s="2">
-        <v>0.90200000000000002</v>
-      </c>
-      <c r="BK24" s="2">
-        <v>0.44</v>
-      </c>
-      <c r="BL24" s="2">
-        <v>8.1010000000000009</v>
-      </c>
-      <c r="BM24" s="2">
-        <v>0.88100000000000001</v>
-      </c>
-      <c r="BN24" s="2">
-        <v>0.434</v>
-      </c>
-    </row>
-    <row r="25" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BG25" s="2">
-        <v>6.9850000000000003</v>
-      </c>
-      <c r="BH25" s="2">
-        <f t="shared" si="17"/>
-        <v>0.54265684223437838</v>
-      </c>
-      <c r="BI25" s="2">
-        <f t="shared" si="18"/>
-        <v>0.91795434885155569</v>
-      </c>
-      <c r="BJ25" s="2">
-        <v>0.89600000000000002</v>
-      </c>
-      <c r="BK25" s="2">
-        <v>0.436</v>
-      </c>
-      <c r="BL25" s="2">
-        <v>9.016</v>
-      </c>
-      <c r="BM25" s="2">
-        <v>0.872</v>
-      </c>
-      <c r="BN25" s="2">
-        <v>0.42099999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BG26" s="2">
-        <v>7.4950000000000001</v>
-      </c>
-      <c r="BH26" s="2">
-        <f t="shared" si="17"/>
-        <v>0.56008678871780104</v>
-      </c>
-      <c r="BI26" s="2">
-        <f t="shared" si="18"/>
-        <v>0.92310789978501107</v>
-      </c>
-      <c r="BJ26" s="2">
-        <v>0.89200000000000002</v>
-      </c>
-      <c r="BK26" s="2">
-        <v>0.42299999999999999</v>
-      </c>
-      <c r="BL26" s="2">
-        <v>9.9990000000000006</v>
-      </c>
-      <c r="BM26" s="2">
-        <v>0.86199999999999999</v>
-      </c>
-      <c r="BN26" s="2">
-        <v>0.41199999999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BG27" s="2">
-        <v>7.9480000000000004</v>
-      </c>
-      <c r="BH27" s="2">
-        <f t="shared" si="17"/>
-        <v>0.57449103724090178</v>
-      </c>
-      <c r="BI27" s="2">
-        <f t="shared" si="18"/>
-        <v>0.9271712290257752</v>
-      </c>
-      <c r="BJ27" s="2">
-        <v>0.88800000000000001</v>
-      </c>
-      <c r="BK27" s="2">
-        <v>0.41399999999999998</v>
-      </c>
-      <c r="BL27" s="2">
-        <v>11.02</v>
-      </c>
-      <c r="BM27" s="2">
-        <v>0.85399999999999998</v>
-      </c>
-      <c r="BN27" s="2">
-        <v>0.39700000000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BG28" s="2">
-        <v>7.9969999999999999</v>
-      </c>
-      <c r="BH28" s="2">
-        <f t="shared" si="17"/>
-        <v>0.57599277718960207</v>
-      </c>
-      <c r="BI28" s="2">
-        <f t="shared" si="18"/>
-        <v>0.92758515793215013</v>
-      </c>
-      <c r="BJ28" s="2">
-        <v>0.88600000000000001</v>
-      </c>
-      <c r="BK28" s="2">
-        <v>0.42</v>
-      </c>
-      <c r="BL28" s="2">
-        <v>11.992000000000001</v>
-      </c>
-      <c r="BM28" s="2">
-        <v>0.84499999999999997</v>
-      </c>
-      <c r="BN28" s="2">
-        <v>0.38900000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BG29" s="2">
-        <v>8.9870000000000001</v>
-      </c>
-      <c r="BH29" s="2">
-        <f t="shared" si="17"/>
-        <v>0.604214590590331</v>
-      </c>
-      <c r="BI29" s="2">
-        <f t="shared" si="18"/>
-        <v>0.93504415022326359</v>
-      </c>
-      <c r="BJ29" s="2">
-        <v>0.879</v>
-      </c>
-      <c r="BK29" s="2">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="BL29" s="2">
-        <v>12.997999999999999</v>
-      </c>
-      <c r="BM29" s="2">
-        <v>0.83699999999999997</v>
-      </c>
-      <c r="BN29" s="2">
-        <v>0.379</v>
-      </c>
-    </row>
-    <row r="30" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BG30" s="2">
-        <v>9.9670000000000005</v>
-      </c>
-      <c r="BH30" s="2">
-        <f t="shared" si="17"/>
-        <v>0.62867991525094347</v>
-      </c>
-      <c r="BI30" s="2">
-        <f t="shared" si="18"/>
-        <v>0.94105442917687832</v>
-      </c>
-      <c r="BJ30" s="2">
-        <v>0.87</v>
-      </c>
-      <c r="BK30" s="2">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="BL30" s="2">
-        <v>13.972</v>
-      </c>
-      <c r="BM30" s="2">
-        <v>0.82699999999999996</v>
-      </c>
-      <c r="BN30" s="2">
-        <v>0.377</v>
-      </c>
-    </row>
-    <row r="31" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="BG31" s="2">
-        <v>11.013</v>
-      </c>
-      <c r="BH31" s="2">
-        <f t="shared" si="17"/>
-        <v>0.65166240927882724</v>
-      </c>
-      <c r="BI31" s="2">
-        <f t="shared" si="18"/>
-        <v>0.94635265209091057</v>
-      </c>
       <c r="BJ31" s="2">
-        <v>0.86199999999999999</v>
-      </c>
-      <c r="BK31" s="2">
-        <v>0.374</v>
-      </c>
-      <c r="BL31" s="2">
-        <v>15.007999999999999</v>
-      </c>
-      <c r="BM31" s="2">
-        <v>0.81699999999999995</v>
-      </c>
-      <c r="BN31" s="2">
         <v>0.373</v>
       </c>
     </row>
-    <row r="32" spans="1:66" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:72" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC32" s="2">
+        <v>11.999000000000001</v>
+      </c>
+      <c r="BD32" s="2">
+        <f t="shared" si="14"/>
+        <v>0.67086534204909554</v>
+      </c>
+      <c r="BE32" s="2">
+        <f t="shared" si="15"/>
+        <v>0.95054301748754755</v>
+      </c>
+      <c r="BF32" s="2">
+        <v>0.85499999999999998</v>
+      </c>
       <c r="BG32" s="2">
-        <v>11.999000000000001</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="BH32" s="2">
-        <f t="shared" si="17"/>
-        <v>0.67086534204909554</v>
+        <v>15.779</v>
       </c>
       <c r="BI32" s="2">
-        <f t="shared" si="18"/>
-        <v>0.95054301748754755</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="BJ32" s="2">
-        <v>0.85499999999999998</v>
-      </c>
-      <c r="BK32" s="2">
-        <v>0.36199999999999999</v>
-      </c>
-      <c r="BL32" s="2">
-        <v>15.779</v>
-      </c>
-      <c r="BM32" s="2">
-        <v>0.81100000000000005</v>
-      </c>
-      <c r="BN32" s="2">
         <v>0.36799999999999999</v>
       </c>
     </row>
@@ -5063,9 +5525,10 @@
     <hyperlink ref="A15" r:id="rId9" xr:uid="{5BC2FFA3-BDD4-4796-90FC-33F2E8AC5983}"/>
     <hyperlink ref="A16" r:id="rId10" xr:uid="{BD0A540B-8EC4-4001-BE15-3CBF3CEF38EB}"/>
     <hyperlink ref="A17" r:id="rId11" location="fig0003" xr:uid="{A08C39A0-20C1-4E98-A85A-A81E8F1031B0}"/>
+    <hyperlink ref="A19" r:id="rId12" xr:uid="{42B52C3E-043A-4627-B085-78F4B980BB88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
-  <drawing r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update plot limits, change to light theme
</commit_message>
<xml_diff>
--- a/sources_list_.xlsx
+++ b/sources_list_.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/peterbaz_stanford_edu/Documents/DiazMarin2026/hygroscopic-salts-main/hygroscopic-salts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1126" documentId="8_{0B5C881D-AA95-4664-BDBF-B508CE6D9B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90B12ACF-FDB2-4ADC-9A5A-42D33CDA1477}"/>
+  <xr:revisionPtr revIDLastSave="1133" documentId="8_{0B5C881D-AA95-4664-BDBF-B508CE6D9B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97C1250C-BD07-4EFE-A769-241DD7D9AFD3}"/>
   <bookViews>
     <workbookView xWindow="10812" yWindow="270" windowWidth="12114" windowHeight="12438" activeTab="3" xr2:uid="{A5D934FD-846B-4DBC-ADED-26484461699C}"/>
   </bookViews>
@@ -1472,6 +1472,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2539,8 +2543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADEB32D0-53C4-465C-8106-B93762800774}">
   <dimension ref="A1:BT32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView tabSelected="1" topLeftCell="AF2" zoomScale="75" workbookViewId="0">
+      <selection activeCell="AO7" sqref="AO7:AO17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.578125" defaultRowHeight="49" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3147,6 +3151,7 @@
       <c r="Y8" s="2">
         <v>0.99</v>
       </c>
+      <c r="Z8"/>
       <c r="AA8" s="2">
         <v>0.3</v>
       </c>
@@ -3322,6 +3327,7 @@
       <c r="Y9" s="2">
         <v>0.98350000000000004</v>
       </c>
+      <c r="Z9"/>
       <c r="AA9" s="2">
         <v>0.5</v>
       </c>
@@ -3488,6 +3494,7 @@
       <c r="Y10" s="2">
         <v>0.96699999999999997</v>
       </c>
+      <c r="Z10"/>
       <c r="AA10" s="2">
         <v>1</v>
       </c>
@@ -3666,6 +3673,7 @@
       <c r="Y11" s="2">
         <v>0.95</v>
       </c>
+      <c r="Z11"/>
       <c r="AA11" s="2">
         <v>1.5</v>
       </c>
@@ -3844,6 +3852,7 @@
       <c r="Y12" s="2">
         <v>0.93200000000000005</v>
       </c>
+      <c r="Z12"/>
       <c r="AA12" s="2">
         <v>2</v>
       </c>
@@ -4017,6 +4026,7 @@
       <c r="Y13" s="2">
         <v>0.91300000000000003</v>
       </c>
+      <c r="Z13"/>
       <c r="AA13" s="2">
         <v>2.5</v>
       </c>
@@ -4177,6 +4187,7 @@
       <c r="Y14" s="2">
         <v>0.89400000000000002</v>
       </c>
+      <c r="Z14"/>
       <c r="AA14" s="2">
         <v>3</v>
       </c>
@@ -4334,6 +4345,7 @@
       <c r="Y15" s="2">
         <v>0.872</v>
       </c>
+      <c r="Z15"/>
       <c r="AA15" s="2">
         <v>3.5</v>
       </c>
@@ -4488,6 +4500,7 @@
       <c r="Y16" s="2">
         <v>0.85199999999999998</v>
       </c>
+      <c r="Z16"/>
       <c r="AA16" s="2">
         <v>4</v>
       </c>
@@ -4645,6 +4658,7 @@
       <c r="Y17" s="2">
         <v>0.83</v>
       </c>
+      <c r="Z17"/>
       <c r="AA17" s="2">
         <v>4.5</v>
       </c>
@@ -4790,6 +4804,7 @@
       <c r="Y18" s="2">
         <v>0.80800000000000005</v>
       </c>
+      <c r="Z18"/>
       <c r="AA18" s="2">
         <v>5</v>
       </c>
@@ -4936,6 +4951,7 @@
       <c r="Y19" s="2">
         <v>0.78400000000000003</v>
       </c>
+      <c r="Z19"/>
       <c r="AA19" s="2">
         <v>5.5</v>
       </c>
@@ -5064,6 +5080,7 @@
       <c r="Y20" s="2">
         <v>0.76200000000000001</v>
       </c>
+      <c r="Z20"/>
       <c r="AA20" s="2">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
add sulfate data and clean up
</commit_message>
<xml_diff>
--- a/sources_list_.xlsx
+++ b/sources_list_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/peterbaz_stanford_edu/Documents/DiazMarin2026/hygroscopic-salts-main/hygroscopic-salts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1133" documentId="8_{0B5C881D-AA95-4664-BDBF-B508CE6D9B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97C1250C-BD07-4EFE-A769-241DD7D9AFD3}"/>
+  <xr:revisionPtr revIDLastSave="1381" documentId="8_{0B5C881D-AA95-4664-BDBF-B508CE6D9B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CB311D1-48AF-462C-A279-FB11CE6CD636}"/>
   <bookViews>
-    <workbookView xWindow="10812" yWindow="270" windowWidth="12114" windowHeight="12438" activeTab="3" xr2:uid="{A5D934FD-846B-4DBC-ADED-26484461699C}"/>
+    <workbookView xWindow="22620" yWindow="165" windowWidth="15690" windowHeight="20895" activeTab="3" xr2:uid="{A5D934FD-846B-4DBC-ADED-26484461699C}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sources" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="345">
   <si>
     <t xml:space="preserve">Data Source </t>
   </si>
@@ -959,9 +959,6 @@
     <t>Deliquescence Limits</t>
   </si>
   <si>
-    <t>68?</t>
-  </si>
-  <si>
     <t>83-86</t>
   </si>
   <si>
@@ -978,6 +975,105 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Na2SO4</t>
+  </si>
+  <si>
+    <t>K2SO4</t>
+  </si>
+  <si>
+    <t>68??</t>
+  </si>
+  <si>
+    <t>Water activity, osmotic and activity coefficients of aqueous solutions of Li2SO4, Na2SO4, K2SO4, (NH4)2SO4, MgSO4, MnSO4, NiSO4, CuSO4, and ZnSO4 at T=298.15 K</t>
+  </si>
+  <si>
+    <t>Sulfates</t>
+  </si>
+  <si>
+    <t>Paper 14 (Na2SO4</t>
+  </si>
+  <si>
+    <t>Uses 'a hygrometric method'</t>
+  </si>
+  <si>
+    <t>Na2SO4 mole fraction</t>
+  </si>
+  <si>
+    <t>Na2SO4 mass fraction</t>
+  </si>
+  <si>
+    <t>Paper 14 (K2SO4)</t>
+  </si>
+  <si>
+    <t>K2SO4 mole fraction</t>
+  </si>
+  <si>
+    <t>K2SO4 mass fraction</t>
+  </si>
+  <si>
+    <t>(NH4)2SO4</t>
+  </si>
+  <si>
+    <t>MgSO4</t>
+  </si>
+  <si>
+    <t>MnSO4</t>
+  </si>
+  <si>
+    <t>78–82</t>
+  </si>
+  <si>
+    <t>82–87</t>
+  </si>
+  <si>
+    <t>95–99</t>
+  </si>
+  <si>
+    <t>Li2SO4</t>
+  </si>
+  <si>
+    <t>ZnSO4</t>
+  </si>
+  <si>
+    <t>CuSO4</t>
+  </si>
+  <si>
+    <t>NiSO4</t>
+  </si>
+  <si>
+    <t>82–85</t>
+  </si>
+  <si>
+    <t>(only hydrtate data) MgSO4∙7H2O    87–89</t>
+  </si>
+  <si>
+    <t>Paper 14 ((NH4)2SO4)</t>
+  </si>
+  <si>
+    <t>Paper 14 (MgSO4)</t>
+  </si>
+  <si>
+    <t>Paper 14 (MnSO4)</t>
+  </si>
+  <si>
+    <t>Paper 14 (Li2SO4)</t>
+  </si>
+  <si>
+    <t>Paper 14 (NiSO4)</t>
+  </si>
+  <si>
+    <t>Paper 14 (CuSO4)</t>
+  </si>
+  <si>
+    <t>Paper 14 (ZnSO4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mole fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mass fraction</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1063,6 +1159,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1799,14 +1898,14 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.578125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="25.578125" style="2"/>
-    <col min="5" max="8" width="13.15625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="25.578125" style="2"/>
+    <col min="1" max="4" width="25.5703125" style="2"/>
+    <col min="5" max="8" width="13.140625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="25.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1838,7 +1937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1870,7 +1969,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1899,7 +1998,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
@@ -1919,7 +2018,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
@@ -1942,7 +2041,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>37</v>
       </c>
@@ -1956,7 +2055,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
@@ -1967,7 +2066,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>44</v>
       </c>
@@ -1984,7 +2083,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>99</v>
       </c>
@@ -2010,7 +2109,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>48</v>
       </c>
@@ -2039,7 +2138,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>50</v>
       </c>
@@ -2062,10 +2161,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -2079,7 +2178,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2100,7 +2199,7 @@
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2109,7 +2208,7 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -2117,12 +2216,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>5</v>
       </c>
@@ -2145,7 +2244,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>119</v>
       </c>
@@ -2174,10 +2273,10 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
     </row>
@@ -2211,17 +2310,17 @@
       <selection activeCell="D16" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.578125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="25.578125" style="2"/>
-    <col min="4" max="4" width="10.578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.578125" style="2"/>
-    <col min="6" max="6" width="10.578125" style="2" customWidth="1"/>
-    <col min="7" max="9" width="13.15625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="25.578125" style="2"/>
+    <col min="1" max="3" width="25.5703125" style="2"/>
+    <col min="4" max="4" width="10.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="2"/>
+    <col min="6" max="6" width="10.5703125" style="2" customWidth="1"/>
+    <col min="7" max="9" width="13.140625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="25.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -2244,7 +2343,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>56</v>
       </c>
@@ -2261,7 +2360,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>58</v>
       </c>
@@ -2278,7 +2377,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>65</v>
       </c>
@@ -2298,7 +2397,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>66</v>
       </c>
@@ -2315,7 +2414,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" ht="360" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>83</v>
       </c>
@@ -2335,7 +2434,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>88</v>
       </c>
@@ -2352,10 +2451,10 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>73</v>
       </c>
@@ -2372,7 +2471,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>133</v>
       </c>
@@ -2395,7 +2494,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>61</v>
       </c>
@@ -2424,7 +2523,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>128</v>
       </c>
@@ -2477,15 +2576,15 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.578125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.578125" style="2"/>
-    <col min="3" max="3" width="13.15625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="25.578125" style="2"/>
+    <col min="1" max="1" width="25.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="2"/>
+    <col min="3" max="3" width="13.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="25.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -2496,7 +2595,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
@@ -2507,7 +2606,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>79</v>
       </c>
@@ -2518,7 +2617,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>81</v>
       </c>
@@ -2541,31 +2640,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADEB32D0-53C4-465C-8106-B93762800774}">
-  <dimension ref="A1:BT32"/>
+  <dimension ref="A1:DM32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF2" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AO7" sqref="AO7:AO17"/>
+    <sheetView tabSelected="1" topLeftCell="CA1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="DO8" sqref="DO8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.578125" defaultRowHeight="49" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.578125" style="2"/>
-    <col min="2" max="3" width="7.578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.578125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="20.578125" style="2"/>
-    <col min="7" max="7" width="7.578125" style="2" customWidth="1"/>
-    <col min="8" max="13" width="8.578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.578125" style="6" customWidth="1"/>
-    <col min="15" max="73" width="8.578125" style="2" customWidth="1"/>
-    <col min="74" max="16384" width="20.578125" style="2"/>
+    <col min="1" max="1" width="20.5703125" style="2"/>
+    <col min="2" max="3" width="7.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="20.5703125" style="2"/>
+    <col min="7" max="7" width="7.5703125" style="2" customWidth="1"/>
+    <col min="8" max="13" width="8.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="6" customWidth="1"/>
+    <col min="15" max="126" width="8.5703125" style="2" customWidth="1"/>
+    <col min="127" max="16384" width="20.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:117" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>227</v>
       </c>
       <c r="N1" s="5"/>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>162</v>
       </c>
       <c r="P1" s="2" t="s">
@@ -2592,33 +2691,86 @@
       <c r="W1" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="4" t="s">
+      <c r="X1" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="AI1" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>264</v>
       </c>
+      <c r="AQ1" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="AR1" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="AS1" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="AT1" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="AU1" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="AV1" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>331</v>
+      </c>
     </row>
-    <row r="2" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -2670,29 +2822,83 @@
       <c r="W2" s="2">
         <v>165.99799999999999</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="X2" s="2">
+        <v>142.04499999999999</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>174.25899999999999</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>132.1395</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>120.3676</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>151.00059999999999</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>109.94459999999999</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>154.756</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>159.6086</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>161.4426</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="AN2" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="AP2" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="AU2" s="2" t="s">
         <v>311</v>
       </c>
+      <c r="AV2" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>311</v>
+      </c>
     </row>
-    <row r="3" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>139</v>
       </c>
@@ -2749,8 +2955,62 @@
         <f>W2/1000</f>
         <v>0.16599799999999998</v>
       </c>
+      <c r="X3" s="2">
+        <f t="shared" ref="X3:Y3" si="1">X2/1000</f>
+        <v>0.14204499999999998</v>
+      </c>
+      <c r="Y3" s="2">
+        <f t="shared" si="1"/>
+        <v>0.174259</v>
+      </c>
+      <c r="Z3" s="2">
+        <f t="shared" ref="Z3" si="2">Z2/1000</f>
+        <v>0.13213949999999999</v>
+      </c>
+      <c r="AA3" s="2">
+        <f t="shared" ref="AA3" si="3">AA2/1000</f>
+        <v>0.12036759999999999</v>
+      </c>
+      <c r="AB3" s="2">
+        <f t="shared" ref="AB3" si="4">AB2/1000</f>
+        <v>0.15100059999999998</v>
+      </c>
+      <c r="AC3" s="2">
+        <f t="shared" ref="AC3" si="5">AC2/1000</f>
+        <v>0.10994459999999999</v>
+      </c>
+      <c r="AD3" s="2">
+        <f t="shared" ref="AD3" si="6">AD2/1000</f>
+        <v>0.154756</v>
+      </c>
+      <c r="AE3" s="2">
+        <f t="shared" ref="AE3" si="7">AE2/1000</f>
+        <v>0.15960859999999999</v>
+      </c>
+      <c r="AF3" s="2">
+        <f t="shared" ref="AF3" si="8">AF2/1000</f>
+        <v>0.16144259999999999</v>
+      </c>
+      <c r="CJ3" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="CK3" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="CM3" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="CN3" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="CO3" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="CP3" s="2" t="s">
+        <v>331</v>
+      </c>
     </row>
-    <row r="4" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>144</v>
       </c>
@@ -2799,8 +3059,35 @@
       <c r="BL4" s="1" t="s">
         <v>268</v>
       </c>
+      <c r="BV4" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="CA4" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="CF4" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="CK4" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="CP4" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="CU4" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="CZ4" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="DE4" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="DJ4" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
-    <row r="5" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S5" s="2" t="s">
         <v>156</v>
       </c>
@@ -2820,7 +3107,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>166</v>
       </c>
@@ -2939,7 +3226,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O7" s="2">
         <v>0.1</v>
       </c>
@@ -3099,8 +3386,116 @@
       <c r="BT7" s="2" t="s">
         <v>301</v>
       </c>
+      <c r="BV7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="BW7" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="BX7" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="BY7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CA7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="CB7" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="CC7" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="CD7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CF7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="CG7" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="CH7" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="CI7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CK7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="CL7" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="CM7" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="CN7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CP7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="CQ7" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="CR7" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="CS7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CU7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="CV7" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="CW7" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="CX7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CZ7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="DA7" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="DB7" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DC7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="DE7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="DF7" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="DG7" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DH7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="DJ7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="DK7" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="DL7" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DM7" s="2" t="s">
+        <v>259</v>
+      </c>
     </row>
-    <row r="8" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>148</v>
       </c>
@@ -3120,15 +3515,15 @@
         <v>1</v>
       </c>
       <c r="P8" s="2">
-        <f t="shared" ref="P8:P13" si="1">$P$3*O8/(1+$P$3*O8)</f>
+        <f t="shared" ref="P8:P13" si="9">$P$3*O8/(1+$P$3*O8)</f>
         <v>1.7696202904672331E-2</v>
       </c>
       <c r="Q8" s="2">
-        <f t="shared" ref="Q8:Q13" si="2">P8*$Q$3/(P8*$Q$3+(1-P8)*$P$3)</f>
+        <f t="shared" ref="Q8:Q13" si="10">P8*$Q$3/(P8*$Q$3+(1-P8)*$P$3)</f>
         <v>5.5216010687396497E-2</v>
       </c>
       <c r="R8" s="2">
-        <f t="shared" ref="R8:R13" si="3">1-P8</f>
+        <f t="shared" ref="R8:R13" si="11">1-P8</f>
         <v>0.98230379709532767</v>
       </c>
       <c r="S8" s="2">
@@ -3141,11 +3536,11 @@
         <v>0.3</v>
       </c>
       <c r="W8" s="2">
-        <f t="shared" ref="W8:W20" si="4">$P$3*V8/(1+$P$3*V8)</f>
+        <f t="shared" ref="W8:W20" si="12">$P$3*V8/(1+$P$3*V8)</f>
         <v>5.3754483891806726E-3</v>
       </c>
       <c r="X8" s="2">
-        <f t="shared" ref="X8:X20" si="5">W8*$Q$3/(W8*$Q$3+(1-W8)*$P$3)</f>
+        <f t="shared" ref="X8:X20" si="13">W8*$Q$3/(W8*$Q$3+(1-W8)*$P$3)</f>
         <v>1.7230794208226582E-2</v>
       </c>
       <c r="Y8" s="2">
@@ -3156,11 +3551,11 @@
         <v>0.3</v>
       </c>
       <c r="AB8" s="2">
-        <f t="shared" ref="AB8:AB20" si="6">$T$3*AA8/(1+$T$3*AA8)</f>
+        <f t="shared" ref="AB8:AB20" si="14">$T$3*AA8/(1+$T$3*AA8)</f>
         <v>4.8080411313031236E-2</v>
       </c>
       <c r="AC8" s="2">
-        <f t="shared" ref="AC8:AC20" si="7">AB8*$T$3/(AB8*$T$3+(1-AB8)*$P$3)</f>
+        <f t="shared" ref="AC8:AC20" si="15">AB8*$T$3/(AB8*$T$3+(1-AB8)*$P$3)</f>
         <v>0.32067138531083489</v>
       </c>
       <c r="AD8" s="2">
@@ -3170,11 +3565,11 @@
         <v>0.3</v>
       </c>
       <c r="AG8" s="2">
-        <f t="shared" ref="AG8:AG19" si="8">$S$3*AF8/(1+$S$3*AF8)</f>
+        <f t="shared" ref="AG8:AG19" si="16">$S$3*AF8/(1+$S$3*AF8)</f>
         <v>1.5793851329559162E-2</v>
       </c>
       <c r="AH8" s="2">
-        <f t="shared" ref="AH8:AH19" si="9">AG8*$S$3/(AG8*$S$3+(1-AG8)*$P$3)</f>
+        <f t="shared" ref="AH8:AH19" si="17">AG8*$S$3/(AG8*$S$3+(1-AG8)*$P$3)</f>
         <v>4.5481299362322918E-2</v>
       </c>
       <c r="AI8" s="2">
@@ -3184,11 +3579,11 @@
         <v>0.3</v>
       </c>
       <c r="AL8" s="2">
-        <f t="shared" ref="AL8:AL17" si="10">$R$3*AK8/(1+$R$3*AK8)</f>
+        <f t="shared" ref="AL8:AL17" si="18">$R$3*AK8/(1+$R$3*AK8)</f>
         <v>2.1876035894410738E-2</v>
       </c>
       <c r="AM8" s="2">
-        <f t="shared" ref="AM8:AM17" si="11">AL8*$R$3/(AL8*$R$3+(1-AL8)*$P$3)</f>
+        <f t="shared" ref="AM8:AM17" si="19">AL8*$R$3/(AL8*$R$3+(1-AL8)*$P$3)</f>
         <v>8.4713208333669743E-2</v>
       </c>
       <c r="AN8" s="2">
@@ -3281,8 +3676,134 @@
       <c r="BT8" s="2">
         <v>0</v>
       </c>
+      <c r="BV8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BW8" s="2">
+        <f>$X$3*BV8/(1+$X$3*BV8)</f>
+        <v>1.4005558050669267E-2</v>
+      </c>
+      <c r="BX8" s="2">
+        <f>BW8*$X$3/(BW8*$X$3+(1-BW8)*$P$3)</f>
+        <v>0.10071934376943174</v>
+      </c>
+      <c r="BY8" s="2">
+        <v>0.99570000000000003</v>
+      </c>
+      <c r="CA8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="CB8" s="2">
+        <f>$Y$3*CA8/(1+$Y$3*CA8)</f>
+        <v>1.7127438961402494E-2</v>
+      </c>
+      <c r="CC8" s="2">
+        <f>CB8*$Y$3/(CB8*$Y$3+(1-CB8)*$P$3)</f>
+        <v>0.14424637730285089</v>
+      </c>
+      <c r="CD8" s="2">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="CF8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="CG8" s="2">
+        <f>$Z$3*CF8/(1+$Z$3*CF8)</f>
+        <v>1.3041618702545501E-2</v>
+      </c>
+      <c r="CH8" s="2">
+        <f>CG8*$Z$3/(CG8*$Z$3+(1-CG8)*$P$3)</f>
+        <v>8.8359762050827212E-2</v>
+      </c>
+      <c r="CI8" s="2">
+        <v>0.99590000000000001</v>
+      </c>
+      <c r="CK8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="CL8" s="2">
+        <f>$AA$3*CK8/(1+$AA$3*CK8)</f>
+        <v>2.3507609102127746E-2</v>
+      </c>
+      <c r="CM8" s="2">
+        <f>CL8*$AA$3/(CL8*$AA$3+(1-CL8)*$P$3)</f>
+        <v>0.13856057466344765</v>
+      </c>
+      <c r="CN8" s="2">
+        <v>0.996</v>
+      </c>
+      <c r="CP8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="CQ8" s="2">
+        <f>$AB$3*CP8/(1+$AB$3*CP8)</f>
+        <v>2.9314809243081819E-2</v>
+      </c>
+      <c r="CR8" s="2">
+        <f>CQ8*$AB$3/(CQ8*$AB$3+(1-CQ8)*$P$3)</f>
+        <v>0.20200170627571937</v>
+      </c>
+      <c r="CS8" s="2">
+        <v>0.99609999999999999</v>
+      </c>
+      <c r="CU8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="CV8" s="2">
+        <f>$AC$3*CU8/(1+$AC$3*CU8)</f>
+        <v>1.0874896386672583E-2</v>
+      </c>
+      <c r="CW8" s="2">
+        <f>CV8*$AC$3/(CV8*$AC$3+(1-CV8)*$P$3)</f>
+        <v>6.2879486352938704E-2</v>
+      </c>
+      <c r="CX8" s="2">
+        <v>0.99560000000000004</v>
+      </c>
+      <c r="CZ8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="DA8" s="2">
+        <f>$AD$3*CZ8/(1+$AD$3*CZ8)</f>
+        <v>3.0021983581764101E-2</v>
+      </c>
+      <c r="DB8" s="2">
+        <f>DA8*$AD$3/(DA8*$AD$3+(1-DA8)*$P$3)</f>
+        <v>0.21003763609108875</v>
+      </c>
+      <c r="DC8" s="2">
+        <v>0.99619999999999997</v>
+      </c>
+      <c r="DE8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="DF8" s="2">
+        <f>$AE$3*DE8/(1+$AE$3*DE8)</f>
+        <v>3.0934245671270493E-2</v>
+      </c>
+      <c r="DG8" s="2">
+        <f>DF8*$AE$3/(DF8*$AE$3+(1-DF8)*$P$3)</f>
+        <v>0.22046669057147453</v>
+      </c>
+      <c r="DH8" s="2">
+        <v>0.99629999999999996</v>
+      </c>
+      <c r="DJ8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="DK8" s="2">
+        <f>$AF$3*DJ8/(1+$AF$3*DJ8)</f>
+        <v>3.1278580914568345E-2</v>
+      </c>
+      <c r="DL8" s="2">
+        <f>DK8*$AF$3/(DK8*$AF$3+(1-DK8)*$P$3)</f>
+        <v>0.22441882125466706</v>
+      </c>
+      <c r="DM8" s="2">
+        <v>0.99619999999999997</v>
+      </c>
     </row>
-    <row r="9" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>151</v>
       </c>
@@ -3296,15 +3817,15 @@
         <v>2</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3.4776985222435643E-2</v>
       </c>
       <c r="Q9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>0.10465347403405539</v>
       </c>
       <c r="R9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>0.96522301477756434</v>
       </c>
       <c r="S9" s="2">
@@ -3317,11 +3838,11 @@
         <v>0.5</v>
       </c>
       <c r="W9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>8.9270892436379302E-3</v>
       </c>
       <c r="X9" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>2.839184762463667E-2</v>
       </c>
       <c r="Y9" s="2">
@@ -3332,11 +3853,11 @@
         <v>0.5</v>
       </c>
       <c r="AB9" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>7.7645209773455834E-2</v>
       </c>
       <c r="AC9" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.44032024106328244</v>
       </c>
       <c r="AD9" s="2">
@@ -3346,11 +3867,11 @@
         <v>0.5</v>
       </c>
       <c r="AG9" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>2.6048811511713465E-2</v>
       </c>
       <c r="AH9" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>7.3571416524238833E-2</v>
       </c>
       <c r="AI9" s="2">
@@ -3360,11 +3881,11 @@
         <v>0.5</v>
       </c>
       <c r="AL9" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>3.5935968795175438E-2</v>
       </c>
       <c r="AM9" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0.13364122903781739</v>
       </c>
       <c r="AN9" s="2">
@@ -3383,11 +3904,11 @@
         <v>5.0099999999999999E-2</v>
       </c>
       <c r="AU9" s="2">
-        <f t="shared" ref="AU9:AU19" si="12">$U$3*AT9/(1+$U$3*AT9)</f>
+        <f t="shared" ref="AU9:AU19" si="20">$U$3*AT9/(1+$U$3*AT9)</f>
         <v>4.2401440212727036E-3</v>
       </c>
       <c r="AV9" s="2">
-        <f t="shared" ref="AV9:AV19" si="13">AU9*$U$3/(AU9*$U$3+(1-AU9)*$P$3)</f>
+        <f t="shared" ref="AV9:AV19" si="21">AU9*$U$3/(AU9*$U$3+(1-AU9)*$P$3)</f>
         <v>1.9694343352171489E-2</v>
       </c>
       <c r="AW9" s="2">
@@ -3406,11 +3927,11 @@
         <v>0.999</v>
       </c>
       <c r="BD9" s="2">
-        <f t="shared" ref="BD9:BD32" si="14">$V$3*BC9/(1+$V$3*BC9)</f>
+        <f t="shared" ref="BD9:BD32" si="22">$V$3*BC9/(1+$V$3*BC9)</f>
         <v>0.14508003004154577</v>
       </c>
       <c r="BE9" s="2">
-        <f t="shared" ref="BE9:BE32" si="15">BD9*$V$3/(BD9*$V$3+(1-BD9)*$P$3)</f>
+        <f t="shared" ref="BE9:BE32" si="23">BD9*$V$3/(BD9*$V$3+(1-BD9)*$P$3)</f>
         <v>0.61540892858775742</v>
       </c>
       <c r="BF9" s="2">
@@ -3432,11 +3953,11 @@
         <v>2E-3</v>
       </c>
       <c r="BM9" s="2">
-        <f t="shared" ref="BM9:BM23" si="16">$W$3*BL9/(1+$W$3*BL9)</f>
+        <f t="shared" ref="BM9:BM23" si="24">$W$3*BL9/(1+$W$3*BL9)</f>
         <v>3.3188581523688464E-4</v>
       </c>
       <c r="BN9" s="2">
-        <f t="shared" ref="BN9:BN23" si="17">BM9*$W$3/(BM9*$W$3+(1-BM9)*$P$3)</f>
+        <f t="shared" ref="BN9:BN23" si="25">BM9*$W$3/(BM9*$W$3+(1-BM9)*$P$3)</f>
         <v>3.0498248189132953E-3</v>
       </c>
       <c r="BO9" s="2">
@@ -3457,21 +3978,147 @@
       <c r="BT9" s="2">
         <v>0</v>
       </c>
+      <c r="BV9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="BW9" s="2">
+        <f t="shared" ref="BW9:BW20" si="26">$X$3*BV9/(1+$X$3*BV9)</f>
+        <v>2.762422343639544E-2</v>
+      </c>
+      <c r="BX9" s="2">
+        <f t="shared" ref="BX9:BX20" si="27">BW9*$X$3/(BW9*$X$3+(1-BW9)*$P$3)</f>
+        <v>0.18300640274843663</v>
+      </c>
+      <c r="BY9" s="2">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="CA9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="CB9" s="2">
+        <f t="shared" ref="CB9:CB15" si="28">$Y$3*CA9/(1+$Y$3*CA9)</f>
+        <v>3.3678059022557626E-2</v>
+      </c>
+      <c r="CC9" s="2">
+        <f t="shared" ref="CC9:CC15" si="29">CB9*$Y$3/(CB9*$Y$3+(1-CB9)*$P$3)</f>
+        <v>0.25212468252311154</v>
+      </c>
+      <c r="CD9" s="2">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="CF9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="CG9" s="2">
+        <f t="shared" ref="CG9:CG24" si="30">$Z$3*CF9/(1+$Z$3*CF9)</f>
+        <v>2.5747448992764127E-2</v>
+      </c>
+      <c r="CH9" s="2">
+        <f t="shared" ref="CH9:CH24" si="31">CG9*$Z$3/(CG9*$Z$3+(1-CG9)*$P$3)</f>
+        <v>0.16237234255027658</v>
+      </c>
+      <c r="CI9" s="2">
+        <v>0.99209999999999998</v>
+      </c>
+      <c r="CK9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="CL9" s="2">
+        <f t="shared" ref="CL9:CL25" si="32">$AA$3*CK9/(1+$AA$3*CK9)</f>
+        <v>3.4851772728285255E-2</v>
+      </c>
+      <c r="CM9" s="2">
+        <f t="shared" ref="CM9:CM25" si="33">CL9*$AA$3/(CL9*$AA$3+(1-CL9)*$P$3)</f>
+        <v>0.19437453814267577</v>
+      </c>
+      <c r="CN9" s="2">
+        <v>0.99409999999999998</v>
+      </c>
+      <c r="CP9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="CQ9" s="2">
+        <f t="shared" ref="CQ9:CQ25" si="34">$AB$3*CP9/(1+$AB$3*CP9)</f>
+        <v>4.3337005835012869E-2</v>
+      </c>
+      <c r="CR9" s="2">
+        <f t="shared" ref="CR9:CR25" si="35">CQ9*$AB$3/(CQ9*$AB$3+(1-CQ9)*$P$3)</f>
+        <v>0.27520647104860979</v>
+      </c>
+      <c r="CS9" s="2">
+        <v>0.99450000000000005</v>
+      </c>
+      <c r="CU9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="CV9" s="2">
+        <f t="shared" ref="CV9:CV20" si="36">$AC$3*CU9/(1+$AC$3*CU9)</f>
+        <v>2.1515810562799446E-2</v>
+      </c>
+      <c r="CW9" s="2">
+        <f t="shared" ref="CW9:CW20" si="37">CV9*$AC$3/(CV9*$AC$3+(1-CV9)*$P$3)</f>
+        <v>0.11831912678773629</v>
+      </c>
+      <c r="CX9" s="2">
+        <v>0.99150000000000005</v>
+      </c>
+      <c r="CZ9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="DA9" s="2">
+        <f t="shared" ref="DA9:DA22" si="38">$AD$3*CZ9/(1+$AD$3*CZ9)</f>
+        <v>4.4366982955711752E-2</v>
+      </c>
+      <c r="DB9" s="2">
+        <f t="shared" ref="DB9:DB22" si="39">DA9*$AD$3/(DA9*$AD$3+(1-DA9)*$P$3)</f>
+        <v>0.28511410755327765</v>
+      </c>
+      <c r="DC9" s="2">
+        <v>0.99460000000000004</v>
+      </c>
+      <c r="DE9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="DF9" s="2">
+        <f t="shared" ref="DF9:DF18" si="40">$AE$3*DE9/(1+$AE$3*DE9)</f>
+        <v>4.5694604446998244E-2</v>
+      </c>
+      <c r="DG9" s="2">
+        <f t="shared" ref="DG9:DG18" si="41">DF9*$AE$3/(DF9*$AE$3+(1-DF9)*$P$3)</f>
+        <v>0.29786534268802795</v>
+      </c>
+      <c r="DH9" s="2">
+        <v>0.99470000000000003</v>
+      </c>
+      <c r="DJ9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="DK9" s="2">
+        <f t="shared" ref="DK9:DK23" si="42">$AF$3*DJ9/(1+$AF$3*DJ9)</f>
+        <v>4.6195407968835159E-2</v>
+      </c>
+      <c r="DL9" s="2">
+        <f t="shared" ref="DL9:DL23" si="43">DK9*$AF$3/(DK9*$AF$3+(1-DK9)*$P$3)</f>
+        <v>0.30266623233490525</v>
+      </c>
+      <c r="DM9" s="2">
+        <v>0.99460000000000004</v>
+      </c>
     </row>
-    <row r="10" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O10" s="2">
         <v>3</v>
       </c>
       <c r="P10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>5.1273901968132293E-2</v>
       </c>
       <c r="Q10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>0.14917440138037943</v>
       </c>
       <c r="R10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>0.94872609803186769</v>
       </c>
       <c r="S10" s="2">
@@ -3484,11 +4131,11 @@
         <v>1</v>
       </c>
       <c r="W10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.7696202904672331E-2</v>
       </c>
       <c r="X10" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>5.5216010687396497E-2</v>
       </c>
       <c r="Y10" s="2">
@@ -3499,11 +4146,11 @@
         <v>1</v>
       </c>
       <c r="AB10" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.14410161910296715</v>
       </c>
       <c r="AC10" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.61141991691823538</v>
       </c>
       <c r="AD10" s="2">
@@ -3513,11 +4160,11 @@
         <v>1</v>
       </c>
       <c r="AG10" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>5.0774994755531842E-2</v>
       </c>
       <c r="AH10" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0.13705919399834871</v>
       </c>
       <c r="AI10" s="2">
@@ -3527,11 +4174,11 @@
         <v>1</v>
       </c>
       <c r="AL10" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6.9378745168912417E-2</v>
       </c>
       <c r="AM10" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0.23577340981369546</v>
       </c>
       <c r="AN10" s="2">
@@ -3550,11 +4197,11 @@
         <v>0.1003</v>
       </c>
       <c r="AU10" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>8.4528386113373218E-3</v>
       </c>
       <c r="AV10" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>3.8664995157047646E-2</v>
       </c>
       <c r="AW10" s="2">
@@ -3573,11 +4220,11 @@
         <v>1.4990000000000001</v>
       </c>
       <c r="BD10" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.20295552381033677</v>
       </c>
       <c r="BE10" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.70597293355965607</v>
       </c>
       <c r="BF10" s="2">
@@ -3599,11 +4246,11 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="BM10" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>8.293016878920665E-4</v>
       </c>
       <c r="BN10" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>7.5898405212930873E-3</v>
       </c>
       <c r="BO10" s="2">
@@ -3624,8 +4271,134 @@
       <c r="BT10" s="2" t="s">
         <v>269</v>
       </c>
+      <c r="BV10" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="BW10" s="2">
+        <f t="shared" si="26"/>
+        <v>4.08718091603456E-2</v>
+      </c>
+      <c r="BX10" s="2">
+        <f t="shared" si="27"/>
+        <v>0.25149683828416014</v>
+      </c>
+      <c r="BY10" s="2">
+        <v>0.98819999999999997</v>
+      </c>
+      <c r="CA10" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="CB10" s="2">
+        <f t="shared" si="28"/>
+        <v>4.9680516844555378E-2</v>
+      </c>
+      <c r="CC10" s="2">
+        <f t="shared" si="29"/>
+        <v>0.33584909993613221</v>
+      </c>
+      <c r="CD10" s="2">
+        <v>0.98839999999999995</v>
+      </c>
+      <c r="CF10" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="CG10" s="2">
+        <f t="shared" si="30"/>
+        <v>3.8130294581735044E-2</v>
+      </c>
+      <c r="CH10" s="2">
+        <f t="shared" si="31"/>
+        <v>0.22526972717211577</v>
+      </c>
+      <c r="CI10" s="2">
+        <v>0.98860000000000003</v>
+      </c>
+      <c r="CK10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="CL10" s="2">
+        <f t="shared" si="32"/>
+        <v>4.5935387080805003E-2</v>
+      </c>
+      <c r="CM10" s="2">
+        <f t="shared" si="33"/>
+        <v>0.24339605243121196</v>
+      </c>
+      <c r="CN10" s="2">
+        <v>0.99239999999999995</v>
+      </c>
+      <c r="CP10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="CQ10" s="2">
+        <f t="shared" si="34"/>
+        <v>5.6959851310482541E-2</v>
+      </c>
+      <c r="CR10" s="2">
+        <f t="shared" si="35"/>
+        <v>0.33610885112900751</v>
+      </c>
+      <c r="CS10" s="2">
+        <v>0.9929</v>
+      </c>
+      <c r="CU10" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="CV10" s="2">
+        <f t="shared" si="36"/>
+        <v>3.1930213630349015E-2</v>
+      </c>
+      <c r="CW10" s="2">
+        <f t="shared" si="37"/>
+        <v>0.16756558342626765</v>
+      </c>
+      <c r="CX10" s="2">
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="CZ10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="DA10" s="2">
+        <f t="shared" si="38"/>
+        <v>5.8293869568427387E-2</v>
+      </c>
+      <c r="DB10" s="2">
+        <f t="shared" si="39"/>
+        <v>0.34715884833069383</v>
+      </c>
+      <c r="DC10" s="2">
+        <v>0.99309999999999998</v>
+      </c>
+      <c r="DE10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="DF10" s="2">
+        <f t="shared" si="40"/>
+        <v>6.001206342918277E-2</v>
+      </c>
+      <c r="DG10" s="2">
+        <f t="shared" si="41"/>
+        <v>0.36128260160585396</v>
+      </c>
+      <c r="DH10" s="2">
+        <v>0.99319999999999997</v>
+      </c>
+      <c r="DJ10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="DK10" s="2">
+        <f t="shared" si="42"/>
+        <v>6.0659809082487817E-2</v>
+      </c>
+      <c r="DL10" s="2">
+        <f t="shared" si="43"/>
+        <v>0.36657198886358855</v>
+      </c>
+      <c r="DM10" s="2">
+        <v>0.99299999999999999</v>
+      </c>
     </row>
-    <row r="11" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>217</v>
       </c>
@@ -3642,15 +4415,15 @@
         <v>4</v>
       </c>
       <c r="P11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>6.7216387142510672E-2</v>
       </c>
       <c r="Q11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>0.1894774723368661</v>
       </c>
       <c r="R11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>0.93278361285748934</v>
       </c>
       <c r="S11" s="2">
@@ -3663,11 +4436,11 @@
         <v>1.5</v>
       </c>
       <c r="W11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2.6311497557258968E-2</v>
       </c>
       <c r="X11" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>8.0598842749763352E-2</v>
       </c>
       <c r="Y11" s="2">
@@ -3678,11 +4451,11 @@
         <v>1.5</v>
       </c>
       <c r="AB11" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.20162517180028336</v>
       </c>
       <c r="AC11" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.70239938773207178</v>
       </c>
       <c r="AD11" s="2">
@@ -3692,11 +4465,11 @@
         <v>1.5</v>
       </c>
       <c r="AG11" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>7.4276790313972899E-2</v>
       </c>
       <c r="AH11" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0.19240345945951545</v>
       </c>
       <c r="AI11" s="2">
@@ -3706,11 +4479,11 @@
         <v>1.5</v>
       </c>
       <c r="AL11" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0.10057909215151825</v>
       </c>
       <c r="AM11" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0.31636489920507044</v>
       </c>
       <c r="AN11" s="2">
@@ -3729,11 +4502,11 @@
         <v>0.2001</v>
       </c>
       <c r="AU11" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>1.6722888232988821E-2</v>
       </c>
       <c r="AV11" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>7.4279542564348072E-2</v>
       </c>
       <c r="AW11" s="2">
@@ -3752,11 +4525,11 @@
         <v>1.9970000000000001</v>
       </c>
       <c r="BD11" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.25330248815515605</v>
       </c>
       <c r="BE11" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.76183257274249183</v>
       </c>
       <c r="BF11" s="2">
@@ -3778,11 +4551,11 @@
         <v>0.01</v>
       </c>
       <c r="BM11" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>1.657229032949884E-3</v>
       </c>
       <c r="BN11" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>1.5065337533308909E-2</v>
       </c>
       <c r="BO11" s="2">
@@ -3803,8 +4576,134 @@
       <c r="BT11" s="2" t="s">
         <v>271</v>
       </c>
+      <c r="BV11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="BW11" s="2">
+        <f t="shared" si="26"/>
+        <v>5.3763278066800521E-2</v>
+      </c>
+      <c r="BX11" s="2">
+        <f t="shared" si="27"/>
+        <v>0.30939207484129311</v>
+      </c>
+      <c r="BY11" s="2">
+        <v>0.98480000000000001</v>
+      </c>
+      <c r="CA11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="CB11" s="2">
+        <f t="shared" si="28"/>
+        <v>6.5161601774547648E-2</v>
+      </c>
+      <c r="CC11" s="2">
+        <f t="shared" si="29"/>
+        <v>0.40271497885508362</v>
+      </c>
+      <c r="CD11" s="2">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="CF11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="CG11" s="2">
+        <f t="shared" si="30"/>
+        <v>5.0202316404582663E-2</v>
+      </c>
+      <c r="CH11" s="2">
+        <f t="shared" si="31"/>
+        <v>0.27938094637390842</v>
+      </c>
+      <c r="CI11" s="2">
+        <v>0.98529999999999995</v>
+      </c>
+      <c r="CK11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="CL11" s="2">
+        <f t="shared" si="32"/>
+        <v>5.6767326571109653E-2</v>
+      </c>
+      <c r="CM11" s="2">
+        <f t="shared" si="33"/>
+        <v>0.28679393747816745</v>
+      </c>
+      <c r="CN11" s="2">
+        <v>0.99060000000000004</v>
+      </c>
+      <c r="CP11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="CQ11" s="2">
+        <f t="shared" si="34"/>
+        <v>7.0200166378382223E-2</v>
+      </c>
+      <c r="CR11" s="2">
+        <f t="shared" si="35"/>
+        <v>0.38756966518667268</v>
+      </c>
+      <c r="CS11" s="2">
+        <v>0.99129999999999996</v>
+      </c>
+      <c r="CU11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="CV11" s="2">
+        <f t="shared" si="36"/>
+        <v>4.2125261969162102E-2</v>
+      </c>
+      <c r="CW11" s="2">
+        <f t="shared" si="37"/>
+        <v>0.21160172253799606</v>
+      </c>
+      <c r="CX11" s="2">
+        <v>0.98329999999999995</v>
+      </c>
+      <c r="CZ11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="DA11" s="2">
+        <f t="shared" si="38"/>
+        <v>7.1820660900816624E-2</v>
+      </c>
+      <c r="DB11" s="2">
+        <f t="shared" si="39"/>
+        <v>0.39929395318048083</v>
+      </c>
+      <c r="DC11" s="2">
+        <v>0.99160000000000004</v>
+      </c>
+      <c r="DE11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="DF11" s="2">
+        <f t="shared" si="40"/>
+        <v>7.3906262458854816E-2</v>
+      </c>
+      <c r="DG11" s="2">
+        <f t="shared" si="41"/>
+        <v>0.41419306498600583</v>
+      </c>
+      <c r="DH11" s="2">
+        <v>0.99170000000000003</v>
+      </c>
+      <c r="DJ11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="DK11" s="2">
+        <f t="shared" si="42"/>
+        <v>7.4692059830781532E-2</v>
+      </c>
+      <c r="DL11" s="2">
+        <f t="shared" si="43"/>
+        <v>0.41974801949731488</v>
+      </c>
+      <c r="DM11" s="2">
+        <v>0.99139999999999995</v>
+      </c>
     </row>
-    <row r="12" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>221</v>
       </c>
@@ -3821,15 +4720,15 @@
         <v>5</v>
       </c>
       <c r="P12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>8.2631928995711312E-2</v>
       </c>
       <c r="Q12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>0.22613496979991718</v>
       </c>
       <c r="R12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>0.91736807100428863</v>
       </c>
       <c r="S12" s="2">
@@ -3842,11 +4741,11 @@
         <v>2</v>
       </c>
       <c r="W12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>3.4776985222435643E-2</v>
       </c>
       <c r="X12" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.10465347403405539</v>
       </c>
       <c r="Y12" s="2">
@@ -3857,11 +4756,11 @@
         <v>2</v>
       </c>
       <c r="AB12" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.25190353146418937</v>
       </c>
       <c r="AC12" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.75885858242033788</v>
       </c>
       <c r="AD12" s="2">
@@ -3871,11 +4770,11 @@
         <v>2</v>
       </c>
       <c r="AG12" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>9.6642944510389517E-2</v>
       </c>
       <c r="AH12" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0.24107662067511987</v>
       </c>
       <c r="AI12" s="2">
@@ -3885,11 +4784,11 @@
         <v>2</v>
       </c>
       <c r="AL12" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0.12975523495738411</v>
       </c>
       <c r="AM12" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0.38158032523007684</v>
       </c>
       <c r="AN12" s="2">
@@ -3908,11 +4807,11 @@
         <v>0.29980000000000001</v>
       </c>
       <c r="AU12" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>2.4848043211501438E-2</v>
       </c>
       <c r="AV12" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>0.10731758230290443</v>
       </c>
       <c r="AW12" s="2">
@@ -3931,11 +4830,11 @@
         <v>2</v>
       </c>
       <c r="BD12" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.25358651678683924</v>
       </c>
       <c r="BE12" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.76210483556447217</v>
       </c>
       <c r="BF12" s="2">
@@ -3955,11 +4854,11 @@
         <v>0.02</v>
       </c>
       <c r="BM12" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>3.3089743375582796E-3</v>
       </c>
       <c r="BN12" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>2.9683483370477211E-2</v>
       </c>
       <c r="BO12" s="2">
@@ -3980,8 +4879,134 @@
       <c r="BT12" s="2" t="s">
         <v>273</v>
       </c>
+      <c r="BV12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="BW12" s="2">
+        <f t="shared" si="26"/>
+        <v>6.631279921757012E-2</v>
+      </c>
+      <c r="BX12" s="2">
+        <f t="shared" si="27"/>
+        <v>0.35897415397354798</v>
+      </c>
+      <c r="BY12" s="2">
+        <v>0.98150000000000004</v>
+      </c>
+      <c r="CA12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="CB12" s="2">
+        <f t="shared" si="28"/>
+        <v>8.0146385504210854E-2</v>
+      </c>
+      <c r="CC12" s="2">
+        <f t="shared" si="29"/>
+        <v>0.45734845520230416</v>
+      </c>
+      <c r="CD12" s="2">
+        <v>0.98150000000000004</v>
+      </c>
+      <c r="CF12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="CG12" s="2">
+        <f t="shared" si="30"/>
+        <v>6.1975072456562995E-2</v>
+      </c>
+      <c r="CH12" s="2">
+        <f t="shared" si="31"/>
+        <v>0.32642682420063474</v>
+      </c>
+      <c r="CI12" s="2">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="CK12" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="CL12" s="2">
+        <f t="shared" si="32"/>
+        <v>6.73560671136543E-2</v>
+      </c>
+      <c r="CM12" s="2">
+        <f t="shared" si="33"/>
+        <v>0.32548339224468037</v>
+      </c>
+      <c r="CN12" s="2">
+        <v>0.98880000000000001</v>
+      </c>
+      <c r="CP12" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="CQ12" s="2">
+        <f t="shared" si="34"/>
+        <v>8.307384017368194E-2</v>
+      </c>
+      <c r="CR12" s="2">
+        <f t="shared" si="35"/>
+        <v>0.43162652840415072</v>
+      </c>
+      <c r="CS12" s="2">
+        <v>0.98980000000000001</v>
+      </c>
+      <c r="CU12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="CV12" s="2">
+        <f t="shared" si="36"/>
+        <v>5.210781363643386E-2</v>
+      </c>
+      <c r="CW12" s="2">
+        <f t="shared" si="37"/>
+        <v>0.25121288345670134</v>
+      </c>
+      <c r="CX12" s="2">
+        <v>0.97929999999999995</v>
+      </c>
+      <c r="CZ12" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="DA12" s="2">
+        <f t="shared" si="38"/>
+        <v>8.4964353871369414E-2</v>
+      </c>
+      <c r="DB12" s="2">
+        <f t="shared" si="39"/>
+        <v>0.44371796384074408</v>
+      </c>
+      <c r="DC12" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="DE12" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="DF12" s="2">
+        <f t="shared" si="40"/>
+        <v>8.7395697085313417E-2</v>
+      </c>
+      <c r="DG12" s="2">
+        <f t="shared" si="41"/>
+        <v>0.45900808487745681</v>
+      </c>
+      <c r="DH12" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="DJ12" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="DK12" s="2">
+        <f t="shared" si="42"/>
+        <v>8.8311242081481708E-2</v>
+      </c>
+      <c r="DL12" s="2">
+        <f t="shared" si="43"/>
+        <v>0.46468730795670476</v>
+      </c>
+      <c r="DM12" s="2">
+        <v>0.98980000000000001</v>
+      </c>
     </row>
-    <row r="13" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>225</v>
       </c>
@@ -3995,15 +5020,15 @@
         <v>6</v>
       </c>
       <c r="P13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>9.7546228194460724E-2</v>
       </c>
       <c r="Q13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>0.25962012589419375</v>
       </c>
       <c r="R13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>0.90245377180553932</v>
       </c>
       <c r="S13" s="2">
@@ -4016,11 +5041,11 @@
         <v>2.5</v>
       </c>
       <c r="W13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>4.3096539597861319E-2</v>
       </c>
       <c r="X13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.12748149715449902</v>
       </c>
       <c r="Y13" s="2">
@@ -4031,11 +5056,11 @@
         <v>2.5</v>
       </c>
       <c r="AB13" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.29622441995696414</v>
       </c>
       <c r="AC13" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.79731154989941444</v>
       </c>
       <c r="AD13" s="2">
@@ -4045,11 +5070,11 @@
         <v>2.5</v>
       </c>
       <c r="AG13" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.11795382929319435</v>
       </c>
       <c r="AH13" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0.28421629958284483</v>
       </c>
       <c r="AI13" s="2">
@@ -4059,11 +5084,11 @@
         <v>2.5</v>
       </c>
       <c r="AL13" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0.15709797260989863</v>
       </c>
       <c r="AM13" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0.43543687083956412</v>
       </c>
       <c r="AN13" s="2">
@@ -4082,11 +5107,11 @@
         <v>0.4002</v>
       </c>
       <c r="AU13" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>3.2895665921423928E-2</v>
       </c>
       <c r="AV13" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>0.13828717688701364</v>
       </c>
       <c r="AW13" s="2">
@@ -4105,11 +5130,11 @@
         <v>2.4969999999999999</v>
       </c>
       <c r="BD13" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.29783436178013001</v>
       </c>
       <c r="BE13" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.79998440022501749</v>
       </c>
       <c r="BF13" s="2">
@@ -4131,11 +5156,11 @@
         <v>0.05</v>
       </c>
       <c r="BM13" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>8.2315787197836665E-3</v>
       </c>
       <c r="BN13" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>7.1045396172442529E-2</v>
       </c>
       <c r="BO13" s="2">
@@ -4156,8 +5181,134 @@
       <c r="BT13" s="2" t="s">
         <v>275</v>
       </c>
+      <c r="BV13" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="BW13" s="2">
+        <f t="shared" si="26"/>
+        <v>7.8533799840954918E-2</v>
+      </c>
+      <c r="BX13" s="2">
+        <f t="shared" si="27"/>
+        <v>0.40191366145034757</v>
+      </c>
+      <c r="BY13" s="2">
+        <v>0.97809999999999997</v>
+      </c>
+      <c r="CA13" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="CB13" s="2">
+        <f t="shared" si="28"/>
+        <v>9.465835756178459E-2</v>
+      </c>
+      <c r="CC13" s="2">
+        <f t="shared" si="29"/>
+        <v>0.50282490732252527</v>
+      </c>
+      <c r="CD13" s="2">
+        <v>0.97829999999999995</v>
+      </c>
+      <c r="CF13" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="CG13" s="2">
+        <f t="shared" si="30"/>
+        <v>7.3459554702808905E-2</v>
+      </c>
+      <c r="CH13" s="2">
+        <f t="shared" si="31"/>
+        <v>0.36770634608272135</v>
+      </c>
+      <c r="CI13" s="2">
+        <v>0.9788</v>
+      </c>
+      <c r="CK13" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="CL13" s="2">
+        <f t="shared" si="32"/>
+        <v>7.77097082452715E-2</v>
+      </c>
+      <c r="CM13" s="2">
+        <f t="shared" si="33"/>
+        <v>0.36019124617513987</v>
+      </c>
+      <c r="CN13" s="2">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="CP13" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="CQ13" s="2">
+        <f t="shared" si="34"/>
+        <v>9.559589386788872E-2</v>
+      </c>
+      <c r="CR13" s="2">
+        <f t="shared" si="35"/>
+        <v>0.46977007845303748</v>
+      </c>
+      <c r="CS13" s="2">
+        <v>0.98819999999999997</v>
+      </c>
+      <c r="CU13" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="CV13" s="2">
+        <f t="shared" si="36"/>
+        <v>6.1884443751322966E-2</v>
+      </c>
+      <c r="CW13" s="2">
+        <f t="shared" si="37"/>
+        <v>0.28703412605661044</v>
+      </c>
+      <c r="CX13" s="2">
+        <v>0.97529999999999994</v>
+      </c>
+      <c r="CZ13" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="DA13" s="2">
+        <f t="shared" si="38"/>
+        <v>9.7740996086722251E-2</v>
+      </c>
+      <c r="DB13" s="2">
+        <f t="shared" si="39"/>
+        <v>0.48202385087535371</v>
+      </c>
+      <c r="DC13" s="2">
+        <v>0.98870000000000002</v>
+      </c>
+      <c r="DE13" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="DF13" s="2">
+        <f t="shared" si="40"/>
+        <v>0.10049780070812771</v>
+      </c>
+      <c r="DG13" s="2">
+        <f t="shared" si="41"/>
+        <v>0.49745356437391069</v>
+      </c>
+      <c r="DH13" s="2">
+        <v>0.98850000000000005</v>
+      </c>
+      <c r="DJ13" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="DK13" s="2">
+        <f t="shared" si="42"/>
+        <v>0.10153533056878149</v>
+      </c>
+      <c r="DL13" s="2">
+        <f t="shared" si="43"/>
+        <v>0.50316604666916975</v>
+      </c>
+      <c r="DM13" s="2">
+        <v>0.98819999999999997</v>
+      </c>
     </row>
-    <row r="14" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>226</v>
       </c>
@@ -4177,11 +5328,11 @@
         <v>3</v>
       </c>
       <c r="W14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>5.1273901968132293E-2</v>
       </c>
       <c r="X14" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.14917440138037943</v>
       </c>
       <c r="Y14" s="2">
@@ -4192,11 +5343,11 @@
         <v>3</v>
       </c>
       <c r="AB14" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.33558746359849817</v>
       </c>
       <c r="AC14" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.82518754740367339</v>
       </c>
       <c r="AD14" s="2">
@@ -4206,11 +5357,11 @@
         <v>3</v>
       </c>
       <c r="AG14" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.13828240725979835</v>
       </c>
       <c r="AH14" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0.3227153660669968</v>
       </c>
       <c r="AI14" s="2">
@@ -4220,11 +5371,11 @@
         <v>3</v>
       </c>
       <c r="AL14" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0.18277485528985751</v>
       </c>
       <c r="AM14" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0.480664440986109</v>
       </c>
       <c r="AN14" s="2">
@@ -4243,11 +5394,11 @@
         <v>0.50019999999999998</v>
       </c>
       <c r="AU14" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>4.0780266594919894E-2</v>
       </c>
       <c r="AV14" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>0.16706871510031945</v>
       </c>
       <c r="AW14" s="2">
@@ -4266,11 +5417,11 @@
         <v>2.5009999999999999</v>
       </c>
       <c r="BD14" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.29816921051903705</v>
       </c>
       <c r="BE14" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.8002403947272414</v>
       </c>
       <c r="BF14" s="2">
@@ -4292,11 +5443,11 @@
         <v>0.1</v>
       </c>
       <c r="BM14" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>1.6328746080807803E-2</v>
       </c>
       <c r="BN14" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>0.13266551805616264</v>
       </c>
       <c r="BO14" s="2">
@@ -4317,8 +5468,134 @@
       <c r="BT14" s="2" t="s">
         <v>277</v>
       </c>
+      <c r="BV14" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="BW14" s="2">
+        <f t="shared" si="26"/>
+        <v>9.0439013253667905E-2</v>
+      </c>
+      <c r="BX14" s="2">
+        <f t="shared" si="27"/>
+        <v>0.43946166395425285</v>
+      </c>
+      <c r="BY14" s="2">
+        <v>0.97489999999999999</v>
+      </c>
+      <c r="CA14" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="CB14" s="2">
+        <f t="shared" si="28"/>
+        <v>0.10871954817785286</v>
+      </c>
+      <c r="CC14" s="2">
+        <f t="shared" si="29"/>
+        <v>0.54126851044293456</v>
+      </c>
+      <c r="CD14" s="2">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="CF14" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="CG14" s="2">
+        <f t="shared" si="30"/>
+        <v>8.4666223309496358E-2</v>
+      </c>
+      <c r="CH14" s="2">
+        <f t="shared" si="31"/>
+        <v>0.40421845523113448</v>
+      </c>
+      <c r="CI14" s="2">
+        <v>0.97560000000000002</v>
+      </c>
+      <c r="CK14" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="CL14" s="2">
+        <f t="shared" si="32"/>
+        <v>8.7835993787360414E-2</v>
+      </c>
+      <c r="CM14" s="2">
+        <f t="shared" si="33"/>
+        <v>0.3915020511047943</v>
+      </c>
+      <c r="CN14" s="2">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="CP14" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="CQ14" s="2">
+        <f t="shared" si="34"/>
+        <v>0.10778053913752784</v>
+      </c>
+      <c r="CR14" s="2">
+        <f t="shared" si="35"/>
+        <v>0.50311597119500651</v>
+      </c>
+      <c r="CS14" s="2">
+        <v>0.98660000000000003</v>
+      </c>
+      <c r="CU14" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="CV14" s="2">
+        <f t="shared" si="36"/>
+        <v>7.146145893721223E-2</v>
+      </c>
+      <c r="CW14" s="2">
+        <f t="shared" si="37"/>
+        <v>0.31958453574619289</v>
+      </c>
+      <c r="CX14" s="2">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="CZ14" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="DA14" s="2">
+        <f t="shared" si="38"/>
+        <v>0.11016575120519151</v>
+      </c>
+      <c r="DB14" s="2">
+        <f t="shared" si="39"/>
+        <v>0.51539408104822848</v>
+      </c>
+      <c r="DC14" s="2">
+        <v>0.98709999999999998</v>
+      </c>
+      <c r="DE14" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="DF14" s="2">
+        <f t="shared" si="40"/>
+        <v>0.11322901974349477</v>
+      </c>
+      <c r="DG14" s="2">
+        <f t="shared" si="41"/>
+        <v>0.5307973541712242</v>
+      </c>
+      <c r="DH14" s="2">
+        <v>0.98680000000000001</v>
+      </c>
+      <c r="DJ14" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="DK14" s="2">
+        <f t="shared" si="42"/>
+        <v>0.11438127204039329</v>
+      </c>
+      <c r="DL14" s="2">
+        <f t="shared" si="43"/>
+        <v>0.53648397867194964</v>
+      </c>
+      <c r="DM14" s="2">
+        <v>0.98650000000000004</v>
+      </c>
     </row>
-    <row r="15" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>247</v>
       </c>
@@ -4335,11 +5612,11 @@
         <v>3.5</v>
       </c>
       <c r="W15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>5.9312686814621103E-2</v>
       </c>
       <c r="X15" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.16981479813424177</v>
       </c>
       <c r="Y15" s="2">
@@ -4354,7 +5631,7 @@
         <v>0.37078049331438545</v>
       </c>
       <c r="AC15" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.84632294595670765</v>
       </c>
       <c r="AD15" s="2">
@@ -4364,11 +5641,11 @@
         <v>3.5</v>
       </c>
       <c r="AG15" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.15769506624096574</v>
       </c>
       <c r="AH15" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0.3572843994516518</v>
       </c>
       <c r="AI15" s="2">
@@ -4378,11 +5655,11 @@
         <v>3.5</v>
       </c>
       <c r="AL15" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0.20693362074058921</v>
       </c>
       <c r="AM15" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0.51918304327307407</v>
       </c>
       <c r="AN15" s="2">
@@ -4401,11 +5678,11 @@
         <v>0.59989999999999999</v>
       </c>
       <c r="AU15" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>4.8514260317260971E-2</v>
       </c>
       <c r="AV15" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>0.19391160513049979</v>
       </c>
       <c r="AW15" s="2">
@@ -4424,11 +5701,11 @@
         <v>2.9940000000000002</v>
       </c>
       <c r="BD15" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.33712971519022544</v>
       </c>
       <c r="BE15" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.827457924973381</v>
       </c>
       <c r="BF15" s="2">
@@ -4450,11 +5727,11 @@
         <v>0.2</v>
       </c>
       <c r="BM15" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>3.2132803768023133E-2</v>
       </c>
       <c r="BN15" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>0.23425365377739787</v>
       </c>
       <c r="BO15" s="2">
@@ -4475,8 +5752,134 @@
       <c r="BT15" s="2" t="s">
         <v>279</v>
       </c>
+      <c r="BV15" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="BW15" s="2">
+        <f t="shared" si="26"/>
+        <v>0.10204052311527284</v>
+      </c>
+      <c r="BX15" s="2">
+        <f t="shared" si="27"/>
+        <v>0.47257361761379757</v>
+      </c>
+      <c r="BY15" s="2">
+        <v>0.9718</v>
+      </c>
+      <c r="CA15" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="CB15" s="2">
+        <f t="shared" si="28"/>
+        <v>0.12235063987659549</v>
+      </c>
+      <c r="CC15" s="2">
+        <f t="shared" si="29"/>
+        <v>0.57419359588472552</v>
+      </c>
+      <c r="CD15" s="2">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="CF15" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="CG15" s="2">
+        <f t="shared" si="30"/>
+        <v>9.5605038420506758E-2</v>
+      </c>
+      <c r="CH15" s="2">
+        <f t="shared" si="31"/>
+        <v>0.43674395365312446</v>
+      </c>
+      <c r="CI15" s="2">
+        <v>0.97240000000000004</v>
+      </c>
+      <c r="CK15" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="CL15" s="2">
+        <f t="shared" si="32"/>
+        <v>9.7742331161695353E-2</v>
+      </c>
+      <c r="CM15" s="2">
+        <f t="shared" si="33"/>
+        <v>0.41989127077425376</v>
+      </c>
+      <c r="CN15" s="2">
+        <v>0.98319999999999996</v>
+      </c>
+      <c r="CP15" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="CQ15" s="2">
+        <f t="shared" si="34"/>
+        <v>0.11964123196912997</v>
+      </c>
+      <c r="CR15" s="2">
+        <f t="shared" si="35"/>
+        <v>0.53251581609543763</v>
+      </c>
+      <c r="CS15" s="2">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="CU15" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="CV15" s="2">
+        <f t="shared" si="36"/>
+        <v>8.084491088828176E-2</v>
+      </c>
+      <c r="CW15" s="2">
+        <f t="shared" si="37"/>
+        <v>0.34929254160310114</v>
+      </c>
+      <c r="CX15" s="2">
+        <v>0.9667</v>
+      </c>
+      <c r="CZ15" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="DA15" s="2">
+        <f t="shared" si="38"/>
+        <v>0.12225295897305</v>
+      </c>
+      <c r="DB15" s="2">
+        <f t="shared" si="39"/>
+        <v>0.54472484600067506</v>
+      </c>
+      <c r="DC15" s="2">
+        <v>0.98550000000000004</v>
+      </c>
+      <c r="DE15" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="DF15" s="2">
+        <f t="shared" si="40"/>
+        <v>0.12560488249642324</v>
+      </c>
+      <c r="DG15" s="2">
+        <f t="shared" si="41"/>
+        <v>0.5599917556598818</v>
+      </c>
+      <c r="DH15" s="2">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="DJ15" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="DK15" s="2">
+        <f t="shared" si="42"/>
+        <v>0.12686505771063983</v>
+      </c>
+      <c r="DL15" s="2">
+        <f t="shared" si="43"/>
+        <v>0.56561411233371872</v>
+      </c>
+      <c r="DM15" s="2">
+        <v>0.98470000000000002</v>
+      </c>
     </row>
-    <row r="16" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>249</v>
       </c>
@@ -4490,11 +5893,11 @@
         <v>4</v>
       </c>
       <c r="W16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>6.7216387142510672E-2</v>
       </c>
       <c r="X16" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.1894774723368661</v>
       </c>
       <c r="Y16" s="2">
@@ -4505,11 +5908,11 @@
         <v>4</v>
       </c>
       <c r="AB16" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.40243281552144905</v>
       </c>
       <c r="AC16" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.86289891638256044</v>
       </c>
       <c r="AD16" s="2">
@@ -4519,11 +5922,11 @@
         <v>4</v>
       </c>
       <c r="AG16" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.17625234356208255</v>
       </c>
       <c r="AH16" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0.38849595046594171</v>
       </c>
       <c r="AI16" s="2">
@@ -4533,11 +5936,11 @@
         <v>4</v>
       </c>
       <c r="AL16" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0.22970503865340117</v>
       </c>
       <c r="AM16" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0.55238239610358042</v>
       </c>
       <c r="AN16" s="2">
@@ -4556,11 +5959,11 @@
         <v>0.70020000000000004</v>
       </c>
       <c r="AU16" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>5.6169966863452679E-2</v>
       </c>
       <c r="AV16" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>0.21922507777099209</v>
       </c>
       <c r="AW16" s="2">
@@ -4579,11 +5982,11 @@
         <v>2.9990000000000001</v>
       </c>
       <c r="BD16" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.33750270704675117</v>
       </c>
       <c r="BE16" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.82769602498945793</v>
       </c>
       <c r="BF16" s="2">
@@ -4605,11 +6008,11 @@
         <v>0.3</v>
       </c>
       <c r="BM16" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>4.7437062737890681E-2</v>
       </c>
       <c r="BN16" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>0.31453947054939485</v>
       </c>
       <c r="BO16" s="2">
@@ -4630,8 +6033,120 @@
       <c r="BT16" s="2" t="s">
         <v>281</v>
       </c>
+      <c r="BV16" s="2">
+        <v>1</v>
+      </c>
+      <c r="BW16" s="2">
+        <f t="shared" si="26"/>
+        <v>0.1243777609463725</v>
+      </c>
+      <c r="BX16" s="2">
+        <f t="shared" si="27"/>
+        <v>0.52830166478726903</v>
+      </c>
+      <c r="BY16" s="2">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="CF16" s="2">
+        <v>1</v>
+      </c>
+      <c r="CG16" s="2">
+        <f t="shared" si="30"/>
+        <v>0.11671662370229109</v>
+      </c>
+      <c r="CH16" s="2">
+        <f t="shared" si="31"/>
+        <v>0.49218972090277874</v>
+      </c>
+      <c r="CI16" s="2">
+        <v>0.96619999999999995</v>
+      </c>
+      <c r="CK16" s="2">
+        <v>1</v>
+      </c>
+      <c r="CL16" s="2">
+        <f t="shared" si="32"/>
+        <v>0.10743580946110901</v>
+      </c>
+      <c r="CM16" s="2">
+        <f t="shared" si="33"/>
+        <v>0.44574959381642776</v>
+      </c>
+      <c r="CN16" s="2">
+        <v>0.98119999999999996</v>
+      </c>
+      <c r="CP16" s="2">
+        <v>1</v>
+      </c>
+      <c r="CQ16" s="2">
+        <f t="shared" si="34"/>
+        <v>0.13119072222898928</v>
+      </c>
+      <c r="CR16" s="2">
+        <f t="shared" si="35"/>
+        <v>0.55863092846517681</v>
+      </c>
+      <c r="CS16" s="2">
+        <v>0.98319999999999996</v>
+      </c>
+      <c r="CU16" s="2">
+        <v>1</v>
+      </c>
+      <c r="CV16" s="2">
+        <f t="shared" si="36"/>
+        <v>9.9054132972042019E-2</v>
+      </c>
+      <c r="CW16" s="2">
+        <f t="shared" si="37"/>
+        <v>0.40155098589247329</v>
+      </c>
+      <c r="CX16" s="2">
+        <v>0.95850000000000002</v>
+      </c>
+      <c r="CZ16" s="2">
+        <v>1</v>
+      </c>
+      <c r="DA16" s="2">
+        <f t="shared" si="38"/>
+        <v>0.13401619043330368</v>
+      </c>
+      <c r="DB16" s="2">
+        <f t="shared" si="39"/>
+        <v>0.57070775196722368</v>
+      </c>
+      <c r="DC16" s="2">
+        <v>0.98380000000000001</v>
+      </c>
+      <c r="DE16" s="2">
+        <v>1</v>
+      </c>
+      <c r="DF16" s="2">
+        <f t="shared" si="40"/>
+        <v>0.13764006234517406</v>
+      </c>
+      <c r="DG16" s="2">
+        <f t="shared" si="41"/>
+        <v>0.58576593994272563</v>
+      </c>
+      <c r="DH16" s="2">
+        <v>0.98329999999999995</v>
+      </c>
+      <c r="DJ16" s="2">
+        <v>1</v>
+      </c>
+      <c r="DK16" s="2">
+        <f t="shared" si="42"/>
+        <v>0.13900178967087998</v>
+      </c>
+      <c r="DL16" s="2">
+        <f t="shared" si="43"/>
+        <v>0.59129932034831578</v>
+      </c>
+      <c r="DM16" s="2">
+        <v>0.98280000000000001</v>
+      </c>
     </row>
-    <row r="17" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>252</v>
       </c>
@@ -4648,11 +6163,11 @@
         <v>4.5</v>
       </c>
       <c r="W17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>7.4988379541517991E-2</v>
       </c>
       <c r="X17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.20823028780433153</v>
       </c>
       <c r="Y17" s="2">
@@ -4663,11 +6178,11 @@
         <v>4.5</v>
       </c>
       <c r="AB17" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.43105317462371995</v>
       </c>
       <c r="AC17" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.87624718737205387</v>
       </c>
       <c r="AD17" s="2">
@@ -4677,11 +6192,11 @@
         <v>4.5</v>
       </c>
       <c r="AG17" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.19400955662868707</v>
       </c>
       <c r="AH17" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0.41681650379759239</v>
       </c>
       <c r="AI17" s="2">
@@ -4691,11 +6206,11 @@
         <v>4.5</v>
       </c>
       <c r="AL17" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0.25120527870326731</v>
       </c>
       <c r="AM17" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0.58129318062265156</v>
       </c>
       <c r="AN17" s="2">
@@ -4714,11 +6229,11 @@
         <v>0.80020000000000002</v>
       </c>
       <c r="AU17" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>6.3681106710595001E-2</v>
       </c>
       <c r="AV17" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>0.2429281809430828</v>
       </c>
       <c r="AW17" s="2">
@@ -4737,11 +6252,11 @@
         <v>3.496</v>
       </c>
       <c r="BD17" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.3725944959271093</v>
       </c>
       <c r="BE17" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.84847966932907226</v>
       </c>
       <c r="BF17" s="2">
@@ -4763,11 +6278,11 @@
         <v>0.4</v>
       </c>
       <c r="BM17" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>6.2264862914375774E-2</v>
       </c>
       <c r="BN17" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>0.3795875394988239</v>
       </c>
       <c r="BO17" s="2">
@@ -4788,17 +6303,129 @@
       <c r="BT17" s="2" t="s">
         <v>283</v>
       </c>
+      <c r="BV17" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="BW17" s="2">
+        <f t="shared" si="26"/>
+        <v>0.17564356476453286</v>
+      </c>
+      <c r="BX17" s="2">
+        <f t="shared" si="27"/>
+        <v>0.62686546326154513</v>
+      </c>
+      <c r="BY17" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="CF17" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="CG17" s="2">
+        <f t="shared" si="30"/>
+        <v>0.16542123172559384</v>
+      </c>
+      <c r="CH17" s="2">
+        <f t="shared" si="31"/>
+        <v>0.59247863448110971</v>
+      </c>
+      <c r="CI17" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="CK17" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="CL17" s="2">
+        <f t="shared" si="32"/>
+        <v>0.1262110540033724</v>
+      </c>
+      <c r="CM17" s="2">
+        <f t="shared" si="33"/>
+        <v>0.4911165151507188</v>
+      </c>
+      <c r="CN17" s="2">
+        <v>0.9768</v>
+      </c>
+      <c r="CP17" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="CQ17" s="2">
+        <f t="shared" si="34"/>
+        <v>0.15340383470135369</v>
+      </c>
+      <c r="CR17" s="2">
+        <f t="shared" si="35"/>
+        <v>0.60298760862623768</v>
+      </c>
+      <c r="CS17" s="2">
+        <v>0.97940000000000005</v>
+      </c>
+      <c r="CU17" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="CV17" s="2">
+        <f t="shared" si="36"/>
+        <v>0.1415696690467792</v>
+      </c>
+      <c r="CW17" s="2">
+        <f t="shared" si="37"/>
+        <v>0.50161456690029094</v>
+      </c>
+      <c r="CX17" s="2">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="CZ17" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="DA17" s="2">
+        <f t="shared" si="38"/>
+        <v>0.15662146607526714</v>
+      </c>
+      <c r="DB17" s="2">
+        <f t="shared" si="39"/>
+        <v>0.61468787526937008</v>
+      </c>
+      <c r="DC17" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="DE17" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="DF17" s="2">
+        <f t="shared" si="40"/>
+        <v>0.16074313576846283</v>
+      </c>
+      <c r="DG17" s="2">
+        <f t="shared" si="41"/>
+        <v>0.62920567697335172</v>
+      </c>
+      <c r="DH17" s="2">
+        <v>0.97950000000000004</v>
+      </c>
+      <c r="DJ17" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="DK17" s="2">
+        <f t="shared" si="42"/>
+        <v>0.16229041595229585</v>
+      </c>
+      <c r="DL17" s="2">
+        <f t="shared" si="43"/>
+        <v>0.63452083653945413</v>
+      </c>
+      <c r="DM17" s="2">
+        <v>0.9788</v>
+      </c>
     </row>
-    <row r="18" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="V18" s="2">
         <v>5</v>
       </c>
       <c r="W18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>8.2631928995711312E-2</v>
       </c>
       <c r="X18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.22613496979991718</v>
       </c>
       <c r="Y18" s="2">
@@ -4809,11 +6436,11 @@
         <v>5</v>
       </c>
       <c r="AB18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.45705730488675578</v>
       </c>
       <c r="AC18" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.88722686942509832</v>
       </c>
       <c r="AD18" s="2">
@@ -4823,11 +6450,11 @@
         <v>5</v>
       </c>
       <c r="AG18" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.21101735367330596</v>
       </c>
       <c r="AH18" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0.44262995209633699</v>
       </c>
       <c r="AI18" s="2">
@@ -4846,11 +6473,11 @@
         <v>0.90010000000000001</v>
       </c>
       <c r="AU18" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>7.1066306676348431E-2</v>
       </c>
       <c r="AV18" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>0.26521286011932754</v>
       </c>
       <c r="AW18" s="2">
@@ -4869,11 +6496,11 @@
         <v>3.9950000000000001</v>
       </c>
       <c r="BD18" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.40427633678677316</v>
       </c>
       <c r="BE18" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.86484761840624835</v>
       </c>
       <c r="BF18" s="2">
@@ -4895,11 +6522,11 @@
         <v>0.5</v>
       </c>
       <c r="BM18" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>7.6638113239255054E-2</v>
       </c>
       <c r="BN18" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>0.43335991811487096</v>
       </c>
       <c r="BO18" s="2">
@@ -4920,8 +6547,120 @@
       <c r="BT18" s="2" t="s">
         <v>285</v>
       </c>
+      <c r="BV18" s="2">
+        <v>2</v>
+      </c>
+      <c r="BW18" s="2">
+        <f t="shared" si="26"/>
+        <v>0.22123838671744189</v>
+      </c>
+      <c r="BX18" s="2">
+        <f t="shared" si="27"/>
+        <v>0.69135783459452771</v>
+      </c>
+      <c r="BY18" s="2">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="CF18" s="2">
+        <v>2</v>
+      </c>
+      <c r="CG18" s="2">
+        <f t="shared" si="30"/>
+        <v>0.20903534741935917</v>
+      </c>
+      <c r="CH18" s="2">
+        <f t="shared" si="31"/>
+        <v>0.65968785873287294</v>
+      </c>
+      <c r="CI18" s="2">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="CK18" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="CL18" s="2">
+        <f t="shared" si="32"/>
+        <v>0.14421269039470483</v>
+      </c>
+      <c r="CM18" s="2">
+        <f t="shared" si="33"/>
+        <v>0.52961853296438766</v>
+      </c>
+      <c r="CN18" s="2">
+        <v>0.97170000000000001</v>
+      </c>
+      <c r="CP18" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="CQ18" s="2">
+        <f t="shared" si="34"/>
+        <v>0.17450940516105304</v>
+      </c>
+      <c r="CR18" s="2">
+        <f t="shared" si="35"/>
+        <v>0.63924294736967291</v>
+      </c>
+      <c r="CS18" s="2">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="CU18" s="2">
+        <v>2</v>
+      </c>
+      <c r="CV18" s="2">
+        <f t="shared" si="36"/>
+        <v>0.18025341973680889</v>
+      </c>
+      <c r="CW18" s="2">
+        <f t="shared" si="37"/>
+        <v>0.57300945871302056</v>
+      </c>
+      <c r="CX18" s="2">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="CZ18" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="DA18" s="2">
+        <f t="shared" si="38"/>
+        <v>0.17807660720544075</v>
+      </c>
+      <c r="DB18" s="2">
+        <f t="shared" si="39"/>
+        <v>0.65049405323760146</v>
+      </c>
+      <c r="DC18" s="2">
+        <v>0.9758</v>
+      </c>
+      <c r="DE18" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="DF18" s="2">
+        <f t="shared" si="40"/>
+        <v>0.18264062071448259</v>
+      </c>
+      <c r="DG18" s="2">
+        <f t="shared" si="41"/>
+        <v>0.66439931922950457</v>
+      </c>
+      <c r="DH18" s="2">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="DJ18" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="DK18" s="2">
+        <f t="shared" si="42"/>
+        <v>0.18435238117392636</v>
+      </c>
+      <c r="DL18" s="2">
+        <f t="shared" si="43"/>
+        <v>0.66947500282370476</v>
+      </c>
+      <c r="DM18" s="2">
+        <v>0.97430000000000005</v>
+      </c>
     </row>
-    <row r="19" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>265</v>
       </c>
@@ -4941,11 +6680,11 @@
         <v>5.5</v>
       </c>
       <c r="W19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>9.0150193456815117E-2</v>
       </c>
       <c r="X19" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.24324778375654069</v>
       </c>
       <c r="Y19" s="2">
@@ -4956,11 +6695,11 @@
         <v>5.5</v>
       </c>
       <c r="AB19" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.48078825688416366</v>
       </c>
       <c r="AC19" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.8964170289391088</v>
       </c>
       <c r="AD19" s="2">
@@ -4970,11 +6709,11 @@
         <v>5.5</v>
       </c>
       <c r="AG19" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.22732219621302879</v>
       </c>
       <c r="AH19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0.46625510004616011</v>
       </c>
       <c r="AI19" s="2">
@@ -4990,11 +6729,11 @@
         <v>1.002</v>
       </c>
       <c r="AU19" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>7.8480293247622956E-2</v>
       </c>
       <c r="AV19" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>0.28663150195679926</v>
       </c>
       <c r="AW19" s="2">
@@ -5013,11 +6752,11 @@
         <v>4.4969999999999999</v>
       </c>
       <c r="BD19" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.43307616969184493</v>
       </c>
       <c r="BE19" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.87809549523948771</v>
       </c>
       <c r="BF19" s="2">
@@ -5039,11 +6778,11 @@
         <v>0.6</v>
       </c>
       <c r="BM19" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>9.0577399684321228E-2</v>
       </c>
       <c r="BN19" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>0.47855462326732134</v>
       </c>
       <c r="BO19" s="2">
@@ -5064,17 +6803,127 @@
       <c r="BT19" s="2" t="s">
         <v>287</v>
       </c>
+      <c r="BV19" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="BW19" s="2">
+        <f t="shared" si="26"/>
+        <v>0.26205388851479117</v>
+      </c>
+      <c r="BX19" s="2">
+        <f t="shared" si="27"/>
+        <v>0.73684193251726393</v>
+      </c>
+      <c r="BY19" s="2">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="CF19" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="CG19" s="2">
+        <f t="shared" si="30"/>
+        <v>0.24831740549235679</v>
+      </c>
+      <c r="CH19" s="2">
+        <f t="shared" si="31"/>
+        <v>0.7078670060447616</v>
+      </c>
+      <c r="CI19" s="2">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="CK19" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="CL19" s="2">
+        <f t="shared" si="32"/>
+        <v>0.16148756667180059</v>
+      </c>
+      <c r="CM19" s="2">
+        <f t="shared" si="33"/>
+        <v>0.56270423862323171</v>
+      </c>
+      <c r="CN19" s="2">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="CP19" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="CQ19" s="2">
+        <f t="shared" si="34"/>
+        <v>0.19458825160702195</v>
+      </c>
+      <c r="CR19" s="2">
+        <f t="shared" si="35"/>
+        <v>0.66943067712203141</v>
+      </c>
+      <c r="CS19" s="2">
+        <v>0.97030000000000005</v>
+      </c>
+      <c r="CU19" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="CV19" s="2">
+        <f t="shared" si="36"/>
+        <v>0.21560106725318787</v>
+      </c>
+      <c r="CW19" s="2">
+        <f t="shared" si="37"/>
+        <v>0.62651243550487024</v>
+      </c>
+      <c r="CX19" s="2">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="CZ19" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="DA19" s="2">
+        <f t="shared" si="38"/>
+        <v>0.19846721282042074</v>
+      </c>
+      <c r="DB19" s="2">
+        <f t="shared" si="39"/>
+        <v>0.68021128958312937</v>
+      </c>
+      <c r="DC19" s="2">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="DJ19" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="DK19" s="2">
+        <f t="shared" si="42"/>
+        <v>0.2052821146769008</v>
+      </c>
+      <c r="DL19" s="2">
+        <f t="shared" si="43"/>
+        <v>0.69832681123776663</v>
+      </c>
+      <c r="DM19" s="2">
+        <v>0.96919999999999995</v>
+      </c>
     </row>
-    <row r="20" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2003</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>318</v>
+      </c>
       <c r="V20" s="2">
         <v>6</v>
       </c>
       <c r="W20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>9.7546228194460724E-2</v>
       </c>
       <c r="X20" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.25962012589419375</v>
       </c>
       <c r="Y20" s="2">
@@ -5085,11 +6934,11 @@
         <v>6</v>
       </c>
       <c r="AB20" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.50253161660310686</v>
       </c>
       <c r="AC20" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.90422219741472754</v>
       </c>
       <c r="AD20" s="2">
@@ -5119,11 +6968,11 @@
         <v>4.9859999999999998</v>
       </c>
       <c r="BD20" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.45857322284429874</v>
       </c>
       <c r="BE20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.88872080714566659</v>
       </c>
       <c r="BF20" s="2">
@@ -5145,11 +6994,11 @@
         <v>0.7</v>
       </c>
       <c r="BM20" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>0.10410208362562001</v>
       </c>
       <c r="BN20" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>0.51707248879871404</v>
       </c>
       <c r="BO20" s="2">
@@ -5170,17 +7019,115 @@
       <c r="BT20" s="2" t="s">
         <v>289</v>
       </c>
+      <c r="BV20" s="2">
+        <v>3</v>
+      </c>
+      <c r="BW20" s="2">
+        <f t="shared" si="26"/>
+        <v>0.29880411041030475</v>
+      </c>
+      <c r="BX20" s="2">
+        <f t="shared" si="27"/>
+        <v>0.77064204437016348</v>
+      </c>
+      <c r="BY20" s="2">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="CF20" s="2">
+        <v>3</v>
+      </c>
+      <c r="CG20" s="2">
+        <f t="shared" si="30"/>
+        <v>0.28388230319205882</v>
+      </c>
+      <c r="CH20" s="2">
+        <f t="shared" si="31"/>
+        <v>0.74409618019668045</v>
+      </c>
+      <c r="CI20" s="2">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="CK20" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="CL20" s="2">
+        <f t="shared" si="32"/>
+        <v>0.17807882302991573</v>
+      </c>
+      <c r="CM20" s="2">
+        <f t="shared" si="33"/>
+        <v>0.59144144261875886</v>
+      </c>
+      <c r="CN20" s="2">
+        <v>0.95979999999999999</v>
+      </c>
+      <c r="CP20" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="CQ20" s="2">
+        <f t="shared" si="34"/>
+        <v>0.21371351563878213</v>
+      </c>
+      <c r="CR20" s="2">
+        <f t="shared" si="35"/>
+        <v>0.69495637239449559</v>
+      </c>
+      <c r="CS20" s="2">
+        <v>0.96489999999999998</v>
+      </c>
+      <c r="CU20" s="2">
+        <v>3</v>
+      </c>
+      <c r="CV20" s="2">
+        <f t="shared" si="36"/>
+        <v>0.24802633231310559</v>
+      </c>
+      <c r="CW20" s="2">
+        <f t="shared" si="37"/>
+        <v>0.6681002941197477</v>
+      </c>
+      <c r="CX20" s="2">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="CZ20" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="DA20" s="2">
+        <f t="shared" si="38"/>
+        <v>0.21787059324828353</v>
+      </c>
+      <c r="DB20" s="2">
+        <f t="shared" si="39"/>
+        <v>0.70527103569412897</v>
+      </c>
+      <c r="DC20" s="2">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="DJ20" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="DK20" s="2">
+        <f t="shared" si="42"/>
+        <v>0.22516459596037394</v>
+      </c>
+      <c r="DL20" s="2">
+        <f t="shared" si="43"/>
+        <v>0.7225460065515239</v>
+      </c>
+      <c r="DM20" s="2">
+        <v>0.96340000000000003</v>
+      </c>
     </row>
-    <row r="21" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC21" s="2">
         <v>4.9909999999999997</v>
       </c>
       <c r="BD21" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.45882208936917845</v>
       </c>
       <c r="BE21" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.88881989265984018</v>
       </c>
       <c r="BF21" s="2">
@@ -5202,11 +7149,11 @@
         <v>0.8</v>
       </c>
       <c r="BM21" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>0.11723039156834966</v>
       </c>
       <c r="BN21" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>0.55029134234819244</v>
       </c>
       <c r="BO21" s="2">
@@ -5227,17 +7174,87 @@
       <c r="BT21" s="2" t="s">
         <v>291</v>
       </c>
+      <c r="CF21" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="CG21" s="2">
+        <f t="shared" si="30"/>
+        <v>0.31623382273327666</v>
+      </c>
+      <c r="CH21" s="2">
+        <f t="shared" si="31"/>
+        <v>0.7723308093783533</v>
+      </c>
+      <c r="CI21" s="2">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="CK21" s="2">
+        <v>2</v>
+      </c>
+      <c r="CL21" s="2">
+        <f t="shared" si="32"/>
+        <v>0.19402625153215608</v>
+      </c>
+      <c r="CM21" s="2">
+        <f t="shared" si="33"/>
+        <v>0.61663457589465009</v>
+      </c>
+      <c r="CN21" s="2">
+        <v>0.95289999999999997</v>
+      </c>
+      <c r="CP21" s="2">
+        <v>2</v>
+      </c>
+      <c r="CQ21" s="2">
+        <f t="shared" si="34"/>
+        <v>0.23195155273282389</v>
+      </c>
+      <c r="CR21" s="2">
+        <f t="shared" si="35"/>
+        <v>0.71682258867437554</v>
+      </c>
+      <c r="CS21" s="2">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="CZ21" s="2">
+        <v>2</v>
+      </c>
+      <c r="DA21" s="2">
+        <f t="shared" si="38"/>
+        <v>0.23635674968996084</v>
+      </c>
+      <c r="DB21" s="2">
+        <f t="shared" si="39"/>
+        <v>0.7266886551650924</v>
+      </c>
+      <c r="DC21" s="2">
+        <v>0.95879999999999999</v>
+      </c>
+      <c r="DJ21" s="2">
+        <v>2</v>
+      </c>
+      <c r="DK21" s="2">
+        <f t="shared" si="42"/>
+        <v>0.24407650792374122</v>
+      </c>
+      <c r="DL21" s="2">
+        <f t="shared" si="43"/>
+        <v>0.74316542813439734</v>
+      </c>
+      <c r="DM21" s="2">
+        <v>0.95699999999999996</v>
+      </c>
     </row>
-    <row r="22" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC22" s="2">
         <v>5.4969999999999999</v>
       </c>
       <c r="BD22" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.48287686089541143</v>
       </c>
       <c r="BE22" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.89801026634902636</v>
       </c>
       <c r="BF22" s="2">
@@ -5259,11 +7276,11 @@
         <v>0.9</v>
       </c>
       <c r="BM22" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>0.12997949709682857</v>
       </c>
       <c r="BN22" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>0.57923430709363155</v>
       </c>
       <c r="BO22" s="2">
@@ -5284,17 +7301,87 @@
       <c r="BT22" s="2" t="s">
         <v>293</v>
       </c>
+      <c r="CF22" s="2">
+        <v>4</v>
+      </c>
+      <c r="CG22" s="2">
+        <f t="shared" si="30"/>
+        <v>0.34578864524604236</v>
+      </c>
+      <c r="CH22" s="2">
+        <f t="shared" si="31"/>
+        <v>0.79495412979224533</v>
+      </c>
+      <c r="CI22" s="2">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="CK22" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="CL22" s="2">
+        <f t="shared" si="32"/>
+        <v>0.23131263360747287</v>
+      </c>
+      <c r="CM22" s="2">
+        <f t="shared" si="33"/>
+        <v>0.66783992295421546</v>
+      </c>
+      <c r="CN22" s="2">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="CP22" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="CQ22" s="2">
+        <f t="shared" si="34"/>
+        <v>0.27404797744321874</v>
+      </c>
+      <c r="CR22" s="2">
+        <f t="shared" si="35"/>
+        <v>0.7598574837174793</v>
+      </c>
+      <c r="CS22" s="2">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="CZ22" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="DA22" s="2">
+        <f t="shared" si="38"/>
+        <v>0.27896228251699851</v>
+      </c>
+      <c r="DB22" s="2">
+        <f t="shared" si="39"/>
+        <v>0.76870797738180074</v>
+      </c>
+      <c r="DC22" s="2">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="DJ22" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="DK22" s="2">
+        <f t="shared" si="42"/>
+        <v>0.28754960881130143</v>
+      </c>
+      <c r="DL22" s="2">
+        <f t="shared" si="43"/>
+        <v>0.78340660830240372</v>
+      </c>
+      <c r="DM22" s="2">
+        <v>0.93799999999999994</v>
+      </c>
     </row>
-    <row r="23" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC23" s="2">
         <v>6.0090000000000003</v>
       </c>
       <c r="BD23" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.50513394581552229</v>
       </c>
       <c r="BE23" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.90588246542043027</v>
       </c>
       <c r="BF23" s="2">
@@ -5316,11 +7403,11 @@
         <v>1</v>
       </c>
       <c r="BM23" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>0.14236559582434957</v>
       </c>
       <c r="BN23" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>0.60467704257395172</v>
       </c>
       <c r="BO23" s="2">
@@ -5341,17 +7428,73 @@
       <c r="BT23" s="2" t="s">
         <v>295</v>
       </c>
+      <c r="CF23" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="CG23" s="2">
+        <f t="shared" si="30"/>
+        <v>0.37289439494577969</v>
+      </c>
+      <c r="CH23" s="2">
+        <f t="shared" si="31"/>
+        <v>0.81348771836052924</v>
+      </c>
+      <c r="CI23" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="CK23" s="2">
+        <v>3</v>
+      </c>
+      <c r="CL23" s="2">
+        <f t="shared" si="32"/>
+        <v>0.26530163629080772</v>
+      </c>
+      <c r="CM23" s="2">
+        <f t="shared" si="33"/>
+        <v>0.70697824783250529</v>
+      </c>
+      <c r="CN23" s="2">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="CP23" s="2">
+        <v>3</v>
+      </c>
+      <c r="CQ23" s="2">
+        <f t="shared" si="34"/>
+        <v>0.31176960689243466</v>
+      </c>
+      <c r="CR23" s="2">
+        <f t="shared" si="35"/>
+        <v>0.79153779675853198</v>
+      </c>
+      <c r="CS23" s="2">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="DJ23" s="2">
+        <v>3</v>
+      </c>
+      <c r="DK23" s="2">
+        <f t="shared" si="42"/>
+        <v>0.32629436705288412</v>
+      </c>
+      <c r="DL23" s="2">
+        <f t="shared" si="43"/>
+        <v>0.81274583790575583</v>
+      </c>
+      <c r="DM23" s="2">
+        <v>0.91300000000000003</v>
+      </c>
     </row>
-    <row r="24" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC24" s="2">
         <v>6.5</v>
       </c>
       <c r="BD24" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.52474984019713378</v>
       </c>
       <c r="BE24" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.91236894675964941</v>
       </c>
       <c r="BF24" s="2">
@@ -5369,17 +7512,45 @@
       <c r="BJ24" s="2">
         <v>0.434</v>
       </c>
+      <c r="CF24" s="2">
+        <v>5</v>
+      </c>
+      <c r="CG24" s="2">
+        <f t="shared" si="30"/>
+        <v>0.3978433760513278</v>
+      </c>
+      <c r="CH24" s="2">
+        <f t="shared" si="31"/>
+        <v>0.82894862836434346</v>
+      </c>
+      <c r="CI24" s="2">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="CP24" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="CQ24" s="2">
+        <f t="shared" si="34"/>
+        <v>0.34576471959050631</v>
+      </c>
+      <c r="CR24" s="2">
+        <f t="shared" si="35"/>
+        <v>0.81583357747846486</v>
+      </c>
+      <c r="CS24" s="2">
+        <v>0.89200000000000002</v>
+      </c>
     </row>
-    <row r="25" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC25" s="2">
         <v>6.9850000000000003</v>
       </c>
       <c r="BD25" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.54265684223437838</v>
       </c>
       <c r="BE25" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.91795434885155569</v>
       </c>
       <c r="BF25" s="2">
@@ -5397,17 +7568,31 @@
       <c r="BJ25" s="2">
         <v>0.42099999999999999</v>
       </c>
+      <c r="CP25" s="2">
+        <v>4</v>
+      </c>
+      <c r="CQ25" s="2">
+        <f t="shared" si="34"/>
+        <v>0.37655953631989575</v>
+      </c>
+      <c r="CR25" s="2">
+        <f t="shared" si="35"/>
+        <v>0.83505726614170628</v>
+      </c>
+      <c r="CS25" s="2">
+        <v>0.86199999999999999</v>
+      </c>
     </row>
-    <row r="26" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC26" s="2">
         <v>7.4950000000000001</v>
       </c>
       <c r="BD26" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.56008678871780104</v>
       </c>
       <c r="BE26" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.92310789978501107</v>
       </c>
       <c r="BF26" s="2">
@@ -5426,16 +7611,16 @@
         <v>0.41199999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC27" s="2">
         <v>7.9480000000000004</v>
       </c>
       <c r="BD27" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.57449103724090178</v>
       </c>
       <c r="BE27" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.9271712290257752</v>
       </c>
       <c r="BF27" s="2">
@@ -5454,16 +7639,16 @@
         <v>0.39700000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC28" s="2">
         <v>7.9969999999999999</v>
       </c>
       <c r="BD28" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.57599277718960207</v>
       </c>
       <c r="BE28" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.92758515793215013</v>
       </c>
       <c r="BF28" s="2">
@@ -5482,16 +7667,16 @@
         <v>0.38900000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC29" s="2">
         <v>8.9870000000000001</v>
       </c>
       <c r="BD29" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.604214590590331</v>
       </c>
       <c r="BE29" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.93504415022326359</v>
       </c>
       <c r="BF29" s="2">
@@ -5510,16 +7695,16 @@
         <v>0.379</v>
       </c>
     </row>
-    <row r="30" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC30" s="2">
         <v>9.9670000000000005</v>
       </c>
       <c r="BD30" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.62867991525094347</v>
       </c>
       <c r="BE30" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.94105442917687832</v>
       </c>
       <c r="BF30" s="2">
@@ -5538,16 +7723,16 @@
         <v>0.377</v>
       </c>
     </row>
-    <row r="31" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC31" s="2">
         <v>11.013</v>
       </c>
       <c r="BD31" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.65166240927882724</v>
       </c>
       <c r="BE31" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.94635265209091057</v>
       </c>
       <c r="BF31" s="2">
@@ -5566,16 +7751,16 @@
         <v>0.373</v>
       </c>
     </row>
-    <row r="32" spans="1:72" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:117" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC32" s="2">
         <v>11.999000000000001</v>
       </c>
       <c r="BD32" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>0.67086534204909554</v>
       </c>
       <c r="BE32" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>0.95054301748754755</v>
       </c>
       <c r="BF32" s="2">
@@ -5608,10 +7793,12 @@
     <hyperlink ref="A16" r:id="rId10" xr:uid="{BD0A540B-8EC4-4001-BE15-3CBF3CEF38EB}"/>
     <hyperlink ref="A17" r:id="rId11" location="fig0003" xr:uid="{A08C39A0-20C1-4E98-A85A-A81E8F1031B0}"/>
     <hyperlink ref="A19" r:id="rId12" xr:uid="{42B52C3E-043A-4627-B085-78F4B980BB88}"/>
-    <hyperlink ref="Y1" r:id="rId13" location=":~:text=Table_title:%20Table%201.%20Table_content:%20header:%20%7C%20Compounds,KClO3%20%7C%20DRH:%2097%E2%80%9398%20%7C%20ERH:%20%7C" xr:uid="{87BD47B9-1CBE-4740-B03B-E88ABF9C4763}"/>
+    <hyperlink ref="A20" r:id="rId13" xr:uid="{3DD93DD8-43FD-4FF1-B344-67CB650DDC46}"/>
+    <hyperlink ref="O1" r:id="rId14" xr:uid="{AED6EA17-9FD0-4DEE-9253-0D12E330FB6E}"/>
+    <hyperlink ref="AI1" r:id="rId15" location=":~:text=Table_title:%20Table%201.%20Table_content:%20header:%20%7C%20Compounds,KClO3%20%7C%20DRH:%2097%E2%80%9398%20%7C%20ERH:%20%7C" xr:uid="{87BD47B9-1CBE-4740-B03B-E88ABF9C4763}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
-  <drawing r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
+  <drawing r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>